<commit_message>
Auto update: 2025-05-18 01:13:34
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,10 +476,8 @@
           <t>JISA VENTURES LTD</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>16455405</t>
-        </is>
+      <c r="B2" t="n">
+        <v>16455405</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -513,10 +511,8 @@
           <t>MARKOVIAN INVESTMENTS LIMITED</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>16455443</t>
-        </is>
+      <c r="B3" t="n">
+        <v>16455443</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -541,6 +537,1375 @@
       <c r="G3" t="inlineStr">
         <is>
           <t>2025-05-18 01:10:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>R. KENDALL INVESTMENTS LIMITED</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>16454651</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>INDO-EURO VENTURES LTD</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>16454655</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SLAM DUNK INVESTMENTS LTD</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>16455167</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>DAVISON FAMILY CAPITAL LTD</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>16455115</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>TALKSGPT AI LTD</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>16455313</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>NEW TOWER CAPITAL LTD</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>16454704</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>GPS BUILDERS LTD</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>16454759</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ALPHA HEDONIST ENTERPRISES LTD</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>16454743</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>DEARG INVESTMENTS LTD</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>16455090</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>STEVE'S VENTURES LIMITED</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>16455332</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ARISSA INVESTMENTS LIMITED</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>16455197</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>E.Q. EQUITY LTD</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>16454966</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>BKH PROPERTY INVESTMENTS LTD</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16454907</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CROWTHER CAPITAL SOLUTIONS LTD</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16454539</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>JL NEW INVESTMENTS LIMITED</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>16454813</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>BELGRAVIA HEIGHTS ESTATES LTD</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>16454964</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>SIC</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>HOOK INVESTMENTS LTD</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>16454933</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CALLA LILY PROPERTY LTD</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>16455024</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>SIC</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>LIBERA CAPITAL MANAGEMENT LIMITED</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>16455027</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>GOODBREACH LTD</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>16455072</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>SIC</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>ANUGRAHA BENEFICIAL HOLDINGS &amp; INVESTMENTS LTD</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>16455184</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>ONE-TENT PROPERTIES LIMITED</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>16455350</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>SIC</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>HAMATECH GLOBAL LIMITED</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>16455295</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>SIC</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>DOUBLE U PROPERTY INVESTMENTS LIMITED</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>SC848872</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>GW CAPITAL HOLDINGS LIMITED</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>16455129</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>CENTERWOOD SUB LIMITED</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>16455117</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>SIC</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>EMERSON CAPITAL HOLDINGS LTD</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>16455220</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>KARNAVATI GLOBAL VENTURES LIMITED</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>16454965</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>TRADIA CAPITAL ACADEMY LTD</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>16455007</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>D HAYDEN CAPITAL LIMITED</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>16455013</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ALPHA DISPATCH SERVICES LTD</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>16454873</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>VKS CAPITAL LTD</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>16454770</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>ARLO EQUITY LTD</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>16455284</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Keyword+SIC</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>ARMAGH INVESTMENTS LIMITED</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>NI729471</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>NIRVANA ADVERTISING VENTURES LIMITED</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>16454522</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>WK CAPITAL LTD</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>16454711</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>MSY UK INVESTMENTS LTD</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>16455242</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2025-05-18 01:13:33</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update: 2025-05-18 07:42:05
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G614"/>
+  <dimension ref="A1:G615"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23147,6 +23147,43 @@
         </is>
       </c>
     </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>TALLY M E VENTURES LIMITED</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>16455468</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D615" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E615" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F615" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G615" t="inlineStr">
+        <is>
+          <t>2025-05-18 07:42:05</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Auto update: 2025-05-18 08:41:45
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G615"/>
+  <dimension ref="A1:G616"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23184,6 +23184,43 @@
         </is>
       </c>
     </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>LENDING CONSULTANCY LTD</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>16455471</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D616" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E616" t="inlineStr">
+        <is>
+          <t>SIC</t>
+        </is>
+      </c>
+      <c r="F616" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G616" t="inlineStr">
+        <is>
+          <t>2025-05-18 08:41:44</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Auto update: 2025-05-18 10:40:21
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G616"/>
+  <dimension ref="A1:G617"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23221,6 +23221,43 @@
         </is>
       </c>
     </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>BIEN DEVELOPMENTS LTD</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>16455494</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D617" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E617" t="inlineStr">
+        <is>
+          <t>SIC</t>
+        </is>
+      </c>
+      <c r="F617" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G617" t="inlineStr">
+        <is>
+          <t>2025-05-18 10:40:21</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Auto update: 2025-05-18 13:16:37
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G617"/>
+  <dimension ref="A1:G618"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23258,6 +23258,43 @@
         </is>
       </c>
     </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>PARTNERS AMERICAN WHISKEY LTD</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>16455528</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D618" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E618" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F618" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G618" t="inlineStr">
+        <is>
+          <t>2025-05-18 13:16:36</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Auto update: 2025-05-18 14:36:04
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G618"/>
+  <dimension ref="A1:G619"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23295,6 +23295,43 @@
         </is>
       </c>
     </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>ALPHA HAULAGE SOLUTIONS LTD</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>16455573</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D619" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E619" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F619" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G619" t="inlineStr">
+        <is>
+          <t>2025-05-18 14:36:02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Auto update: 2025-05-18 14:48:44
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G619"/>
+  <dimension ref="A1:G620"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23332,6 +23332,43 @@
         </is>
       </c>
     </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>PERFICIENT VENTURES LTD</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>16455594</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D620" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E620" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F620" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G620" t="inlineStr">
+        <is>
+          <t>2025-05-18 14:48:42</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Auto update: 2025-05-18 15:24:54
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G620"/>
+  <dimension ref="A1:G621"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23369,6 +23369,43 @@
         </is>
       </c>
     </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>BLUEBOW TECHNOLOGIES LTD</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>16455597</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D621" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E621" t="inlineStr">
+        <is>
+          <t>SIC</t>
+        </is>
+      </c>
+      <c r="F621" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G621" t="inlineStr">
+        <is>
+          <t>2025-05-18 15:24:53</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Auto update: 2025-05-18 21:42:51
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,10 +476,8 @@
           <t>LENDING CONSULTANCY LTD</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>16455471</t>
-        </is>
+      <c r="B2" t="n">
+        <v>16455471</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -513,10 +511,8 @@
           <t>JISA VENTURES LTD</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>16455405</t>
-        </is>
+      <c r="B3" t="n">
+        <v>16455405</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -550,10 +546,8 @@
           <t>TALLY M E VENTURES LIMITED</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>16455468</t>
-        </is>
+      <c r="B4" t="n">
+        <v>16455468</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -587,10 +581,8 @@
           <t>PERFICIENT VENTURES LTD</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>16455594</t>
-        </is>
+      <c r="B5" t="n">
+        <v>16455594</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -624,10 +616,8 @@
           <t>BLUEBOW TECHNOLOGIES LTD</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>16455597</t>
-        </is>
+      <c r="B6" t="n">
+        <v>16455597</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -661,10 +651,8 @@
           <t>BIEN DEVELOPMENTS LTD</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>16455494</t>
-        </is>
+      <c r="B7" t="n">
+        <v>16455494</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -698,10 +686,8 @@
           <t>ALPHA HAULAGE SOLUTIONS LTD</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>16455573</t>
-        </is>
+      <c r="B8" t="n">
+        <v>16455573</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -735,10 +721,8 @@
           <t>MARKOVIAN INVESTMENTS LIMITED</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>16455443</t>
-        </is>
+      <c r="B9" t="n">
+        <v>16455443</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -772,34 +756,513 @@
           <t>PARTNERS AMERICAN WHISKEY LTD</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" t="n">
+        <v>16455528</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2025-05-18 15:36:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>LENDING CONSULTANCY LTD</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>16455471</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>SIC</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2025-05-18 21:42:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ECHO VENTURES GROUP LIMITED</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>16455744</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2025-05-18 21:42:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ESLB INVESTMENTS LIMITED</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>16455669</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2025-05-18 21:42:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>JISA VENTURES LTD</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>16455405</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2025-05-18 21:42:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>TALLY M E VENTURES LIMITED</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>16455468</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2025-05-18 21:42:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>PERFICIENT VENTURES LTD</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16455594</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2025-05-18 21:42:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>BLUEBOW TECHNOLOGIES LTD</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16455597</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>SIC</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2025-05-18 21:42:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>JENKINS VENTURES LTD</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>16455788</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2025-05-18 21:42:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>BIEN DEVELOPMENTS LTD</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>16455494</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>SIC</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2025-05-18 21:42:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ALPHA HAULAGE SOLUTIONS LTD</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>16455573</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2025-05-18 21:42:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>MARIOS PROPERTY INVESTMENTS LTD</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>16455816</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2025-05-18 21:42:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>MARKOVIAN INVESTMENTS LIMITED</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>16455443</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2025-05-18 21:42:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>PARTNERS AMERICAN WHISKEY LTD</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>16455528</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2025-05-18</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Keyword</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2025-05-18</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2025-05-18 15:36:00</t>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2025-05-18 21:42:50</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update: 2025-05-18 23:26:30
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -788,13 +788,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>LENDING CONSULTANCY LTD</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>16455471</t>
-        </is>
+          <t>ECHO VENTURES GROUP LIMITED</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>16455744</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -808,7 +806,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>SIC</t>
+          <t>Keyword</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -825,13 +823,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ECHO VENTURES GROUP LIMITED</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>16455744</t>
-        </is>
+          <t>ESLB INVESTMENTS LIMITED</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>16455669</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -862,13 +858,11 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ESLB INVESTMENTS LIMITED</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>16455669</t>
-        </is>
+          <t>JENKINS VENTURES LTD</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>16455788</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -892,20 +886,18 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-18 21:42:48</t>
+          <t>2025-05-18 21:42:49</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>JISA VENTURES LTD</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>16455405</t>
-        </is>
+          <t>MARIOS PROPERTY INVESTMENTS LTD</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>16455816</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -929,19 +921,19 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-18 21:42:49</t>
+          <t>2025-05-18 21:42:50</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>TALLY M E VENTURES LIMITED</t>
+          <t>LENDING CONSULTANCY LTD</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16455468</t>
+          <t>16455471</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -956,7 +948,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Keyword</t>
+          <t>SIC</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -966,19 +958,19 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-18 21:42:49</t>
+          <t>2025-05-18 23:26:26</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PERFICIENT VENTURES LTD</t>
+          <t>ECHO VENTURES GROUP LIMITED</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16455594</t>
+          <t>16455744</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1003,19 +995,19 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-18 21:42:49</t>
+          <t>2025-05-18 23:26:27</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BLUEBOW TECHNOLOGIES LTD</t>
+          <t>ESLB INVESTMENTS LIMITED</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16455597</t>
+          <t>16455669</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1030,7 +1022,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>SIC</t>
+          <t>Keyword</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1040,19 +1032,19 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-18 21:42:49</t>
+          <t>2025-05-18 23:26:27</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>JENKINS VENTURES LTD</t>
+          <t>JISA VENTURES LTD</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16455788</t>
+          <t>16455405</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1077,19 +1069,19 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-18 21:42:49</t>
+          <t>2025-05-18 23:26:27</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BIEN DEVELOPMENTS LTD</t>
+          <t>TALLY M E VENTURES LIMITED</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16455494</t>
+          <t>16455468</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1104,7 +1096,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>SIC</t>
+          <t>Keyword</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1114,19 +1106,19 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-18 21:42:50</t>
+          <t>2025-05-18 23:26:27</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ALPHA HAULAGE SOLUTIONS LTD</t>
+          <t>PERFICIENT VENTURES LTD</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>16455573</t>
+          <t>16455594</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1151,19 +1143,19 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-18 21:42:50</t>
+          <t>2025-05-18 23:26:28</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>MARIOS PROPERTY INVESTMENTS LTD</t>
+          <t>BLUEBOW TECHNOLOGIES LTD</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16455816</t>
+          <t>16455597</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1178,7 +1170,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Keyword</t>
+          <t>SIC</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1188,19 +1180,19 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-18 21:42:50</t>
+          <t>2025-05-18 23:26:28</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>MARKOVIAN INVESTMENTS LIMITED</t>
+          <t>JENKINS VENTURES LTD</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16455443</t>
+          <t>16455788</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1225,44 +1217,192 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-18 21:42:50</t>
+          <t>2025-05-18 23:26:28</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>BIEN DEVELOPMENTS LTD</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>16455494</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>SIC</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2025-05-18 23:26:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>ALPHA HAULAGE SOLUTIONS LTD</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>16455573</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2025-05-18 23:26:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>MARIOS PROPERTY INVESTMENTS LTD</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>16455816</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2025-05-18 23:26:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>MARKOVIAN INVESTMENTS LIMITED</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>16455443</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2025-05-18 23:26:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
           <t>PARTNERS AMERICAN WHISKEY LTD</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>16455528</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>2025-05-18</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>active</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Keyword</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>2025-05-18</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>2025-05-18 21:42:50</t>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Keyword</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2025-05-18 23:26:29</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update: 2025-05-18 23:35:04
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -958,7 +958,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-18 23:26:26</t>
+          <t>2025-05-18 23:35:01</t>
         </is>
       </c>
     </row>
@@ -995,7 +995,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-18 23:26:27</t>
+          <t>2025-05-18 23:35:01</t>
         </is>
       </c>
     </row>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-18 23:26:27</t>
+          <t>2025-05-18 23:35:01</t>
         </is>
       </c>
     </row>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-18 23:26:27</t>
+          <t>2025-05-18 23:35:02</t>
         </is>
       </c>
     </row>
@@ -1106,7 +1106,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-18 23:26:27</t>
+          <t>2025-05-18 23:35:02</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-18 23:26:28</t>
+          <t>2025-05-18 23:35:02</t>
         </is>
       </c>
     </row>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-18 23:26:28</t>
+          <t>2025-05-18 23:35:02</t>
         </is>
       </c>
     </row>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-18 23:26:28</t>
+          <t>2025-05-18 23:35:03</t>
         </is>
       </c>
     </row>
@@ -1254,7 +1254,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-05-18 23:26:28</t>
+          <t>2025-05-18 23:35:03</t>
         </is>
       </c>
     </row>
@@ -1291,7 +1291,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-05-18 23:26:29</t>
+          <t>2025-05-18 23:35:03</t>
         </is>
       </c>
     </row>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-05-18 23:26:29</t>
+          <t>2025-05-18 23:35:03</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-18 23:26:29</t>
+          <t>2025-05-18 23:35:03</t>
         </is>
       </c>
     </row>
@@ -1402,7 +1402,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-18 23:26:29</t>
+          <t>2025-05-18 23:35:04</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update: 2025-05-19 17:51:49
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,52 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Company Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Company Number</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Incorporation Date</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Date Downloaded</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Time Discovered</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Auto update: 2025-05-19 19:52:05
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -510,12 +510,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HARRY'S OFFLICENCE &amp; TAKEAWAY LTD</t>
+          <t>CALIBRE LDN LIMITED</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16456203</t>
+          <t>16457945</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -547,12 +547,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>J&amp;S DISTRIBUTIONS LIMITED</t>
+          <t>SHOTTON CURRY HOUSE LIMITED</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16456242</t>
+          <t>16459062</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -584,12 +584,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>B HOLLAND &amp; SONS (HOLDINGS) LTD</t>
+          <t>CAZAM PROPERTY LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16456243</t>
+          <t>16459061</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -621,12 +621,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SOCIAL SLOT LTD</t>
+          <t>M S GROUP FIRST UK LIMITED</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16456245</t>
+          <t>16459057</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -658,12 +658,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>UKG BB HOLDINGS LTD</t>
+          <t>PARKSIDE GETAWAYS LIMITED</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16456246</t>
+          <t>16459059</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -695,12 +695,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>KINARA PROPERTIES LTD</t>
+          <t>DRIVERIGHT REPAIRS LTD</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16456244</t>
+          <t>16459058</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -732,12 +732,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MARKETING DG LTD</t>
+          <t>GK ZYGALA LIMITED</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16456254</t>
+          <t>16457953</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -769,12 +769,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>EVO AVIATION LIMITED</t>
+          <t>MAPLE (510) LIMITED</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16456253</t>
+          <t>16457954</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -806,12 +806,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SWIFT BUSINESS GROWTH.AI LTD</t>
+          <t>PANEER CRAFT LTD. LIMITED</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16456250</t>
+          <t>16457973</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -843,12 +843,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>JC DEEP TECH LTD</t>
+          <t>CAMBRIDGE VETS LTD</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16456256</t>
+          <t>16457975</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -880,12 +880,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>HAUS OF PALETTE LTD</t>
+          <t>ROCK&amp;WALLS LTD</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16456236</t>
+          <t>16457974</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -917,12 +917,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>A STAR HEALTH LTD</t>
+          <t>PROOFENANCE LTD</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16456234</t>
+          <t>16457943</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -954,12 +954,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>JANITZA UK LIMITED</t>
+          <t>HARRY'S OFFLICENCE &amp; TAKEAWAY LTD</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16456233</t>
+          <t>16456203</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -991,12 +991,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>HOUSE OF RODEOS LTD</t>
+          <t>INSPOCL LTD</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16456218</t>
+          <t>16457967</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1028,12 +1028,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>JAI-HO STAFFING LTD</t>
+          <t>LEADANICS LIMITED</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16456221</t>
+          <t>16457965</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1065,12 +1065,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>WINDOW CLEANING SOUTHEND LTD</t>
+          <t>DEVIPROX LTD</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16456227</t>
+          <t>16457970</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1102,12 +1102,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IDCHEM CONSULTING LIMITED</t>
+          <t>LGAM PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16456205</t>
+          <t>16457957</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1139,12 +1139,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>STEFANPERSAUDLEGACYPROJECT LIMITED</t>
+          <t>BUILTBRITE LTD</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>16456208</t>
+          <t>16457962</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1176,12 +1176,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>STOA PROJECTS LTD</t>
+          <t>GUIDED BRAKE SERVICE LTD</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16456212</t>
+          <t>16457264</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1213,12 +1213,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CHIMNEY CHAPS LTD</t>
+          <t>OMR ELECTRICAL LTD</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16456261</t>
+          <t>16457261</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1250,12 +1250,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>LEOFRIC LTD</t>
+          <t>AUSTIN RICE LTD</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>16456712</t>
+          <t>NI729522</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1287,12 +1287,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>BREEZY HOMES LIMITED</t>
+          <t>HOLYWELL HOMES LTD</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16456709</t>
+          <t>16457259</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1324,12 +1324,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ATSP FIN LTD</t>
+          <t>RELIABLE STAFFING RECRUITS LIMITED</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16456749</t>
+          <t>16457238</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1361,12 +1361,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ELLISA'S BEAUTY LTD</t>
+          <t>GODMADE LTD</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16456750</t>
+          <t>16459074</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1398,12 +1398,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>KHAZAG FREIGHT SERVICES PVT LTD</t>
+          <t>LATINOS TEESSIDE &amp; HISPANIC SENIORS COMMUNITY LTD</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16456754</t>
+          <t>16459078</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1435,12 +1435,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>FARYAL ENTERPRISE LIMITED</t>
+          <t>RENTAL DISREPAIR CLAIMS LTD</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16456748</t>
+          <t>16459077</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1472,12 +1472,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>HONG KONG XUNHUA FREIGHT LIMITED</t>
+          <t>INP SERVICES LTD</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16456735</t>
+          <t>16459069</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1509,12 +1509,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>DEHBINI LIMITED</t>
+          <t>SSFBN LIMITED</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16456493</t>
+          <t>16459541</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1546,12 +1546,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>FLIP IT GLOBAL LTD</t>
+          <t>J.R'S SOUTHERN TWIST LTD</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16456758</t>
+          <t>16459542</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1583,12 +1583,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>APEX PREMIER PROPERTY SOLUTIONS LTD</t>
+          <t>OCEANHEART MARINE SERVICE CO., LTD</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16456756</t>
+          <t>16459543</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1620,12 +1620,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>NEWCO SWANSEA SOCIAL INFRASTRUCTURE LP</t>
+          <t>INDEXIE LTD</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>LP024176</t>
+          <t>16459546</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1657,12 +1657,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>MEC SURVEYORS LTD</t>
+          <t>UBAH MEDIA LAB LTD</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16456734</t>
+          <t>16459548</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1694,12 +1694,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>BKK EQUESTRIAN LTD</t>
+          <t>CA ELECTRICAL (YORKSHIRE) LTD</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>16456733</t>
+          <t>16459547</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1731,12 +1731,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>WGHR JI LTD</t>
+          <t>LOUD AND CLEAR COACHING LIMITED</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16456731</t>
+          <t>16459549</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1768,12 +1768,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>OPM ILL GO SHOP 4U LTD</t>
+          <t>NORDIC COOPERATION TECHNOLOGIES LIMITED</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16456764</t>
+          <t>16459514</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1805,12 +1805,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>PHONE STUDIO SOUTH LIMITED</t>
+          <t>CLARK AND CO DESIGN LIMITED</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16456765</t>
+          <t>16459516</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1842,12 +1842,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>CTLO LTD</t>
+          <t>MILLE TRADING LTD</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16456701</t>
+          <t>16459518</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1879,12 +1879,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>OILMYCAR LTD</t>
+          <t>SPYRO APPAREL LTD</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16456706</t>
+          <t>16459515</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1916,12 +1916,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>NEHHEALTHCARE LTD</t>
+          <t>THE CHAIR SALON LONDON LTD</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>16456708</t>
+          <t>16459512</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1953,12 +1953,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>MAJESTIC EXTERIOR CLEANING SERVICES LTD</t>
+          <t>AMIS &amp; WARD DEVELOPMENT LTD</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16457230</t>
+          <t>16459520</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1990,12 +1990,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>JORDAN CAMPBELL LTD</t>
+          <t>CLICKSPHARE CRAFT LTD</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>NI729519</t>
+          <t>16459521</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2027,12 +2027,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Y-3 APARTMENTS LTD</t>
+          <t>TASHAN MEDIA LTD</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16457262</t>
+          <t>16459523</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2064,12 +2064,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>YSGARLAD PROPERTIES LTD</t>
+          <t>S&amp;S ISTITHMĀR LTD</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16457268</t>
+          <t>16459522</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2101,12 +2101,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>METAHAVEN LTD</t>
+          <t>WANNABEE LTD</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16457273</t>
+          <t>16459526</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2138,12 +2138,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>GLIMORA GLOBAL LTD</t>
+          <t>FINTIVITY LTD</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16457265</t>
+          <t>16459072</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2175,12 +2175,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>POWERS ELECTRICAL LTD</t>
+          <t>FASHLER LTD</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>16457270</t>
+          <t>16459082</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2212,12 +2212,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>PHOENIX CONSULTING INTERNATIONAL LIMITED</t>
+          <t>CTPROPS LIMITED</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>16457267</t>
+          <t>16459084</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2249,12 +2249,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>DCR HOLDINGS &amp; INVESTMENTS LTD</t>
+          <t>MALHAMDALE GLAMPING LIMITED</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16457272</t>
+          <t>16459064</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2286,12 +2286,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>FARRINGDON HOUSE FINANCIAL SERVICES LIMITED</t>
+          <t>NEW MOUNT DAISY LIMITED</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>16457279</t>
+          <t>16457237</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2360,12 +2360,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>NEW MOUNT DAISY LIMITED</t>
+          <t>FARRINGDON HOUSE FINANCIAL SERVICES LIMITED</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16457237</t>
+          <t>16457279</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2397,12 +2397,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>RELIABLE STAFFING RECRUITS LIMITED</t>
+          <t>ELLISA'S BEAUTY LTD</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>16457238</t>
+          <t>16456750</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2434,12 +2434,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>HOLYWELL HOMES LTD</t>
+          <t>BREEZY HOMES LIMITED</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>16457259</t>
+          <t>16456709</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2471,12 +2471,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>AUSTIN RICE LTD</t>
+          <t>LEOFRIC LTD</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>NI729522</t>
+          <t>16456712</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2508,12 +2508,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>OMR ELECTRICAL LTD</t>
+          <t>CHIMNEY CHAPS LTD</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>16457261</t>
+          <t>16456261</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2545,12 +2545,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>GUIDED BRAKE SERVICE LTD</t>
+          <t>STOA PROJECTS LTD</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>16457264</t>
+          <t>16456212</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2582,12 +2582,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>BUILTBRITE LTD</t>
+          <t>STEFANPERSAUDLEGACYPROJECT LIMITED</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>16457962</t>
+          <t>16456208</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2619,12 +2619,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>LGAM PROPERTIES LTD</t>
+          <t>IDCHEM CONSULTING LIMITED</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16457957</t>
+          <t>16456205</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2656,12 +2656,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>DEVIPROX LTD</t>
+          <t>WINDOW CLEANING SOUTHEND LTD</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16457970</t>
+          <t>16456227</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2693,12 +2693,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>LEADANICS LIMITED</t>
+          <t>JAI-HO STAFFING LTD</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>16457965</t>
+          <t>16456221</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2730,12 +2730,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>INSPOCL LTD</t>
+          <t>HOUSE OF RODEOS LTD</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16457967</t>
+          <t>16456218</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2767,12 +2767,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>PROOFENANCE LTD</t>
+          <t>JANITZA UK LIMITED</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>16457943</t>
+          <t>16456233</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2804,12 +2804,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>CALIBRE LDN LIMITED</t>
+          <t>A STAR HEALTH LTD</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>16457945</t>
+          <t>16456234</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2841,12 +2841,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>ROCK&amp;WALLS LTD</t>
+          <t>HAUS OF PALETTE LTD</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>16457974</t>
+          <t>16456236</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2878,12 +2878,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>CAMBRIDGE VETS LTD</t>
+          <t>JC DEEP TECH LTD</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>16457975</t>
+          <t>16456256</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2915,12 +2915,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>PANEER CRAFT LTD. LIMITED</t>
+          <t>SWIFT BUSINESS GROWTH.AI LTD</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>16457973</t>
+          <t>16456250</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2952,12 +2952,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>MAPLE (510) LIMITED</t>
+          <t>EVO AVIATION LIMITED</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>16457954</t>
+          <t>16456253</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2989,12 +2989,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>GK ZYGALA LIMITED</t>
+          <t>MARKETING DG LTD</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>16457953</t>
+          <t>16456254</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3026,12 +3026,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>DRIVERIGHT REPAIRS LTD</t>
+          <t>KINARA PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>16459058</t>
+          <t>16456244</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3063,12 +3063,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>PARKSIDE GETAWAYS LIMITED</t>
+          <t>UKG BB HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16459059</t>
+          <t>16456246</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3100,12 +3100,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>M S GROUP FIRST UK LIMITED</t>
+          <t>SOCIAL SLOT LTD</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16459057</t>
+          <t>16456245</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3137,12 +3137,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>CAZAM PROPERTY LTD</t>
+          <t>B HOLLAND &amp; SONS (HOLDINGS) LTD</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>16459061</t>
+          <t>16456243</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3174,12 +3174,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>SHOTTON CURRY HOUSE LIMITED</t>
+          <t>J&amp;S DISTRIBUTIONS LIMITED</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16459062</t>
+          <t>16456242</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3211,12 +3211,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>GODMADE LTD</t>
+          <t>ATSP FIN LTD</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>16459074</t>
+          <t>16456749</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3248,12 +3248,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>LATINOS TEESSIDE &amp; HISPANIC SENIORS COMMUNITY LTD</t>
+          <t>KHAZAG FREIGHT SERVICES PVT LTD</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>16459078</t>
+          <t>16456754</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3285,12 +3285,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>RENTAL DISREPAIR CLAIMS LTD</t>
+          <t>DCR HOLDINGS &amp; INVESTMENTS LTD</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>16459077</t>
+          <t>16457272</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3322,12 +3322,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>INP SERVICES LTD</t>
+          <t>FARYAL ENTERPRISE LIMITED</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>16459069</t>
+          <t>16456748</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3359,12 +3359,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>MALHAMDALE GLAMPING LIMITED</t>
+          <t>PHOENIX CONSULTING INTERNATIONAL LIMITED</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>16459064</t>
+          <t>16457267</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3396,12 +3396,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>CTPROPS LIMITED</t>
+          <t>POWERS ELECTRICAL LTD</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>16459084</t>
+          <t>16457270</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3433,12 +3433,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>FASHLER LTD</t>
+          <t>GLIMORA GLOBAL LTD</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>16459082</t>
+          <t>16457265</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3470,12 +3470,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>FINTIVITY LTD</t>
+          <t>METAHAVEN LTD</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>16459072</t>
+          <t>16457273</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3507,12 +3507,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>WANNABEE LTD</t>
+          <t>YSGARLAD PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>16459526</t>
+          <t>16457268</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3544,12 +3544,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>S&amp;S ISTITHMĀR LTD</t>
+          <t>Y-3 APARTMENTS LTD</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>16459522</t>
+          <t>16457262</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3581,12 +3581,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>TASHAN MEDIA LTD</t>
+          <t>JORDAN CAMPBELL LTD</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>16459523</t>
+          <t>NI729519</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3618,12 +3618,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>CLICKSPHARE CRAFT LTD</t>
+          <t>MAJESTIC EXTERIOR CLEANING SERVICES LTD</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>16459521</t>
+          <t>16457230</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3655,12 +3655,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>AMIS &amp; WARD DEVELOPMENT LTD</t>
+          <t>NEHHEALTHCARE LTD</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>16459520</t>
+          <t>16456708</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3692,12 +3692,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>THE CHAIR SALON LONDON LTD</t>
+          <t>OILMYCAR LTD</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>16459512</t>
+          <t>16456706</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3729,12 +3729,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>SPYRO APPAREL LTD</t>
+          <t>CTLO LTD</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16459515</t>
+          <t>16456701</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3766,12 +3766,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>MILLE TRADING LTD</t>
+          <t>PHONE STUDIO SOUTH LIMITED</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>16459518</t>
+          <t>16456765</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3803,12 +3803,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>CLARK AND CO DESIGN LIMITED</t>
+          <t>OPM ILL GO SHOP 4U LTD</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>16459516</t>
+          <t>16456764</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3840,12 +3840,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>NORDIC COOPERATION TECHNOLOGIES LIMITED</t>
+          <t>WGHR JI LTD</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>16459514</t>
+          <t>16456731</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3877,12 +3877,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>LOUD AND CLEAR COACHING LIMITED</t>
+          <t>BKK EQUESTRIAN LTD</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>16459549</t>
+          <t>16456733</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3914,12 +3914,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>CA ELECTRICAL (YORKSHIRE) LTD</t>
+          <t>MEC SURVEYORS LTD</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>16459547</t>
+          <t>16456734</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3951,12 +3951,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>UBAH MEDIA LAB LTD</t>
+          <t>NEWCO SWANSEA SOCIAL INFRASTRUCTURE LP</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>16459548</t>
+          <t>LP024176</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3988,12 +3988,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>INDEXIE LTD</t>
+          <t>APEX PREMIER PROPERTY SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>16459546</t>
+          <t>16456756</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -4025,12 +4025,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>OCEANHEART MARINE SERVICE CO., LTD</t>
+          <t>FLIP IT GLOBAL LTD</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>16459543</t>
+          <t>16456758</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4062,12 +4062,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>J.R'S SOUTHERN TWIST LTD</t>
+          <t>DEHBINI LIMITED</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>16459542</t>
+          <t>16456493</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -4099,12 +4099,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>SSFBN LIMITED</t>
+          <t>HONG KONG XUNHUA FREIGHT LIMITED</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>16459541</t>
+          <t>16456735</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">

</xml_diff>

<commit_message>
Auto update: 2025-05-19 20:37:58
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -503,7 +503,7 @@
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16457945</t>
+          <t>16456234</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -532,7 +532,7 @@
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16459062</t>
+          <t>16456242</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -561,7 +561,7 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16459061</t>
+          <t>16456243</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -590,7 +590,7 @@
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16459057</t>
+          <t>16456245</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -619,7 +619,7 @@
       <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16459059</t>
+          <t>16456246</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -648,7 +648,7 @@
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16459058</t>
+          <t>16456244</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -677,7 +677,7 @@
       <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16457953</t>
+          <t>16456254</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -706,7 +706,7 @@
       <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16457954</t>
+          <t>16456253</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -735,7 +735,7 @@
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16457973</t>
+          <t>16456250</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -764,7 +764,7 @@
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16457975</t>
+          <t>16456256</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -793,7 +793,7 @@
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16457974</t>
+          <t>16456236</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -822,7 +822,7 @@
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16457943</t>
+          <t>16456233</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -851,7 +851,7 @@
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16456203</t>
+          <t>16457945</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -880,7 +880,7 @@
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16457967</t>
+          <t>16456218</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -909,7 +909,7 @@
       <c r="A17" t="inlineStr"/>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16457965</t>
+          <t>16456221</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -938,7 +938,7 @@
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16457970</t>
+          <t>16456227</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -967,7 +967,7 @@
       <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16457957</t>
+          <t>16456205</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -996,7 +996,7 @@
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr">
         <is>
-          <t>16457962</t>
+          <t>16456208</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1025,7 +1025,7 @@
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16457264</t>
+          <t>16456212</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1054,7 +1054,7 @@
       <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16457261</t>
+          <t>16456261</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1083,7 +1083,7 @@
       <c r="A23" t="inlineStr"/>
       <c r="B23" t="inlineStr">
         <is>
-          <t>NI729522</t>
+          <t>16456712</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1112,7 +1112,7 @@
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16457259</t>
+          <t>16456709</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1141,7 +1141,7 @@
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16457238</t>
+          <t>16456750</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1170,7 +1170,7 @@
       <c r="A26" t="inlineStr"/>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16459074</t>
+          <t>16456749</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1199,7 +1199,7 @@
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16459078</t>
+          <t>16456754</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1228,7 +1228,7 @@
       <c r="A28" t="inlineStr"/>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16459077</t>
+          <t>16457272</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1257,7 +1257,7 @@
       <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16459069</t>
+          <t>16456748</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1286,7 +1286,7 @@
       <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16459541</t>
+          <t>16456735</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1315,7 +1315,7 @@
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16459542</t>
+          <t>16456493</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1344,7 +1344,7 @@
       <c r="A32" t="inlineStr"/>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16459543</t>
+          <t>16456758</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1373,7 +1373,7 @@
       <c r="A33" t="inlineStr"/>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16459546</t>
+          <t>16456756</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1402,7 +1402,7 @@
       <c r="A34" t="inlineStr"/>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16459548</t>
+          <t>LP024176</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1431,7 +1431,7 @@
       <c r="A35" t="inlineStr"/>
       <c r="B35" t="inlineStr">
         <is>
-          <t>16459547</t>
+          <t>16456734</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1460,7 +1460,7 @@
       <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16459549</t>
+          <t>16456733</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1489,7 +1489,7 @@
       <c r="A37" t="inlineStr"/>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16459514</t>
+          <t>16456731</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1518,7 +1518,7 @@
       <c r="A38" t="inlineStr"/>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16459516</t>
+          <t>16456764</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1547,7 +1547,7 @@
       <c r="A39" t="inlineStr"/>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16459518</t>
+          <t>16456765</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1576,7 +1576,7 @@
       <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16459515</t>
+          <t>16456701</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1605,7 +1605,7 @@
       <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr">
         <is>
-          <t>16459512</t>
+          <t>16456706</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1634,7 +1634,7 @@
       <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16459520</t>
+          <t>16456708</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1663,7 +1663,7 @@
       <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16459521</t>
+          <t>16457230</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1692,7 +1692,7 @@
       <c r="A44" t="inlineStr"/>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16459523</t>
+          <t>NI729519</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1721,7 +1721,7 @@
       <c r="A45" t="inlineStr"/>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16459522</t>
+          <t>16457262</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1750,7 +1750,7 @@
       <c r="A46" t="inlineStr"/>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16459526</t>
+          <t>16457268</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1779,7 +1779,7 @@
       <c r="A47" t="inlineStr"/>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16459072</t>
+          <t>16457273</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1808,7 +1808,7 @@
       <c r="A48" t="inlineStr"/>
       <c r="B48" t="inlineStr">
         <is>
-          <t>16459082</t>
+          <t>16457265</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1837,7 +1837,7 @@
       <c r="A49" t="inlineStr"/>
       <c r="B49" t="inlineStr">
         <is>
-          <t>16459084</t>
+          <t>16457270</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1866,7 +1866,7 @@
       <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16459064</t>
+          <t>16457267</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1895,7 +1895,7 @@
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr">
         <is>
-          <t>16457237</t>
+          <t>16457279</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1953,7 +1953,7 @@
       <c r="A53" t="inlineStr"/>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16457279</t>
+          <t>16457237</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1982,7 +1982,7 @@
       <c r="A54" t="inlineStr"/>
       <c r="B54" t="inlineStr">
         <is>
-          <t>16456750</t>
+          <t>16459074</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2011,7 +2011,7 @@
       <c r="A55" t="inlineStr"/>
       <c r="B55" t="inlineStr">
         <is>
-          <t>16456709</t>
+          <t>16457259</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2040,7 +2040,7 @@
       <c r="A56" t="inlineStr"/>
       <c r="B56" t="inlineStr">
         <is>
-          <t>16456712</t>
+          <t>NI729522</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2069,7 +2069,7 @@
       <c r="A57" t="inlineStr"/>
       <c r="B57" t="inlineStr">
         <is>
-          <t>16456261</t>
+          <t>16457261</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2098,7 +2098,7 @@
       <c r="A58" t="inlineStr"/>
       <c r="B58" t="inlineStr">
         <is>
-          <t>16456212</t>
+          <t>16457264</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2127,7 +2127,7 @@
       <c r="A59" t="inlineStr"/>
       <c r="B59" t="inlineStr">
         <is>
-          <t>16456208</t>
+          <t>16457962</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2156,7 +2156,7 @@
       <c r="A60" t="inlineStr"/>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16456205</t>
+          <t>16457957</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2185,7 +2185,7 @@
       <c r="A61" t="inlineStr"/>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16456227</t>
+          <t>16457970</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2214,7 +2214,7 @@
       <c r="A62" t="inlineStr"/>
       <c r="B62" t="inlineStr">
         <is>
-          <t>16456221</t>
+          <t>16457965</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2243,7 +2243,7 @@
       <c r="A63" t="inlineStr"/>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16456218</t>
+          <t>16457967</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2272,7 +2272,7 @@
       <c r="A64" t="inlineStr"/>
       <c r="B64" t="inlineStr">
         <is>
-          <t>16456233</t>
+          <t>16456203</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2301,7 +2301,7 @@
       <c r="A65" t="inlineStr"/>
       <c r="B65" t="inlineStr">
         <is>
-          <t>16456234</t>
+          <t>16457943</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2330,7 +2330,7 @@
       <c r="A66" t="inlineStr"/>
       <c r="B66" t="inlineStr">
         <is>
-          <t>16456236</t>
+          <t>16457974</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2359,7 +2359,7 @@
       <c r="A67" t="inlineStr"/>
       <c r="B67" t="inlineStr">
         <is>
-          <t>16456256</t>
+          <t>16457975</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2388,7 +2388,7 @@
       <c r="A68" t="inlineStr"/>
       <c r="B68" t="inlineStr">
         <is>
-          <t>16456250</t>
+          <t>16457973</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2417,7 +2417,7 @@
       <c r="A69" t="inlineStr"/>
       <c r="B69" t="inlineStr">
         <is>
-          <t>16456253</t>
+          <t>16457954</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2446,7 +2446,7 @@
       <c r="A70" t="inlineStr"/>
       <c r="B70" t="inlineStr">
         <is>
-          <t>16456254</t>
+          <t>16457953</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2475,7 +2475,7 @@
       <c r="A71" t="inlineStr"/>
       <c r="B71" t="inlineStr">
         <is>
-          <t>16456244</t>
+          <t>16459058</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2504,7 +2504,7 @@
       <c r="A72" t="inlineStr"/>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16456246</t>
+          <t>16459059</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2533,7 +2533,7 @@
       <c r="A73" t="inlineStr"/>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16456245</t>
+          <t>16459057</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2562,7 +2562,7 @@
       <c r="A74" t="inlineStr"/>
       <c r="B74" t="inlineStr">
         <is>
-          <t>16456243</t>
+          <t>16459061</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2591,7 +2591,7 @@
       <c r="A75" t="inlineStr"/>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16456242</t>
+          <t>16459062</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2620,7 +2620,7 @@
       <c r="A76" t="inlineStr"/>
       <c r="B76" t="inlineStr">
         <is>
-          <t>16456749</t>
+          <t>16457238</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2649,7 +2649,7 @@
       <c r="A77" t="inlineStr"/>
       <c r="B77" t="inlineStr">
         <is>
-          <t>16456754</t>
+          <t>16459078</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2678,7 +2678,7 @@
       <c r="A78" t="inlineStr"/>
       <c r="B78" t="inlineStr">
         <is>
-          <t>16457272</t>
+          <t>16459064</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2707,7 +2707,7 @@
       <c r="A79" t="inlineStr"/>
       <c r="B79" t="inlineStr">
         <is>
-          <t>16456748</t>
+          <t>16459077</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2736,7 +2736,7 @@
       <c r="A80" t="inlineStr"/>
       <c r="B80" t="inlineStr">
         <is>
-          <t>16457267</t>
+          <t>16459084</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2765,7 +2765,7 @@
       <c r="A81" t="inlineStr"/>
       <c r="B81" t="inlineStr">
         <is>
-          <t>16457270</t>
+          <t>16459082</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2794,7 +2794,7 @@
       <c r="A82" t="inlineStr"/>
       <c r="B82" t="inlineStr">
         <is>
-          <t>16457265</t>
+          <t>16459072</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2823,7 +2823,7 @@
       <c r="A83" t="inlineStr"/>
       <c r="B83" t="inlineStr">
         <is>
-          <t>16457273</t>
+          <t>16459526</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2852,7 +2852,7 @@
       <c r="A84" t="inlineStr"/>
       <c r="B84" t="inlineStr">
         <is>
-          <t>16457268</t>
+          <t>16459522</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2881,7 +2881,7 @@
       <c r="A85" t="inlineStr"/>
       <c r="B85" t="inlineStr">
         <is>
-          <t>16457262</t>
+          <t>16459523</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2910,7 +2910,7 @@
       <c r="A86" t="inlineStr"/>
       <c r="B86" t="inlineStr">
         <is>
-          <t>NI729519</t>
+          <t>16459521</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2939,7 +2939,7 @@
       <c r="A87" t="inlineStr"/>
       <c r="B87" t="inlineStr">
         <is>
-          <t>16457230</t>
+          <t>16459520</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2968,7 +2968,7 @@
       <c r="A88" t="inlineStr"/>
       <c r="B88" t="inlineStr">
         <is>
-          <t>16456708</t>
+          <t>16459512</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2997,7 +2997,7 @@
       <c r="A89" t="inlineStr"/>
       <c r="B89" t="inlineStr">
         <is>
-          <t>16456706</t>
+          <t>16459515</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3026,7 +3026,7 @@
       <c r="A90" t="inlineStr"/>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16456701</t>
+          <t>16459518</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3055,7 +3055,7 @@
       <c r="A91" t="inlineStr"/>
       <c r="B91" t="inlineStr">
         <is>
-          <t>16456765</t>
+          <t>16459516</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3084,7 +3084,7 @@
       <c r="A92" t="inlineStr"/>
       <c r="B92" t="inlineStr">
         <is>
-          <t>16456764</t>
+          <t>16459514</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3113,7 +3113,7 @@
       <c r="A93" t="inlineStr"/>
       <c r="B93" t="inlineStr">
         <is>
-          <t>16456731</t>
+          <t>16459549</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3142,7 +3142,7 @@
       <c r="A94" t="inlineStr"/>
       <c r="B94" t="inlineStr">
         <is>
-          <t>16456733</t>
+          <t>16459547</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3171,7 +3171,7 @@
       <c r="A95" t="inlineStr"/>
       <c r="B95" t="inlineStr">
         <is>
-          <t>16456734</t>
+          <t>16459548</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3200,7 +3200,7 @@
       <c r="A96" t="inlineStr"/>
       <c r="B96" t="inlineStr">
         <is>
-          <t>LP024176</t>
+          <t>16459546</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3229,7 +3229,7 @@
       <c r="A97" t="inlineStr"/>
       <c r="B97" t="inlineStr">
         <is>
-          <t>16456756</t>
+          <t>16459543</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3258,7 +3258,7 @@
       <c r="A98" t="inlineStr"/>
       <c r="B98" t="inlineStr">
         <is>
-          <t>16456758</t>
+          <t>16459542</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3287,7 +3287,7 @@
       <c r="A99" t="inlineStr"/>
       <c r="B99" t="inlineStr">
         <is>
-          <t>16456493</t>
+          <t>16459541</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3316,7 +3316,7 @@
       <c r="A100" t="inlineStr"/>
       <c r="B100" t="inlineStr">
         <is>
-          <t>16456735</t>
+          <t>16459069</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">

</xml_diff>

<commit_message>
Auto update: 2025-05-19 21:33:46
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,11 @@
           <t>Time Discovered</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -502,16 +507,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CALIBRE LDN LIMITED</t>
+          <t>A STAR HEALTH LTD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16457945</t>
+          <t>16456234</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -535,16 +541,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SHOTTON CURRY HOUSE LIMITED</t>
+          <t>J&amp;S DISTRIBUTIONS LIMITED</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16459062</t>
+          <t>16456242</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -568,16 +575,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CAZAM PROPERTY LTD</t>
+          <t>B HOLLAND &amp; SONS (HOLDINGS) LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16459061</t>
+          <t>16456243</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -601,16 +609,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>M S GROUP FIRST UK LIMITED</t>
+          <t>SOCIAL SLOT LTD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16459057</t>
+          <t>16456245</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -634,16 +643,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PARKSIDE GETAWAYS LIMITED</t>
+          <t>UKG BB HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16459059</t>
+          <t>16456246</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -667,16 +677,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DRIVERIGHT REPAIRS LTD</t>
+          <t>KINARA PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16459058</t>
+          <t>16456244</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -700,16 +711,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GK ZYGALA LIMITED</t>
+          <t>MARKETING DG LTD</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16457953</t>
+          <t>16456254</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -733,16 +745,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MAPLE (510) LIMITED</t>
+          <t>EVO AVIATION LIMITED</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16457954</t>
+          <t>16456253</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -766,16 +779,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PANEER CRAFT LTD. LIMITED</t>
+          <t>SWIFT BUSINESS GROWTH.AI LTD</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16457973</t>
+          <t>16456250</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -799,16 +813,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CAMBRIDGE VETS LTD</t>
+          <t>JC DEEP TECH LTD</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16457975</t>
+          <t>16456256</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -832,16 +847,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ROCK&amp;WALLS LTD</t>
+          <t>HAUS OF PALETTE LTD</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16457974</t>
+          <t>16456236</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -865,16 +881,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PROOFENANCE LTD</t>
+          <t>JANITZA UK LIMITED</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16457943</t>
+          <t>16456233</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -898,16 +915,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>HARRY'S OFFLICENCE &amp; TAKEAWAY LTD</t>
+          <t>CALIBRE LDN LIMITED</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16456203</t>
+          <t>16457945</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -931,16 +949,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>INSPOCL LTD</t>
+          <t>HOUSE OF RODEOS LTD</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16457967</t>
+          <t>16456218</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -964,16 +983,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>LEADANICS LIMITED</t>
+          <t>JAI-HO STAFFING LTD</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16457965</t>
+          <t>16456221</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -997,16 +1017,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DEVIPROX LTD</t>
+          <t>WINDOW CLEANING SOUTHEND LTD</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16457970</t>
+          <t>16456227</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1030,16 +1051,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>LGAM PROPERTIES LTD</t>
+          <t>IDCHEM CONSULTING LIMITED</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16457957</t>
+          <t>16456205</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1063,16 +1085,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BUILTBRITE LTD</t>
+          <t>STEFANPERSAUDLEGACYPROJECT LIMITED</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>16457962</t>
+          <t>16456208</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1096,16 +1119,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GUIDED BRAKE SERVICE LTD</t>
+          <t>STOA PROJECTS LTD</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16457264</t>
+          <t>16456212</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1129,16 +1153,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>OMR ELECTRICAL LTD</t>
+          <t>CHIMNEY CHAPS LTD</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16457261</t>
+          <t>16456261</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1162,16 +1187,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>AUSTIN RICE LTD</t>
+          <t>LEOFRIC LTD</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>NI729522</t>
+          <t>16456712</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1195,16 +1221,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>HOLYWELL HOMES LTD</t>
+          <t>BREEZY HOMES LIMITED</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16457259</t>
+          <t>16456709</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1228,16 +1255,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>RELIABLE STAFFING RECRUITS LIMITED</t>
+          <t>ELLISA'S BEAUTY LTD</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16457238</t>
+          <t>16456750</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1261,16 +1289,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>GODMADE LTD</t>
+          <t>ATSP FIN LTD</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16459074</t>
+          <t>16456749</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1294,16 +1323,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>LATINOS TEESSIDE &amp; HISPANIC SENIORS COMMUNITY LTD</t>
+          <t>KHAZAG FREIGHT SERVICES PVT LTD</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16459078</t>
+          <t>16456754</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1327,16 +1357,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>RENTAL DISREPAIR CLAIMS LTD</t>
+          <t>DCR HOLDINGS &amp; INVESTMENTS LTD</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16459077</t>
+          <t>16457272</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1360,16 +1391,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>INP SERVICES LTD</t>
+          <t>FARYAL ENTERPRISE LIMITED</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16459069</t>
+          <t>16456748</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1393,16 +1425,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SSFBN LIMITED</t>
+          <t>HONG KONG XUNHUA FREIGHT LIMITED</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16459541</t>
+          <t>16456735</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1426,16 +1459,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>J.R'S SOUTHERN TWIST LTD</t>
+          <t>DEHBINI LIMITED</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16459542</t>
+          <t>16456493</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1459,16 +1493,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>OCEANHEART MARINE SERVICE CO., LTD</t>
+          <t>FLIP IT GLOBAL LTD</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16459543</t>
+          <t>16456758</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1492,16 +1527,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>INDEXIE LTD</t>
+          <t>APEX PREMIER PROPERTY SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16459546</t>
+          <t>16456756</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1525,16 +1561,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>UBAH MEDIA LAB LTD</t>
+          <t>NEWCO SWANSEA SOCIAL INFRASTRUCTURE LP</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16459548</t>
+          <t>LP024176</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1558,16 +1595,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CA ELECTRICAL (YORKSHIRE) LTD</t>
+          <t>MEC SURVEYORS LTD</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>16459547</t>
+          <t>16456734</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1591,16 +1629,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>LOUD AND CLEAR COACHING LIMITED</t>
+          <t>BKK EQUESTRIAN LTD</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16459549</t>
+          <t>16456733</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1624,16 +1663,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>NORDIC COOPERATION TECHNOLOGIES LIMITED</t>
+          <t>WGHR JI LTD</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16459514</t>
+          <t>16456731</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1657,16 +1697,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CLARK AND CO DESIGN LIMITED</t>
+          <t>OPM ILL GO SHOP 4U LTD</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16459516</t>
+          <t>16456764</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1690,16 +1731,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>MILLE TRADING LTD</t>
+          <t>PHONE STUDIO SOUTH LIMITED</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16459518</t>
+          <t>16456765</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1723,16 +1765,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>SPYRO APPAREL LTD</t>
+          <t>CTLO LTD</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16459515</t>
+          <t>16456701</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1756,16 +1799,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>THE CHAIR SALON LONDON LTD</t>
+          <t>OILMYCAR LTD</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>16459512</t>
+          <t>16456706</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1789,16 +1833,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>AMIS &amp; WARD DEVELOPMENT LTD</t>
+          <t>NEHHEALTHCARE LTD</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16459520</t>
+          <t>16456708</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1822,16 +1867,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>CLICKSPHARE CRAFT LTD</t>
+          <t>MAJESTIC EXTERIOR CLEANING SERVICES LTD</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16459521</t>
+          <t>16457230</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1855,16 +1901,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>TASHAN MEDIA LTD</t>
+          <t>JORDAN CAMPBELL LTD</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16459523</t>
+          <t>NI729519</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1888,16 +1935,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>S&amp;S ISTITHMĀR LTD</t>
+          <t>Y-3 APARTMENTS LTD</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16459522</t>
+          <t>16457262</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1921,16 +1969,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>WANNABEE LTD</t>
+          <t>YSGARLAD PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16459526</t>
+          <t>16457268</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1954,16 +2003,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>FINTIVITY LTD</t>
+          <t>METAHAVEN LTD</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16459072</t>
+          <t>16457273</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1987,16 +2037,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>FASHLER LTD</t>
+          <t>GLIMORA GLOBAL LTD</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>16459082</t>
+          <t>16457265</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2020,16 +2071,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>CTPROPS LIMITED</t>
+          <t>POWERS ELECTRICAL LTD</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>16459084</t>
+          <t>16457270</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2053,16 +2105,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>MALHAMDALE GLAMPING LIMITED</t>
+          <t>PHOENIX CONSULTING INTERNATIONAL LIMITED</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16459064</t>
+          <t>16457267</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2086,16 +2139,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>NEW MOUNT DAISY LIMITED</t>
+          <t>FARRINGDON HOUSE FINANCIAL SERVICES LIMITED</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>16457237</t>
+          <t>16457279</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2119,6 +2173,7 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2152,16 +2207,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>FARRINGDON HOUSE FINANCIAL SERVICES LIMITED</t>
+          <t>NEW MOUNT DAISY LIMITED</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16457279</t>
+          <t>16457237</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2185,16 +2241,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>ELLISA'S BEAUTY LTD</t>
+          <t>GODMADE LTD</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>16456750</t>
+          <t>16459074</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2218,16 +2275,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>BREEZY HOMES LIMITED</t>
+          <t>HOLYWELL HOMES LTD</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>16456709</t>
+          <t>16457259</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2251,16 +2309,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>LEOFRIC LTD</t>
+          <t>AUSTIN RICE LTD</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>16456712</t>
+          <t>NI729522</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2284,16 +2343,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>CHIMNEY CHAPS LTD</t>
+          <t>OMR ELECTRICAL LTD</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>16456261</t>
+          <t>16457261</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2317,16 +2377,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>STOA PROJECTS LTD</t>
+          <t>GUIDED BRAKE SERVICE LTD</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>16456212</t>
+          <t>16457264</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2350,16 +2411,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>STEFANPERSAUDLEGACYPROJECT LIMITED</t>
+          <t>BUILTBRITE LTD</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>16456208</t>
+          <t>16457962</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2383,16 +2445,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>IDCHEM CONSULTING LIMITED</t>
+          <t>LGAM PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16456205</t>
+          <t>16457957</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2416,16 +2479,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>WINDOW CLEANING SOUTHEND LTD</t>
+          <t>DEVIPROX LTD</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16456227</t>
+          <t>16457970</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2449,16 +2513,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>JAI-HO STAFFING LTD</t>
+          <t>LEADANICS LIMITED</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>16456221</t>
+          <t>16457965</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2482,16 +2547,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>HOUSE OF RODEOS LTD</t>
+          <t>INSPOCL LTD</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16456218</t>
+          <t>16457967</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2515,16 +2581,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>JANITZA UK LIMITED</t>
+          <t>HARRY'S OFFLICENCE &amp; TAKEAWAY LTD</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>16456233</t>
+          <t>16456203</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2548,16 +2615,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>A STAR HEALTH LTD</t>
+          <t>PROOFENANCE LTD</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>16456234</t>
+          <t>16457943</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2581,16 +2649,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>HAUS OF PALETTE LTD</t>
+          <t>ROCK&amp;WALLS LTD</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>16456236</t>
+          <t>16457974</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2614,16 +2683,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>JC DEEP TECH LTD</t>
+          <t>CAMBRIDGE VETS LTD</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>16456256</t>
+          <t>16457975</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2647,16 +2717,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>SWIFT BUSINESS GROWTH.AI LTD</t>
+          <t>PANEER CRAFT LTD. LIMITED</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>16456250</t>
+          <t>16457973</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2680,16 +2751,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>EVO AVIATION LIMITED</t>
+          <t>MAPLE (510) LIMITED</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>16456253</t>
+          <t>16457954</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2713,16 +2785,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>MARKETING DG LTD</t>
+          <t>GK ZYGALA LIMITED</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>16456254</t>
+          <t>16457953</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2746,16 +2819,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>KINARA PROPERTIES LTD</t>
+          <t>DRIVERIGHT REPAIRS LTD</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>16456244</t>
+          <t>16459058</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2779,16 +2853,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>UKG BB HOLDINGS LTD</t>
+          <t>PARKSIDE GETAWAYS LIMITED</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16456246</t>
+          <t>16459059</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2812,16 +2887,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>SOCIAL SLOT LTD</t>
+          <t>M S GROUP FIRST UK LIMITED</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16456245</t>
+          <t>16459057</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2845,16 +2921,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>B HOLLAND &amp; SONS (HOLDINGS) LTD</t>
+          <t>CAZAM PROPERTY LTD</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>16456243</t>
+          <t>16459061</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2878,16 +2955,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>J&amp;S DISTRIBUTIONS LIMITED</t>
+          <t>SHOTTON CURRY HOUSE LIMITED</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16456242</t>
+          <t>16459062</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2911,16 +2989,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>ATSP FIN LTD</t>
+          <t>RELIABLE STAFFING RECRUITS LIMITED</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>16456749</t>
+          <t>16457238</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2944,16 +3023,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>KHAZAG FREIGHT SERVICES PVT LTD</t>
+          <t>LATINOS TEESSIDE &amp; HISPANIC SENIORS COMMUNITY LTD</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>16456754</t>
+          <t>16459078</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2977,16 +3057,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>DCR HOLDINGS &amp; INVESTMENTS LTD</t>
+          <t>MALHAMDALE GLAMPING LIMITED</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>16457272</t>
+          <t>16459064</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3010,16 +3091,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>FARYAL ENTERPRISE LIMITED</t>
+          <t>RENTAL DISREPAIR CLAIMS LTD</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>16456748</t>
+          <t>16459077</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3043,16 +3125,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>PHOENIX CONSULTING INTERNATIONAL LIMITED</t>
+          <t>CTPROPS LIMITED</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>16457267</t>
+          <t>16459084</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3076,16 +3159,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>POWERS ELECTRICAL LTD</t>
+          <t>FASHLER LTD</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>16457270</t>
+          <t>16459082</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3109,16 +3193,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>GLIMORA GLOBAL LTD</t>
+          <t>FINTIVITY LTD</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>16457265</t>
+          <t>16459072</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3142,16 +3227,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>METAHAVEN LTD</t>
+          <t>WANNABEE LTD</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>16457273</t>
+          <t>16459526</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3175,16 +3261,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>YSGARLAD PROPERTIES LTD</t>
+          <t>S&amp;S ISTITHMĀR LTD</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>16457268</t>
+          <t>16459522</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3208,16 +3295,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Y-3 APARTMENTS LTD</t>
+          <t>TASHAN MEDIA LTD</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>16457262</t>
+          <t>16459523</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3241,16 +3329,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>JORDAN CAMPBELL LTD</t>
+          <t>CLICKSPHARE CRAFT LTD</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>NI729519</t>
+          <t>16459521</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3274,16 +3363,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>MAJESTIC EXTERIOR CLEANING SERVICES LTD</t>
+          <t>AMIS &amp; WARD DEVELOPMENT LTD</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>16457230</t>
+          <t>16459520</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3307,16 +3397,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>NEHHEALTHCARE LTD</t>
+          <t>THE CHAIR SALON LONDON LTD</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>16456708</t>
+          <t>16459512</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3340,16 +3431,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>OILMYCAR LTD</t>
+          <t>SPYRO APPAREL LTD</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>16456706</t>
+          <t>16459515</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3373,16 +3465,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>CTLO LTD</t>
+          <t>MILLE TRADING LTD</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16456701</t>
+          <t>16459518</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3406,16 +3499,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>PHONE STUDIO SOUTH LIMITED</t>
+          <t>CLARK AND CO DESIGN LIMITED</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>16456765</t>
+          <t>16459516</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3439,16 +3533,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>OPM ILL GO SHOP 4U LTD</t>
+          <t>NORDIC COOPERATION TECHNOLOGIES LIMITED</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>16456764</t>
+          <t>16459514</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3472,16 +3567,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>WGHR JI LTD</t>
+          <t>LOUD AND CLEAR COACHING LIMITED</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>16456731</t>
+          <t>16459549</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3505,16 +3601,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>BKK EQUESTRIAN LTD</t>
+          <t>CA ELECTRICAL (YORKSHIRE) LTD</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>16456733</t>
+          <t>16459547</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3538,16 +3635,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>MEC SURVEYORS LTD</t>
+          <t>UBAH MEDIA LAB LTD</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>16456734</t>
+          <t>16459548</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3571,16 +3669,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>NEWCO SWANSEA SOCIAL INFRASTRUCTURE LP</t>
+          <t>INDEXIE LTD</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>LP024176</t>
+          <t>16459546</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3604,16 +3703,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>APEX PREMIER PROPERTY SOLUTIONS LTD</t>
+          <t>OCEANHEART MARINE SERVICE CO., LTD</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>16456756</t>
+          <t>16459543</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3637,16 +3737,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>FLIP IT GLOBAL LTD</t>
+          <t>J.R'S SOUTHERN TWIST LTD</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>16456758</t>
+          <t>16459542</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3670,16 +3771,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>DEHBINI LIMITED</t>
+          <t>SSFBN LIMITED</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>16456493</t>
+          <t>16459541</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3703,16 +3805,17 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>HONG KONG XUNHUA FREIGHT LIMITED</t>
+          <t>INP SERVICES LTD</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>16456735</t>
+          <t>16459069</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3736,6 +3839,7 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3769,6 +3873,7 @@
           <t>20:46:00</t>
         </is>
       </c>
+      <c r="H101" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Auto update: 2025-05-19 22:39:17
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -516,12 +516,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CALIBRE LDN LIMITED</t>
+          <t>A STAR HEALTH LTD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16457945</t>
+          <t>16456234</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -554,12 +554,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SHOTTON CURRY HOUSE LIMITED</t>
+          <t>J&amp;S DISTRIBUTIONS LIMITED</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16459062</t>
+          <t>16456242</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -592,12 +592,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CAZAM PROPERTY LTD</t>
+          <t>B HOLLAND &amp; SONS (HOLDINGS) LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16459061</t>
+          <t>16456243</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -630,12 +630,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>M S GROUP FIRST UK LIMITED</t>
+          <t>SOCIAL SLOT LTD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16459057</t>
+          <t>16456245</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -668,12 +668,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PARKSIDE GETAWAYS LIMITED</t>
+          <t>UKG BB HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16459059</t>
+          <t>16456246</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -706,12 +706,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DRIVERIGHT REPAIRS LTD</t>
+          <t>KINARA PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16459058</t>
+          <t>16456244</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -744,12 +744,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GK ZYGALA LIMITED</t>
+          <t>MARKETING DG LTD</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16457953</t>
+          <t>16456254</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -782,12 +782,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MAPLE (510) LIMITED</t>
+          <t>EVO AVIATION LIMITED</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16457954</t>
+          <t>16456253</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -820,12 +820,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PANEER CRAFT LTD. LIMITED</t>
+          <t>SWIFT BUSINESS GROWTH.AI LTD</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16457973</t>
+          <t>16456250</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -858,12 +858,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CAMBRIDGE VETS LTD</t>
+          <t>JC DEEP TECH LTD</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16457975</t>
+          <t>16456256</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -896,12 +896,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ROCK&amp;WALLS LTD</t>
+          <t>HAUS OF PALETTE LTD</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16457974</t>
+          <t>16456236</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -934,12 +934,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PROOFENANCE LTD</t>
+          <t>JANITZA UK LIMITED</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16457943</t>
+          <t>16456233</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -972,12 +972,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>HARRY'S OFFLICENCE &amp; TAKEAWAY LTD</t>
+          <t>CALIBRE LDN LIMITED</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16456203</t>
+          <t>16457945</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1010,12 +1010,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>INSPOCL LTD</t>
+          <t>HOUSE OF RODEOS LTD</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16457967</t>
+          <t>16456218</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1048,12 +1048,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>LEADANICS LIMITED</t>
+          <t>JAI-HO STAFFING LTD</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16457965</t>
+          <t>16456221</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1086,12 +1086,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DEVIPROX LTD</t>
+          <t>WINDOW CLEANING SOUTHEND LTD</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16457970</t>
+          <t>16456227</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1124,12 +1124,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>LGAM PROPERTIES LTD</t>
+          <t>IDCHEM CONSULTING LIMITED</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16457957</t>
+          <t>16456205</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1162,12 +1162,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BUILTBRITE LTD</t>
+          <t>STEFANPERSAUDLEGACYPROJECT LIMITED</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>16457962</t>
+          <t>16456208</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1200,12 +1200,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GUIDED BRAKE SERVICE LTD</t>
+          <t>STOA PROJECTS LTD</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16457264</t>
+          <t>16456212</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1238,12 +1238,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>OMR ELECTRICAL LTD</t>
+          <t>CHIMNEY CHAPS LTD</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16457261</t>
+          <t>16456261</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1276,12 +1276,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>AUSTIN RICE LTD</t>
+          <t>LEOFRIC LTD</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>NI729522</t>
+          <t>16456712</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1314,12 +1314,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>HOLYWELL HOMES LTD</t>
+          <t>BREEZY HOMES LIMITED</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16457259</t>
+          <t>16456709</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1352,12 +1352,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>RELIABLE STAFFING RECRUITS LIMITED</t>
+          <t>ELLISA'S BEAUTY LTD</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16457238</t>
+          <t>16456750</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1390,12 +1390,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>GODMADE LTD</t>
+          <t>ATSP FIN LTD</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16459074</t>
+          <t>16456749</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1428,12 +1428,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>LATINOS TEESSIDE &amp; HISPANIC SENIORS COMMUNITY LTD</t>
+          <t>KHAZAG FREIGHT SERVICES PVT LTD</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16459078</t>
+          <t>16456754</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1466,12 +1466,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>RENTAL DISREPAIR CLAIMS LTD</t>
+          <t>DCR HOLDINGS &amp; INVESTMENTS LTD</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16459077</t>
+          <t>16457272</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1497,19 +1497,19 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Investments</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>INP SERVICES LTD</t>
+          <t>FARYAL ENTERPRISE LIMITED</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16459069</t>
+          <t>16456748</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1542,12 +1542,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SSFBN LIMITED</t>
+          <t>HONG KONG XUNHUA FREIGHT LIMITED</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16459541</t>
+          <t>16456735</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1580,12 +1580,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>J.R'S SOUTHERN TWIST LTD</t>
+          <t>DEHBINI LIMITED</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16459542</t>
+          <t>16456493</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1618,12 +1618,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>OCEANHEART MARINE SERVICE CO., LTD</t>
+          <t>FLIP IT GLOBAL LTD</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16459543</t>
+          <t>16456758</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1656,12 +1656,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>INDEXIE LTD</t>
+          <t>APEX PREMIER PROPERTY SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16459546</t>
+          <t>16456756</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1694,12 +1694,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>UBAH MEDIA LAB LTD</t>
+          <t>NEWCO SWANSEA SOCIAL INFRASTRUCTURE LP</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16459548</t>
+          <t>LP024176</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1725,19 +1725,19 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CA ELECTRICAL (YORKSHIRE) LTD</t>
+          <t>MEC SURVEYORS LTD</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>16459547</t>
+          <t>16456734</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1770,12 +1770,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>LOUD AND CLEAR COACHING LIMITED</t>
+          <t>BKK EQUESTRIAN LTD</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16459549</t>
+          <t>16456733</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1808,12 +1808,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>NORDIC COOPERATION TECHNOLOGIES LIMITED</t>
+          <t>WGHR JI LTD</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16459514</t>
+          <t>16456731</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1846,12 +1846,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CLARK AND CO DESIGN LIMITED</t>
+          <t>OPM ILL GO SHOP 4U LTD</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16459516</t>
+          <t>16456764</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1884,12 +1884,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>MILLE TRADING LTD</t>
+          <t>PHONE STUDIO SOUTH LIMITED</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16459518</t>
+          <t>16456765</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1922,12 +1922,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>SPYRO APPAREL LTD</t>
+          <t>CTLO LTD</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16459515</t>
+          <t>16456701</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1960,12 +1960,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>THE CHAIR SALON LONDON LTD</t>
+          <t>OILMYCAR LTD</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>16459512</t>
+          <t>16456706</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1998,12 +1998,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>AMIS &amp; WARD DEVELOPMENT LTD</t>
+          <t>NEHHEALTHCARE LTD</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16459520</t>
+          <t>16456708</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2036,12 +2036,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>CLICKSPHARE CRAFT LTD</t>
+          <t>MAJESTIC EXTERIOR CLEANING SERVICES LTD</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16459521</t>
+          <t>16457230</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2074,12 +2074,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>TASHAN MEDIA LTD</t>
+          <t>JORDAN CAMPBELL LTD</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16459523</t>
+          <t>NI729519</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2112,12 +2112,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>S&amp;S ISTITHMĀR LTD</t>
+          <t>Y-3 APARTMENTS LTD</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16459522</t>
+          <t>16457262</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2150,12 +2150,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>WANNABEE LTD</t>
+          <t>YSGARLAD PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16459526</t>
+          <t>16457268</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2188,12 +2188,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>FINTIVITY LTD</t>
+          <t>METAHAVEN LTD</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16459072</t>
+          <t>16457273</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2226,12 +2226,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>FASHLER LTD</t>
+          <t>GLIMORA GLOBAL LTD</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>16459082</t>
+          <t>16457265</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2264,12 +2264,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>CTPROPS LIMITED</t>
+          <t>POWERS ELECTRICAL LTD</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>16459084</t>
+          <t>16457270</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2302,12 +2302,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>MALHAMDALE GLAMPING LIMITED</t>
+          <t>PHOENIX CONSULTING INTERNATIONAL LIMITED</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16459064</t>
+          <t>16457267</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2340,12 +2340,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>NEW MOUNT DAISY LIMITED</t>
+          <t>FARRINGDON HOUSE FINANCIAL SERVICES LIMITED</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>16457237</t>
+          <t>16457279</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2416,12 +2416,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>FARRINGDON HOUSE FINANCIAL SERVICES LIMITED</t>
+          <t>NEW MOUNT DAISY LIMITED</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16457279</t>
+          <t>16457237</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2454,12 +2454,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>ELLISA'S BEAUTY LTD</t>
+          <t>GODMADE LTD</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>16456750</t>
+          <t>16459074</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2492,12 +2492,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>BREEZY HOMES LIMITED</t>
+          <t>HOLYWELL HOMES LTD</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>16456709</t>
+          <t>16457259</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2530,12 +2530,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>LEOFRIC LTD</t>
+          <t>AUSTIN RICE LTD</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>16456712</t>
+          <t>NI729522</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2568,12 +2568,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>CHIMNEY CHAPS LTD</t>
+          <t>OMR ELECTRICAL LTD</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>16456261</t>
+          <t>16457261</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2606,12 +2606,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>STOA PROJECTS LTD</t>
+          <t>GUIDED BRAKE SERVICE LTD</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>16456212</t>
+          <t>16457264</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2644,12 +2644,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>STEFANPERSAUDLEGACYPROJECT LIMITED</t>
+          <t>BUILTBRITE LTD</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>16456208</t>
+          <t>16457962</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2682,12 +2682,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>IDCHEM CONSULTING LIMITED</t>
+          <t>LGAM PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16456205</t>
+          <t>16457957</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2720,12 +2720,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>WINDOW CLEANING SOUTHEND LTD</t>
+          <t>DEVIPROX LTD</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16456227</t>
+          <t>16457970</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2758,12 +2758,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>JAI-HO STAFFING LTD</t>
+          <t>LEADANICS LIMITED</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>16456221</t>
+          <t>16457965</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2796,12 +2796,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>HOUSE OF RODEOS LTD</t>
+          <t>INSPOCL LTD</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16456218</t>
+          <t>16457967</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2834,12 +2834,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>JANITZA UK LIMITED</t>
+          <t>HARRY'S OFFLICENCE &amp; TAKEAWAY LTD</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>16456233</t>
+          <t>16456203</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2872,12 +2872,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>A STAR HEALTH LTD</t>
+          <t>PROOFENANCE LTD</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>16456234</t>
+          <t>16457943</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2910,12 +2910,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>HAUS OF PALETTE LTD</t>
+          <t>ROCK&amp;WALLS LTD</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>16456236</t>
+          <t>16457974</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2948,12 +2948,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>JC DEEP TECH LTD</t>
+          <t>CAMBRIDGE VETS LTD</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>16456256</t>
+          <t>16457975</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2986,12 +2986,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>SWIFT BUSINESS GROWTH.AI LTD</t>
+          <t>PANEER CRAFT LTD. LIMITED</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>16456250</t>
+          <t>16457973</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3024,12 +3024,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>EVO AVIATION LIMITED</t>
+          <t>MAPLE (510) LIMITED</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>16456253</t>
+          <t>16457954</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3062,12 +3062,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>MARKETING DG LTD</t>
+          <t>GK ZYGALA LIMITED</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>16456254</t>
+          <t>16457953</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3100,12 +3100,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>KINARA PROPERTIES LTD</t>
+          <t>DRIVERIGHT REPAIRS LTD</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>16456244</t>
+          <t>16459058</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3138,12 +3138,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>UKG BB HOLDINGS LTD</t>
+          <t>PARKSIDE GETAWAYS LIMITED</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16456246</t>
+          <t>16459059</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3176,12 +3176,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>SOCIAL SLOT LTD</t>
+          <t>M S GROUP FIRST UK LIMITED</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16456245</t>
+          <t>16459057</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3214,12 +3214,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>B HOLLAND &amp; SONS (HOLDINGS) LTD</t>
+          <t>CAZAM PROPERTY LTD</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>16456243</t>
+          <t>16459061</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3252,12 +3252,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>J&amp;S DISTRIBUTIONS LIMITED</t>
+          <t>SHOTTON CURRY HOUSE LIMITED</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16456242</t>
+          <t>16459062</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3290,12 +3290,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>ATSP FIN LTD</t>
+          <t>RELIABLE STAFFING RECRUITS LIMITED</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>16456749</t>
+          <t>16457238</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3328,12 +3328,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>KHAZAG FREIGHT SERVICES PVT LTD</t>
+          <t>LATINOS TEESSIDE &amp; HISPANIC SENIORS COMMUNITY LTD</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>16456754</t>
+          <t>16459078</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3366,12 +3366,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>DCR HOLDINGS &amp; INVESTMENTS LTD</t>
+          <t>MALHAMDALE GLAMPING LIMITED</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>16457272</t>
+          <t>16459064</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3397,19 +3397,19 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>FARYAL ENTERPRISE LIMITED</t>
+          <t>RENTAL DISREPAIR CLAIMS LTD</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>16456748</t>
+          <t>16459077</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3442,12 +3442,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>PHOENIX CONSULTING INTERNATIONAL LIMITED</t>
+          <t>CTPROPS LIMITED</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>16457267</t>
+          <t>16459084</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3480,12 +3480,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>POWERS ELECTRICAL LTD</t>
+          <t>FASHLER LTD</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>16457270</t>
+          <t>16459082</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3518,12 +3518,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>GLIMORA GLOBAL LTD</t>
+          <t>FINTIVITY LTD</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>16457265</t>
+          <t>16459072</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3556,12 +3556,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>METAHAVEN LTD</t>
+          <t>WANNABEE LTD</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>16457273</t>
+          <t>16459526</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3594,12 +3594,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>YSGARLAD PROPERTIES LTD</t>
+          <t>S&amp;S ISTITHMĀR LTD</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>16457268</t>
+          <t>16459522</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3632,12 +3632,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Y-3 APARTMENTS LTD</t>
+          <t>TASHAN MEDIA LTD</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>16457262</t>
+          <t>16459523</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3670,12 +3670,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>JORDAN CAMPBELL LTD</t>
+          <t>CLICKSPHARE CRAFT LTD</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>NI729519</t>
+          <t>16459521</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3708,12 +3708,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>MAJESTIC EXTERIOR CLEANING SERVICES LTD</t>
+          <t>AMIS &amp; WARD DEVELOPMENT LTD</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>16457230</t>
+          <t>16459520</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3746,12 +3746,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>NEHHEALTHCARE LTD</t>
+          <t>THE CHAIR SALON LONDON LTD</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>16456708</t>
+          <t>16459512</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3784,12 +3784,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>OILMYCAR LTD</t>
+          <t>SPYRO APPAREL LTD</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>16456706</t>
+          <t>16459515</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3822,12 +3822,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>CTLO LTD</t>
+          <t>MILLE TRADING LTD</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16456701</t>
+          <t>16459518</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3860,12 +3860,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>PHONE STUDIO SOUTH LIMITED</t>
+          <t>CLARK AND CO DESIGN LIMITED</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>16456765</t>
+          <t>16459516</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3898,12 +3898,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>OPM ILL GO SHOP 4U LTD</t>
+          <t>NORDIC COOPERATION TECHNOLOGIES LIMITED</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>16456764</t>
+          <t>16459514</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3936,12 +3936,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>WGHR JI LTD</t>
+          <t>LOUD AND CLEAR COACHING LIMITED</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>16456731</t>
+          <t>16459549</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3974,12 +3974,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>BKK EQUESTRIAN LTD</t>
+          <t>CA ELECTRICAL (YORKSHIRE) LTD</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>16456733</t>
+          <t>16459547</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -4012,12 +4012,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>MEC SURVEYORS LTD</t>
+          <t>UBAH MEDIA LAB LTD</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>16456734</t>
+          <t>16459548</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -4050,12 +4050,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>NEWCO SWANSEA SOCIAL INFRASTRUCTURE LP</t>
+          <t>INDEXIE LTD</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>LP024176</t>
+          <t>16459546</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4081,19 +4081,19 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>APEX PREMIER PROPERTY SOLUTIONS LTD</t>
+          <t>OCEANHEART MARINE SERVICE CO., LTD</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>16456756</t>
+          <t>16459543</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -4126,12 +4126,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>FLIP IT GLOBAL LTD</t>
+          <t>J.R'S SOUTHERN TWIST LTD</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>16456758</t>
+          <t>16459542</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4164,12 +4164,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>DEHBINI LIMITED</t>
+          <t>SSFBN LIMITED</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>16456493</t>
+          <t>16459541</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -4202,12 +4202,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>HONG KONG XUNHUA FREIGHT LIMITED</t>
+          <t>INP SERVICES LTD</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>16456735</t>
+          <t>16459069</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">

</xml_diff>

<commit_message>
Auto update: 2025-05-19 23:30:46
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -516,12 +516,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>A STAR HEALTH LTD</t>
+          <t>PROOFENANCE LTD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16456234</t>
+          <t>16457943</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -554,12 +554,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>J&amp;S DISTRIBUTIONS LIMITED</t>
+          <t>SHOTTON CURRY HOUSE LIMITED</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16456242</t>
+          <t>16459062</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -592,12 +592,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>B HOLLAND &amp; SONS (HOLDINGS) LTD</t>
+          <t>CAZAM PROPERTY LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16456243</t>
+          <t>16459061</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -630,12 +630,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SOCIAL SLOT LTD</t>
+          <t>M S GROUP FIRST UK LIMITED</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16456245</t>
+          <t>16459057</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -668,12 +668,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>UKG BB HOLDINGS LTD</t>
+          <t>PARKSIDE GETAWAYS LIMITED</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16456246</t>
+          <t>16459059</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -706,12 +706,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>KINARA PROPERTIES LTD</t>
+          <t>DRIVERIGHT REPAIRS LTD</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16456244</t>
+          <t>16459058</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -744,12 +744,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MARKETING DG LTD</t>
+          <t>GK ZYGALA LIMITED</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16456254</t>
+          <t>16457953</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -782,12 +782,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>EVO AVIATION LIMITED</t>
+          <t>MAPLE (510) LIMITED</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16456253</t>
+          <t>16457954</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -820,12 +820,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SWIFT BUSINESS GROWTH.AI LTD</t>
+          <t>PANEER CRAFT LTD. LIMITED</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16456250</t>
+          <t>16457973</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -858,12 +858,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>JC DEEP TECH LTD</t>
+          <t>CAMBRIDGE VETS LTD</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16456256</t>
+          <t>16457975</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -896,12 +896,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>HAUS OF PALETTE LTD</t>
+          <t>ROCK&amp;WALLS LTD</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16456236</t>
+          <t>16457974</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -934,12 +934,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>JANITZA UK LIMITED</t>
+          <t>HARRY'S OFFLICENCE &amp; TAKEAWAY LTD</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16456233</t>
+          <t>16456203</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -972,12 +972,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CALIBRE LDN LIMITED</t>
+          <t>A STAR HEALTH LTD</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16457945</t>
+          <t>16456234</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1010,12 +1010,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>HOUSE OF RODEOS LTD</t>
+          <t>INSPOCL LTD</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16456218</t>
+          <t>16457967</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1048,12 +1048,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>JAI-HO STAFFING LTD</t>
+          <t>LEADANICS LIMITED</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16456221</t>
+          <t>16457965</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1086,12 +1086,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>WINDOW CLEANING SOUTHEND LTD</t>
+          <t>DEVIPROX LTD</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16456227</t>
+          <t>16457970</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1124,12 +1124,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IDCHEM CONSULTING LIMITED</t>
+          <t>LGAM PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16456205</t>
+          <t>16457957</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1162,12 +1162,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>STEFANPERSAUDLEGACYPROJECT LIMITED</t>
+          <t>BUILTBRITE LTD</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>16456208</t>
+          <t>16457962</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1200,12 +1200,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>STOA PROJECTS LTD</t>
+          <t>GUIDED BRAKE SERVICE LTD</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16456212</t>
+          <t>16457264</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1238,12 +1238,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CHIMNEY CHAPS LTD</t>
+          <t>OMR ELECTRICAL LTD</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16456261</t>
+          <t>16457261</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1276,12 +1276,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>LEOFRIC LTD</t>
+          <t>AUSTIN RICE LTD</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>16456712</t>
+          <t>NI729522</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1314,12 +1314,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>BREEZY HOMES LIMITED</t>
+          <t>HOLYWELL HOMES LTD</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16456709</t>
+          <t>16457259</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1352,12 +1352,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ELLISA'S BEAUTY LTD</t>
+          <t>GODMADE LTD</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16456750</t>
+          <t>16459074</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1390,12 +1390,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ATSP FIN LTD</t>
+          <t>RELIABLE STAFFING RECRUITS LIMITED</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16456749</t>
+          <t>16457238</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1428,12 +1428,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>KHAZAG FREIGHT SERVICES PVT LTD</t>
+          <t>LATINOS TEESSIDE &amp; HISPANIC SENIORS COMMUNITY LTD</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16456754</t>
+          <t>16459078</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1466,12 +1466,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>DCR HOLDINGS &amp; INVESTMENTS LTD</t>
+          <t>MALHAMDALE GLAMPING LIMITED</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16457272</t>
+          <t>16459064</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1497,19 +1497,19 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>FARYAL ENTERPRISE LIMITED</t>
+          <t>RENTAL DISREPAIR CLAIMS LTD</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16456748</t>
+          <t>16459077</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1542,12 +1542,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>HONG KONG XUNHUA FREIGHT LIMITED</t>
+          <t>INP SERVICES LTD</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16456735</t>
+          <t>16459069</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1580,12 +1580,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>DEHBINI LIMITED</t>
+          <t>SSFBN LIMITED</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16456493</t>
+          <t>16459541</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1618,12 +1618,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>FLIP IT GLOBAL LTD</t>
+          <t>J.R'S SOUTHERN TWIST LTD</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16456758</t>
+          <t>16459542</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1656,12 +1656,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>APEX PREMIER PROPERTY SOLUTIONS LTD</t>
+          <t>OCEANHEART MARINE SERVICE CO., LTD</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16456756</t>
+          <t>16459543</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1694,12 +1694,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>NEWCO SWANSEA SOCIAL INFRASTRUCTURE LP</t>
+          <t>INDEXIE LTD</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>LP024176</t>
+          <t>16459546</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1725,19 +1725,19 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>MEC SURVEYORS LTD</t>
+          <t>UBAH MEDIA LAB LTD</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>16456734</t>
+          <t>16459548</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1770,12 +1770,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>BKK EQUESTRIAN LTD</t>
+          <t>CA ELECTRICAL (YORKSHIRE) LTD</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16456733</t>
+          <t>16459547</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1808,12 +1808,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>WGHR JI LTD</t>
+          <t>LOUD AND CLEAR COACHING LIMITED</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16456731</t>
+          <t>16459549</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1846,12 +1846,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>OPM ILL GO SHOP 4U LTD</t>
+          <t>NORDIC COOPERATION TECHNOLOGIES LIMITED</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16456764</t>
+          <t>16459514</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1884,12 +1884,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>PHONE STUDIO SOUTH LIMITED</t>
+          <t>CLARK AND CO DESIGN LIMITED</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16456765</t>
+          <t>16459516</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1922,12 +1922,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CTLO LTD</t>
+          <t>MILLE TRADING LTD</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16456701</t>
+          <t>16459518</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1960,12 +1960,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>OILMYCAR LTD</t>
+          <t>SPYRO APPAREL LTD</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>16456706</t>
+          <t>16459515</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1998,12 +1998,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>NEHHEALTHCARE LTD</t>
+          <t>THE CHAIR SALON LONDON LTD</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16456708</t>
+          <t>16459512</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2036,12 +2036,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>MAJESTIC EXTERIOR CLEANING SERVICES LTD</t>
+          <t>AMIS &amp; WARD DEVELOPMENT LTD</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16457230</t>
+          <t>16459520</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2074,12 +2074,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>JORDAN CAMPBELL LTD</t>
+          <t>CLICKSPHARE CRAFT LTD</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>NI729519</t>
+          <t>16459521</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2112,12 +2112,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Y-3 APARTMENTS LTD</t>
+          <t>TASHAN MEDIA LTD</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16457262</t>
+          <t>16459523</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2150,12 +2150,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>YSGARLAD PROPERTIES LTD</t>
+          <t>S&amp;S ISTITHMĀR LTD</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16457268</t>
+          <t>16459522</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2188,12 +2188,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>METAHAVEN LTD</t>
+          <t>WANNABEE LTD</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16457273</t>
+          <t>16459526</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2226,12 +2226,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>GLIMORA GLOBAL LTD</t>
+          <t>FINTIVITY LTD</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>16457265</t>
+          <t>16459072</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2264,12 +2264,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>POWERS ELECTRICAL LTD</t>
+          <t>FASHLER LTD</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>16457270</t>
+          <t>16459082</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2302,12 +2302,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>PHOENIX CONSULTING INTERNATIONAL LIMITED</t>
+          <t>CTPROPS LIMITED</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16457267</t>
+          <t>16459084</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2340,12 +2340,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>FARRINGDON HOUSE FINANCIAL SERVICES LIMITED</t>
+          <t>NEW MOUNT DAISY LIMITED</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>16457279</t>
+          <t>16457237</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2416,12 +2416,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>NEW MOUNT DAISY LIMITED</t>
+          <t>FARRINGDON HOUSE FINANCIAL SERVICES LIMITED</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16457237</t>
+          <t>16457279</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2454,12 +2454,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>GODMADE LTD</t>
+          <t>ATSP FIN LTD</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>16459074</t>
+          <t>16456749</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2492,12 +2492,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>HOLYWELL HOMES LTD</t>
+          <t>BREEZY HOMES LIMITED</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>16457259</t>
+          <t>16456709</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2530,12 +2530,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>AUSTIN RICE LTD</t>
+          <t>LEOFRIC LTD</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>NI729522</t>
+          <t>16456712</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2568,12 +2568,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>OMR ELECTRICAL LTD</t>
+          <t>CHIMNEY CHAPS LTD</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>16457261</t>
+          <t>16456261</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2606,12 +2606,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>GUIDED BRAKE SERVICE LTD</t>
+          <t>STOA PROJECTS LTD</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>16457264</t>
+          <t>16456212</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2644,12 +2644,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>BUILTBRITE LTD</t>
+          <t>STEFANPERSAUDLEGACYPROJECT LIMITED</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>16457962</t>
+          <t>16456208</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2682,12 +2682,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>LGAM PROPERTIES LTD</t>
+          <t>IDCHEM CONSULTING LIMITED</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16457957</t>
+          <t>16456205</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2720,12 +2720,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>DEVIPROX LTD</t>
+          <t>WINDOW CLEANING SOUTHEND LTD</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16457970</t>
+          <t>16456227</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2758,12 +2758,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>LEADANICS LIMITED</t>
+          <t>JAI-HO STAFFING LTD</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>16457965</t>
+          <t>16456221</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2796,12 +2796,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>INSPOCL LTD</t>
+          <t>HOUSE OF RODEOS LTD</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16457967</t>
+          <t>16456218</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2834,12 +2834,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>HARRY'S OFFLICENCE &amp; TAKEAWAY LTD</t>
+          <t>CALIBRE LDN LIMITED</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>16456203</t>
+          <t>16457945</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2872,12 +2872,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>PROOFENANCE LTD</t>
+          <t>JANITZA UK LIMITED</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>16457943</t>
+          <t>16456233</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2910,12 +2910,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>ROCK&amp;WALLS LTD</t>
+          <t>HAUS OF PALETTE LTD</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>16457974</t>
+          <t>16456236</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2948,12 +2948,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>CAMBRIDGE VETS LTD</t>
+          <t>JC DEEP TECH LTD</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>16457975</t>
+          <t>16456256</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2986,12 +2986,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>PANEER CRAFT LTD. LIMITED</t>
+          <t>SWIFT BUSINESS GROWTH.AI LTD</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>16457973</t>
+          <t>16456250</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3024,12 +3024,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>MAPLE (510) LIMITED</t>
+          <t>EVO AVIATION LIMITED</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>16457954</t>
+          <t>16456253</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3062,12 +3062,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>GK ZYGALA LIMITED</t>
+          <t>MARKETING DG LTD</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>16457953</t>
+          <t>16456254</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3100,12 +3100,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>DRIVERIGHT REPAIRS LTD</t>
+          <t>KINARA PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>16459058</t>
+          <t>16456244</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3138,12 +3138,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>PARKSIDE GETAWAYS LIMITED</t>
+          <t>UKG BB HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16459059</t>
+          <t>16456246</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3176,12 +3176,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>M S GROUP FIRST UK LIMITED</t>
+          <t>SOCIAL SLOT LTD</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16459057</t>
+          <t>16456245</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3214,12 +3214,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>CAZAM PROPERTY LTD</t>
+          <t>B HOLLAND &amp; SONS (HOLDINGS) LTD</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>16459061</t>
+          <t>16456243</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3252,12 +3252,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>SHOTTON CURRY HOUSE LIMITED</t>
+          <t>J&amp;S DISTRIBUTIONS LIMITED</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16459062</t>
+          <t>16456242</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3290,12 +3290,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>RELIABLE STAFFING RECRUITS LIMITED</t>
+          <t>ELLISA'S BEAUTY LTD</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>16457238</t>
+          <t>16456750</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3328,12 +3328,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>LATINOS TEESSIDE &amp; HISPANIC SENIORS COMMUNITY LTD</t>
+          <t>KHAZAG FREIGHT SERVICES PVT LTD</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>16459078</t>
+          <t>16456754</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3366,12 +3366,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>MALHAMDALE GLAMPING LIMITED</t>
+          <t>PHOENIX CONSULTING INTERNATIONAL LIMITED</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>16459064</t>
+          <t>16457267</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3404,12 +3404,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>RENTAL DISREPAIR CLAIMS LTD</t>
+          <t>DCR HOLDINGS &amp; INVESTMENTS LTD</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>16459077</t>
+          <t>16457272</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3435,19 +3435,19 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Investments</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>CTPROPS LIMITED</t>
+          <t>POWERS ELECTRICAL LTD</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>16459084</t>
+          <t>16457270</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3480,12 +3480,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>FASHLER LTD</t>
+          <t>GLIMORA GLOBAL LTD</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>16459082</t>
+          <t>16457265</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3518,12 +3518,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>FINTIVITY LTD</t>
+          <t>METAHAVEN LTD</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>16459072</t>
+          <t>16457273</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3556,12 +3556,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>WANNABEE LTD</t>
+          <t>YSGARLAD PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>16459526</t>
+          <t>16457268</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3594,12 +3594,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>S&amp;S ISTITHMĀR LTD</t>
+          <t>Y-3 APARTMENTS LTD</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>16459522</t>
+          <t>16457262</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3632,12 +3632,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>TASHAN MEDIA LTD</t>
+          <t>JORDAN CAMPBELL LTD</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>16459523</t>
+          <t>NI729519</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3670,12 +3670,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>CLICKSPHARE CRAFT LTD</t>
+          <t>MAJESTIC EXTERIOR CLEANING SERVICES LTD</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>16459521</t>
+          <t>16457230</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3708,12 +3708,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>AMIS &amp; WARD DEVELOPMENT LTD</t>
+          <t>NEHHEALTHCARE LTD</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>16459520</t>
+          <t>16456708</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3746,12 +3746,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>THE CHAIR SALON LONDON LTD</t>
+          <t>OILMYCAR LTD</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>16459512</t>
+          <t>16456706</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3784,12 +3784,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>SPYRO APPAREL LTD</t>
+          <t>CTLO LTD</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>16459515</t>
+          <t>16456701</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3822,12 +3822,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>MILLE TRADING LTD</t>
+          <t>PHONE STUDIO SOUTH LIMITED</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16459518</t>
+          <t>16456765</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3860,12 +3860,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>CLARK AND CO DESIGN LIMITED</t>
+          <t>OPM ILL GO SHOP 4U LTD</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>16459516</t>
+          <t>16456764</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3898,12 +3898,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>NORDIC COOPERATION TECHNOLOGIES LIMITED</t>
+          <t>WGHR JI LTD</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>16459514</t>
+          <t>16456731</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3936,12 +3936,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>LOUD AND CLEAR COACHING LIMITED</t>
+          <t>BKK EQUESTRIAN LTD</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>16459549</t>
+          <t>16456733</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3974,12 +3974,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>CA ELECTRICAL (YORKSHIRE) LTD</t>
+          <t>MEC SURVEYORS LTD</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>16459547</t>
+          <t>16456734</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -4012,12 +4012,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>UBAH MEDIA LAB LTD</t>
+          <t>NEWCO SWANSEA SOCIAL INFRASTRUCTURE LP</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>16459548</t>
+          <t>LP024176</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -4043,19 +4043,19 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>INDEXIE LTD</t>
+          <t>APEX PREMIER PROPERTY SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>16459546</t>
+          <t>16456756</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4088,12 +4088,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>OCEANHEART MARINE SERVICE CO., LTD</t>
+          <t>FLIP IT GLOBAL LTD</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>16459543</t>
+          <t>16456758</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -4126,12 +4126,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>J.R'S SOUTHERN TWIST LTD</t>
+          <t>DEHBINI LIMITED</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>16459542</t>
+          <t>16456493</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4164,12 +4164,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>SSFBN LIMITED</t>
+          <t>HONG KONG XUNHUA FREIGHT LIMITED</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>16459541</t>
+          <t>16456735</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -4202,12 +4202,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>INP SERVICES LTD</t>
+          <t>FARYAL ENTERPRISE LIMITED</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>16459069</t>
+          <t>16456748</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">

</xml_diff>

<commit_message>
Auto update: 2025-05-20 03:31:34
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:H132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,17 +478,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NEWMINERALS LTD</t>
+          <t>KILICBABACATERING LTD</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>16455878</t>
+          <t>16460380</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -499,12 +499,12 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -516,17 +516,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PROOFENANCE LTD</t>
+          <t>BANDOS BY ADEBISI LTD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16457943</t>
+          <t>16460361</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -537,12 +537,12 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -554,17 +554,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SHOTTON CURRY HOUSE LIMITED</t>
+          <t>2BCLOTHING LTD</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16459062</t>
+          <t>16460354</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -575,12 +575,12 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -592,17 +592,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CAZAM PROPERTY LTD</t>
+          <t>SKYFREIGHTGLOBAL LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16459061</t>
+          <t>16460366</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -613,12 +613,12 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -630,17 +630,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>M S GROUP FIRST UK LIMITED</t>
+          <t>LITBUILD LTD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16459057</t>
+          <t>16460368</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -651,12 +651,12 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -668,17 +668,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PARKSIDE GETAWAYS LIMITED</t>
+          <t>ACCORD FIRE DOORS LTD</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16459059</t>
+          <t>16460363</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -689,12 +689,12 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -706,17 +706,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DRIVERIGHT REPAIRS LTD</t>
+          <t>LUXCOMMERCE LTD</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16459058</t>
+          <t>16460360</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -727,12 +727,12 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -744,17 +744,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GK ZYGALA LIMITED</t>
+          <t>MAK'S TRADERS LTD</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16457953</t>
+          <t>16460355</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -765,12 +765,12 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -782,17 +782,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MAPLE (510) LIMITED</t>
+          <t>APEX PLUMBING AND HEATING SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16457954</t>
+          <t>16460374</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -803,12 +803,12 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -820,17 +820,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PANEER CRAFT LTD. LIMITED</t>
+          <t>BA CORP SOLUTIONS &amp; EVENTS LTD</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16457973</t>
+          <t>16460375</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -841,12 +841,12 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -858,17 +858,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CAMBRIDGE VETS LTD</t>
+          <t>ETECH VENTURE LIMITED</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16457975</t>
+          <t>16460372</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -879,12 +879,12 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -896,17 +896,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ROCK&amp;WALLS LTD</t>
+          <t>BY FATOU JAI LTD</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16457974</t>
+          <t>16460371</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -917,12 +917,12 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -934,17 +934,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>HARRY'S OFFLICENCE &amp; TAKEAWAY LTD</t>
+          <t>ORIENT CANTEEN LTD</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16456203</t>
+          <t>16460365</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -955,12 +955,12 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -972,17 +972,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>A STAR HEALTH LTD</t>
+          <t>CLEANING MONK LTD</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16456234</t>
+          <t>16460369</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -993,12 +993,12 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1010,17 +1010,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>INSPOCL LTD</t>
+          <t>MASR PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16457967</t>
+          <t>16460367</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1031,12 +1031,12 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1048,17 +1048,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>LEADANICS LIMITED</t>
+          <t>FIND YOUR INDUSTRY LTD</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16457965</t>
+          <t>16460362</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1069,12 +1069,12 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1086,17 +1086,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DEVIPROX LTD</t>
+          <t>OMID'S ENTERPRISE LTD</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16457970</t>
+          <t>16460381</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1107,12 +1107,12 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1124,17 +1124,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>LGAM PROPERTIES LTD</t>
+          <t>CLEARLABS PERFORMANCE LTD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16457957</t>
+          <t>16460364</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1145,12 +1145,12 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1162,17 +1162,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BUILTBRITE LTD</t>
+          <t>NARCISSIST APPAREL LTD</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>16457962</t>
+          <t>16460378</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1183,12 +1183,12 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1200,17 +1200,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GUIDED BRAKE SERVICE LTD</t>
+          <t>DERICA SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16457264</t>
+          <t>16460357</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1221,12 +1221,12 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1238,17 +1238,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>OMR ELECTRICAL LTD</t>
+          <t>MOTIVATION AND PROSPERITY LTD</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16457261</t>
+          <t>16460379</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1259,12 +1259,12 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1276,17 +1276,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>AUSTIN RICE LTD</t>
+          <t>CLARITY VENTURE SUPPORT LTD</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>NI729522</t>
+          <t>16460376</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1297,12 +1297,12 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1314,17 +1314,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>HOLYWELL HOMES LTD</t>
+          <t>MISBAH GOODS LTD</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16457259</t>
+          <t>16460377</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1335,12 +1335,12 @@
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1352,17 +1352,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>GODMADE LTD</t>
+          <t>PAVITA LOGISTICS LTD</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16459074</t>
+          <t>16460373</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1373,12 +1373,12 @@
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1390,17 +1390,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>RELIABLE STAFFING RECRUITS LIMITED</t>
+          <t>ROAMING RETAIL LIMITED</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16457238</t>
+          <t>16460382</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1411,12 +1411,12 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1428,17 +1428,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>LATINOS TEESSIDE &amp; HISPANIC SENIORS COMMUNITY LTD</t>
+          <t>TRUE NORTH JOINERY LTD</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16459078</t>
+          <t>16460359</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1449,12 +1449,12 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1466,17 +1466,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>MALHAMDALE GLAMPING LIMITED</t>
+          <t>VIVID MART LTD</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16459064</t>
+          <t>16460370</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1487,12 +1487,12 @@
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1504,17 +1504,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>RENTAL DISREPAIR CLAIMS LTD</t>
+          <t>MASTER THE CHAIN LTD</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16459077</t>
+          <t>16460358</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1525,12 +1525,12 @@
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1542,17 +1542,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>INP SERVICES LTD</t>
+          <t>FONETHICS SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16459069</t>
+          <t>SC848969</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1563,12 +1563,12 @@
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1580,17 +1580,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SSFBN LIMITED</t>
+          <t>M&amp;S SOCIAL CARE CONSULTANTS LTD</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16459541</t>
+          <t>16460353</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1601,12 +1601,12 @@
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1618,17 +1618,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>J.R'S SOUTHERN TWIST LTD</t>
+          <t>FAMILY COMMREPORT LTD</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16459542</t>
+          <t>16460356</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1639,12 +1639,12 @@
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1656,12 +1656,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>OCEANHEART MARINE SERVICE CO., LTD</t>
+          <t>KHAZAG FREIGHT SERVICES PVT LTD</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16459543</t>
+          <t>16456754</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1694,12 +1694,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>INDEXIE LTD</t>
+          <t>YSGARLAD PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16459546</t>
+          <t>16457268</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1732,12 +1732,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>UBAH MEDIA LAB LTD</t>
+          <t>METAHAVEN LTD</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>16459548</t>
+          <t>16457273</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1770,12 +1770,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CA ELECTRICAL (YORKSHIRE) LTD</t>
+          <t>GLIMORA GLOBAL LTD</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16459547</t>
+          <t>16457265</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1808,12 +1808,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>LOUD AND CLEAR COACHING LIMITED</t>
+          <t>POWERS ELECTRICAL LTD</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16459549</t>
+          <t>16457270</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1846,12 +1846,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>NORDIC COOPERATION TECHNOLOGIES LIMITED</t>
+          <t>DCR HOLDINGS &amp; INVESTMENTS LTD</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16459514</t>
+          <t>16457272</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1877,19 +1877,19 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Investments</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>CLARK AND CO DESIGN LIMITED</t>
+          <t>PHOENIX CONSULTING INTERNATIONAL LIMITED</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16459516</t>
+          <t>16457267</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1922,12 +1922,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>MILLE TRADING LTD</t>
+          <t>MARKETING DG LTD</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16459518</t>
+          <t>16456254</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1960,12 +1960,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>SPYRO APPAREL LTD</t>
+          <t>ELLISA'S BEAUTY LTD</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>16459515</t>
+          <t>16456750</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1998,12 +1998,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>THE CHAIR SALON LONDON LTD</t>
+          <t>J&amp;S DISTRIBUTIONS LIMITED</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16459512</t>
+          <t>16456242</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2036,12 +2036,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>AMIS &amp; WARD DEVELOPMENT LTD</t>
+          <t>B HOLLAND &amp; SONS (HOLDINGS) LTD</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16459520</t>
+          <t>16456243</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2074,12 +2074,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>CLICKSPHARE CRAFT LTD</t>
+          <t>SOCIAL SLOT LTD</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16459521</t>
+          <t>16456245</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2112,12 +2112,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>TASHAN MEDIA LTD</t>
+          <t>UKG BB HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16459523</t>
+          <t>16456246</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2150,12 +2150,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>S&amp;S ISTITHMĀR LTD</t>
+          <t>KINARA PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16459522</t>
+          <t>16456244</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2188,12 +2188,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>WANNABEE LTD</t>
+          <t>JORDAN CAMPBELL LTD</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16459526</t>
+          <t>NI729519</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2226,12 +2226,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>FINTIVITY LTD</t>
+          <t>Y-3 APARTMENTS LTD</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>16459072</t>
+          <t>16457262</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2264,12 +2264,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>FASHLER LTD</t>
+          <t>AMIKOBA LTD</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>16459082</t>
+          <t>16459545</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2302,12 +2302,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>CTPROPS LIMITED</t>
+          <t>MAJESTIC EXTERIOR CLEANING SERVICES LTD</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16459084</t>
+          <t>16457230</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2340,12 +2340,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>NEW MOUNT DAISY LIMITED</t>
+          <t>NEWCO SWANSEA SOCIAL INFRASTRUCTURE LP</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>16457237</t>
+          <t>LP024176</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2371,19 +2371,19 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>FITCARDIOLOGY LTD</t>
+          <t>SWIFT BUSINESS GROWTH.AI LTD</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>16457244</t>
+          <t>16456250</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2416,12 +2416,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>FARRINGDON HOUSE FINANCIAL SERVICES LIMITED</t>
+          <t>FARYAL ENTERPRISE LIMITED</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16457279</t>
+          <t>16456748</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2454,12 +2454,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>ATSP FIN LTD</t>
+          <t>HONG KONG XUNHUA FREIGHT LIMITED</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>16456749</t>
+          <t>16456735</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2492,12 +2492,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>BREEZY HOMES LIMITED</t>
+          <t>DEHBINI LIMITED</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>16456709</t>
+          <t>16456493</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2530,12 +2530,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>LEOFRIC LTD</t>
+          <t>FLIP IT GLOBAL LTD</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>16456712</t>
+          <t>16456758</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2568,12 +2568,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>CHIMNEY CHAPS LTD</t>
+          <t>APEX PREMIER PROPERTY SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>16456261</t>
+          <t>16456756</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2606,12 +2606,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>STOA PROJECTS LTD</t>
+          <t>MEC SURVEYORS LTD</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>16456212</t>
+          <t>16456734</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2644,12 +2644,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>STEFANPERSAUDLEGACYPROJECT LIMITED</t>
+          <t>NEHHEALTHCARE LTD</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>16456208</t>
+          <t>16456708</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2682,12 +2682,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>IDCHEM CONSULTING LIMITED</t>
+          <t>BKK EQUESTRIAN LTD</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16456205</t>
+          <t>16456733</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2720,12 +2720,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>WINDOW CLEANING SOUTHEND LTD</t>
+          <t>WGHR JI LTD</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16456227</t>
+          <t>16456731</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2758,12 +2758,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>JAI-HO STAFFING LTD</t>
+          <t>OPM ILL GO SHOP 4U LTD</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>16456221</t>
+          <t>16456764</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2796,12 +2796,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>HOUSE OF RODEOS LTD</t>
+          <t>PHONE STUDIO SOUTH LIMITED</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16456218</t>
+          <t>16456765</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2834,12 +2834,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>CALIBRE LDN LIMITED</t>
+          <t>CTLO LTD</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>16457945</t>
+          <t>16456701</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2872,12 +2872,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>JANITZA UK LIMITED</t>
+          <t>OILMYCAR LTD</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>16456233</t>
+          <t>16456706</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2910,12 +2910,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>HAUS OF PALETTE LTD</t>
+          <t>EVO AVIATION LIMITED</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>16456236</t>
+          <t>16456253</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2948,12 +2948,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>JC DEEP TECH LTD</t>
+          <t>NEWMINERALS LTD</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>16456256</t>
+          <t>16455878</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2986,12 +2986,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>SWIFT BUSINESS GROWTH.AI LTD</t>
+          <t>PROOFENANCE LTD</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>16456250</t>
+          <t>16457943</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3024,12 +3024,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>EVO AVIATION LIMITED</t>
+          <t>INDEXIE LTD</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>16456253</t>
+          <t>16459546</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3062,12 +3062,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>MARKETING DG LTD</t>
+          <t>J.R'S SOUTHERN TWIST LTD</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>16456254</t>
+          <t>16459542</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3100,12 +3100,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>KINARA PROPERTIES LTD</t>
+          <t>SSFBN LIMITED</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>16456244</t>
+          <t>16459541</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3138,12 +3138,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>UKG BB HOLDINGS LTD</t>
+          <t>INP SERVICES LTD</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16456246</t>
+          <t>16459069</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3176,12 +3176,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>SOCIAL SLOT LTD</t>
+          <t>RENTAL DISREPAIR CLAIMS LTD</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16456245</t>
+          <t>16459077</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3214,12 +3214,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>B HOLLAND &amp; SONS (HOLDINGS) LTD</t>
+          <t>MALHAMDALE GLAMPING LIMITED</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>16456243</t>
+          <t>16459064</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3252,12 +3252,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>J&amp;S DISTRIBUTIONS LIMITED</t>
+          <t>LATINOS TEESSIDE &amp; HISPANIC SENIORS COMMUNITY LTD</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16456242</t>
+          <t>16459078</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3290,12 +3290,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>ELLISA'S BEAUTY LTD</t>
+          <t>RELIABLE STAFFING RECRUITS LIMITED</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>16456750</t>
+          <t>16457238</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3328,12 +3328,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>KHAZAG FREIGHT SERVICES PVT LTD</t>
+          <t>GODMADE LTD</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>16456754</t>
+          <t>16459074</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3366,12 +3366,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>PHOENIX CONSULTING INTERNATIONAL LIMITED</t>
+          <t>HOLYWELL HOMES LTD</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>16457267</t>
+          <t>16457259</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3404,12 +3404,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>DCR HOLDINGS &amp; INVESTMENTS LTD</t>
+          <t>AUSTIN RICE LTD</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>16457272</t>
+          <t>NI729522</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3435,19 +3435,19 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>POWERS ELECTRICAL LTD</t>
+          <t>OMR ELECTRICAL LTD</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>16457270</t>
+          <t>16457261</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3480,12 +3480,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>GLIMORA GLOBAL LTD</t>
+          <t>GUIDED BRAKE SERVICE LTD</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>16457265</t>
+          <t>16457264</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3518,12 +3518,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>METAHAVEN LTD</t>
+          <t>BUILTBRITE LTD</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>16457273</t>
+          <t>16457962</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3556,12 +3556,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>YSGARLAD PROPERTIES LTD</t>
+          <t>LGAM PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>16457268</t>
+          <t>16457957</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3594,12 +3594,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Y-3 APARTMENTS LTD</t>
+          <t>DEVIPROX LTD</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>16457262</t>
+          <t>16457970</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3632,12 +3632,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>JORDAN CAMPBELL LTD</t>
+          <t>LEADANICS LIMITED</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>NI729519</t>
+          <t>16457965</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3670,12 +3670,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>MAJESTIC EXTERIOR CLEANING SERVICES LTD</t>
+          <t>INSPOCL LTD</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>16457230</t>
+          <t>16457967</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3708,12 +3708,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>NEHHEALTHCARE LTD</t>
+          <t>A STAR HEALTH LTD</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>16456708</t>
+          <t>16456234</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3746,12 +3746,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>OILMYCAR LTD</t>
+          <t>HARRY'S OFFLICENCE &amp; TAKEAWAY LTD</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>16456706</t>
+          <t>16456203</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3784,12 +3784,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>CTLO LTD</t>
+          <t>ROCK&amp;WALLS LTD</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>16456701</t>
+          <t>16457974</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3822,12 +3822,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>PHONE STUDIO SOUTH LIMITED</t>
+          <t>CAMBRIDGE VETS LTD</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16456765</t>
+          <t>16457975</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3860,12 +3860,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>OPM ILL GO SHOP 4U LTD</t>
+          <t>PANEER CRAFT LTD. LIMITED</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>16456764</t>
+          <t>16457973</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3898,12 +3898,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>WGHR JI LTD</t>
+          <t>MAPLE (510) LIMITED</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>16456731</t>
+          <t>16457954</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3936,12 +3936,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>BKK EQUESTRIAN LTD</t>
+          <t>GK ZYGALA LIMITED</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>16456733</t>
+          <t>16457953</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3974,12 +3974,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>MEC SURVEYORS LTD</t>
+          <t>DRIVERIGHT REPAIRS LTD</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>16456734</t>
+          <t>16459058</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -4012,12 +4012,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>NEWCO SWANSEA SOCIAL INFRASTRUCTURE LP</t>
+          <t>PARKSIDE GETAWAYS LIMITED</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>LP024176</t>
+          <t>16459059</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -4043,19 +4043,19 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>APEX PREMIER PROPERTY SOLUTIONS LTD</t>
+          <t>M S GROUP FIRST UK LIMITED</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>16456756</t>
+          <t>16459057</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4088,12 +4088,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>FLIP IT GLOBAL LTD</t>
+          <t>CAZAM PROPERTY LTD</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>16456758</t>
+          <t>16459061</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -4126,12 +4126,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>DEHBINI LIMITED</t>
+          <t>SHOTTON CURRY HOUSE LIMITED</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>16456493</t>
+          <t>16459062</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4164,12 +4164,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>HONG KONG XUNHUA FREIGHT LIMITED</t>
+          <t>OCEANHEART MARINE SERVICE CO., LTD</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>16456735</t>
+          <t>16459543</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -4202,12 +4202,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>FARYAL ENTERPRISE LIMITED</t>
+          <t>UBAH MEDIA LAB LTD</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>16456748</t>
+          <t>16459548</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -4240,12 +4240,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>AMIKOBA LTD</t>
+          <t>HAUS OF PALETTE LTD</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>16459545</t>
+          <t>16456236</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -4270,6 +4270,1184 @@
         </is>
       </c>
       <c r="H101" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>CA ELECTRICAL (YORKSHIRE) LTD</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>16459547</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr"/>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>JANITZA UK LIMITED</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>16456233</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr"/>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>CALIBRE LDN LIMITED</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>16457945</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr"/>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>HOUSE OF RODEOS LTD</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>16456218</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr"/>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>JAI-HO STAFFING LTD</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>16456221</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr"/>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>WINDOW CLEANING SOUTHEND LTD</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>16456227</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>IDCHEM CONSULTING LIMITED</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>16456205</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr"/>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>STEFANPERSAUDLEGACYPROJECT LIMITED</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>16456208</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr"/>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>STOA PROJECTS LTD</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>16456212</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr"/>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>CHIMNEY CHAPS LTD</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>16456261</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr"/>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>LEOFRIC LTD</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>16456712</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr"/>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>BREEZY HOMES LIMITED</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>16456709</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr"/>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>ATSP FIN LTD</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>16456749</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr"/>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>FARRINGDON HOUSE FINANCIAL SERVICES LIMITED</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>16457279</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr"/>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>FITCARDIOLOGY LTD</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>16457244</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr"/>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>NEW MOUNT DAISY LIMITED</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>16457237</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr"/>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>CTPROPS LIMITED</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>16459084</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr"/>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>FASHLER LTD</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>16459082</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr"/>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>FINTIVITY LTD</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>16459072</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr"/>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>WANNABEE LTD</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>16459526</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr"/>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>S&amp;S ISTITHMĀR LTD</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>16459522</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr"/>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>TASHAN MEDIA LTD</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>16459523</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr"/>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>CLICKSPHARE CRAFT LTD</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>16459521</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr"/>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>AMIS &amp; WARD DEVELOPMENT LTD</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>16459520</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr"/>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>THE CHAIR SALON LONDON LTD</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>16459512</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr"/>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>SPYRO APPAREL LTD</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>16459515</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr"/>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>MILLE TRADING LTD</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>16459518</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr"/>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>CLARK AND CO DESIGN LIMITED</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>16459516</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr"/>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>NORDIC COOPERATION TECHNOLOGIES LIMITED</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>16459514</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr"/>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>LOUD AND CLEAR COACHING LIMITED</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>16459549</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr"/>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>JC DEEP TECH LTD</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>16456256</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr"/>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
         <is>
           <t>Other</t>
         </is>

</xml_diff>

<commit_message>
Auto update: 2025-05-20 04:43:32
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H132"/>
+  <dimension ref="A1:H137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,12 +516,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BANDOS BY ADEBISI LTD</t>
+          <t>DERICA SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16460361</t>
+          <t>16460357</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -554,12 +554,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2BCLOTHING LTD</t>
+          <t>CLARITY VENTURE SUPPORT LTD</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16460354</t>
+          <t>16460376</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -592,12 +592,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SKYFREIGHTGLOBAL LTD</t>
+          <t>MISBAH GOODS LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16460366</t>
+          <t>16460377</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -630,12 +630,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>LITBUILD LTD</t>
+          <t>PAVITA LOGISTICS LTD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16460368</t>
+          <t>16460373</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -668,12 +668,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ACCORD FIRE DOORS LTD</t>
+          <t>ROAMING RETAIL LIMITED</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16460363</t>
+          <t>16460382</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -706,12 +706,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LUXCOMMERCE LTD</t>
+          <t>TRUE NORTH JOINERY LTD</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16460360</t>
+          <t>16460359</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -744,12 +744,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MAK'S TRADERS LTD</t>
+          <t>VIVID MART LTD</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16460355</t>
+          <t>16460370</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -782,12 +782,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>APEX PLUMBING AND HEATING SOLUTIONS LTD</t>
+          <t>MASTER THE CHAIN LTD</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16460374</t>
+          <t>16460358</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -820,12 +820,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BA CORP SOLUTIONS &amp; EVENTS LTD</t>
+          <t>FONETHICS SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16460375</t>
+          <t>SC848969</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -858,12 +858,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ETECH VENTURE LIMITED</t>
+          <t>M&amp;S SOCIAL CARE CONSULTANTS LTD</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16460372</t>
+          <t>16460353</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -896,12 +896,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BY FATOU JAI LTD</t>
+          <t>FAMILY COMMREPORT LTD</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16460371</t>
+          <t>16460356</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -934,12 +934,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ORIENT CANTEEN LTD</t>
+          <t>BANDOS BY ADEBISI LTD</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16460365</t>
+          <t>16460361</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -972,12 +972,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CLEANING MONK LTD</t>
+          <t>VITANOVA LEARNING LIMITED</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16460369</t>
+          <t>16460384</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -998,7 +998,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>04:43:32</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1010,12 +1010,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MASR PROPERTIES LTD</t>
+          <t>MEARNS CLEANING SERVICES LTD</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16460367</t>
+          <t>16460387</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>04:43:32</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1048,12 +1048,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>FIND YOUR INDUSTRY LTD</t>
+          <t>MONEY MART LTD</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16460362</t>
+          <t>16460383</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1074,7 +1074,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>04:43:32</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1086,12 +1086,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>OMID'S ENTERPRISE LTD</t>
+          <t>AA SELLER HUB LTD</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16460381</t>
+          <t>16460385</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>04:43:32</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1124,12 +1124,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CLEARLABS PERFORMANCE LTD</t>
+          <t>MOTIVATION AND PROSPERITY LTD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16460364</t>
+          <t>16460379</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1162,12 +1162,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>NARCISSIST APPAREL LTD</t>
+          <t>GMS7 LIMITED</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>16460378</t>
+          <t>16460386</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1188,7 +1188,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>04:43:32</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1200,12 +1200,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>DERICA SOLUTIONS LTD</t>
+          <t>NARCISSIST APPAREL LTD</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16460357</t>
+          <t>16460378</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1238,12 +1238,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>MOTIVATION AND PROSPERITY LTD</t>
+          <t>BA CORP SOLUTIONS &amp; EVENTS LTD</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16460379</t>
+          <t>16460375</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1276,12 +1276,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CLARITY VENTURE SUPPORT LTD</t>
+          <t>LUXCOMMERCE LTD</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>16460376</t>
+          <t>16460360</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1314,12 +1314,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>MISBAH GOODS LTD</t>
+          <t>CLEARLABS PERFORMANCE LTD</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16460377</t>
+          <t>16460364</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1352,12 +1352,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>PAVITA LOGISTICS LTD</t>
+          <t>ACCORD FIRE DOORS LTD</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16460373</t>
+          <t>16460363</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1390,12 +1390,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ROAMING RETAIL LIMITED</t>
+          <t>LITBUILD LTD</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16460382</t>
+          <t>16460368</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1428,12 +1428,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>TRUE NORTH JOINERY LTD</t>
+          <t>2BCLOTHING LTD</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16460359</t>
+          <t>16460354</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1466,12 +1466,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>VIVID MART LTD</t>
+          <t>MAK'S TRADERS LTD</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16460370</t>
+          <t>16460355</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1504,12 +1504,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>MASTER THE CHAIN LTD</t>
+          <t>APEX PLUMBING AND HEATING SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16460358</t>
+          <t>16460374</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1542,12 +1542,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>FONETHICS SOLUTIONS LTD</t>
+          <t>SKYFREIGHTGLOBAL LTD</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>SC848969</t>
+          <t>16460366</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1580,12 +1580,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>M&amp;S SOCIAL CARE CONSULTANTS LTD</t>
+          <t>ETECH VENTURE LIMITED</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16460353</t>
+          <t>16460372</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1618,12 +1618,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>FAMILY COMMREPORT LTD</t>
+          <t>ORIENT CANTEEN LTD</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16460356</t>
+          <t>16460365</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1656,17 +1656,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>KHAZAG FREIGHT SERVICES PVT LTD</t>
+          <t>OMID'S ENTERPRISE LTD</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16456754</t>
+          <t>16460381</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1677,12 +1677,12 @@
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1694,17 +1694,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>YSGARLAD PROPERTIES LTD</t>
+          <t>CLEANING MONK LTD</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16457268</t>
+          <t>16460369</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1715,12 +1715,12 @@
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -1732,17 +1732,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>METAHAVEN LTD</t>
+          <t>MASR PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>16457273</t>
+          <t>16460367</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1753,12 +1753,12 @@
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1770,17 +1770,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>GLIMORA GLOBAL LTD</t>
+          <t>BY FATOU JAI LTD</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16457265</t>
+          <t>16460371</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1791,12 +1791,12 @@
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -1808,17 +1808,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>POWERS ELECTRICAL LTD</t>
+          <t>FIND YOUR INDUSTRY LTD</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16457270</t>
+          <t>16460362</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1829,12 +1829,12 @@
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1846,12 +1846,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>DCR HOLDINGS &amp; INVESTMENTS LTD</t>
+          <t>JANITZA UK LIMITED</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16457272</t>
+          <t>16456233</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1877,19 +1877,19 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>PHOENIX CONSULTING INTERNATIONAL LIMITED</t>
+          <t>UBAH MEDIA LAB LTD</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16457267</t>
+          <t>16459548</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1922,12 +1922,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>MARKETING DG LTD</t>
+          <t>HAUS OF PALETTE LTD</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16456254</t>
+          <t>16456236</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1960,12 +1960,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>ELLISA'S BEAUTY LTD</t>
+          <t>CA ELECTRICAL (YORKSHIRE) LTD</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>16456750</t>
+          <t>16459547</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1998,12 +1998,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>J&amp;S DISTRIBUTIONS LIMITED</t>
+          <t>HOUSE OF RODEOS LTD</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16456242</t>
+          <t>16456218</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2036,12 +2036,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>B HOLLAND &amp; SONS (HOLDINGS) LTD</t>
+          <t>CALIBRE LDN LIMITED</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16456243</t>
+          <t>16457945</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2074,12 +2074,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>SOCIAL SLOT LTD</t>
+          <t>JAI-HO STAFFING LTD</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16456245</t>
+          <t>16456221</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2112,12 +2112,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>UKG BB HOLDINGS LTD</t>
+          <t>WINDOW CLEANING SOUTHEND LTD</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16456246</t>
+          <t>16456227</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2150,12 +2150,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>KINARA PROPERTIES LTD</t>
+          <t>SHOTTON CURRY HOUSE LIMITED</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16456244</t>
+          <t>16459062</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2188,12 +2188,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>JORDAN CAMPBELL LTD</t>
+          <t>OCEANHEART MARINE SERVICE CO., LTD</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>NI729519</t>
+          <t>16459543</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2226,12 +2226,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Y-3 APARTMENTS LTD</t>
+          <t>PANEER CRAFT LTD. LIMITED</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>16457262</t>
+          <t>16457973</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2264,12 +2264,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>AMIKOBA LTD</t>
+          <t>CAZAM PROPERTY LTD</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>16459545</t>
+          <t>16459061</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2302,12 +2302,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>MAJESTIC EXTERIOR CLEANING SERVICES LTD</t>
+          <t>M S GROUP FIRST UK LIMITED</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16457230</t>
+          <t>16459057</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2340,12 +2340,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>NEWCO SWANSEA SOCIAL INFRASTRUCTURE LP</t>
+          <t>PARKSIDE GETAWAYS LIMITED</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>LP024176</t>
+          <t>16459059</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2371,19 +2371,19 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>SWIFT BUSINESS GROWTH.AI LTD</t>
+          <t>DRIVERIGHT REPAIRS LTD</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>16456250</t>
+          <t>16459058</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2416,12 +2416,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>FARYAL ENTERPRISE LIMITED</t>
+          <t>GK ZYGALA LIMITED</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16456748</t>
+          <t>16457953</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2454,12 +2454,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>HONG KONG XUNHUA FREIGHT LIMITED</t>
+          <t>MAPLE (510) LIMITED</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>16456735</t>
+          <t>16457954</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2492,12 +2492,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>DEHBINI LIMITED</t>
+          <t>STEFANPERSAUDLEGACYPROJECT LIMITED</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>16456493</t>
+          <t>16456208</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2530,12 +2530,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>FLIP IT GLOBAL LTD</t>
+          <t>CAMBRIDGE VETS LTD</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>16456758</t>
+          <t>16457975</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2568,12 +2568,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>APEX PREMIER PROPERTY SOLUTIONS LTD</t>
+          <t>ROCK&amp;WALLS LTD</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>16456756</t>
+          <t>16457974</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2606,12 +2606,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>MEC SURVEYORS LTD</t>
+          <t>HARRY'S OFFLICENCE &amp; TAKEAWAY LTD</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>16456734</t>
+          <t>16456203</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2644,12 +2644,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>NEHHEALTHCARE LTD</t>
+          <t>IDCHEM CONSULTING LIMITED</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>16456708</t>
+          <t>16456205</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2682,12 +2682,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>BKK EQUESTRIAN LTD</t>
+          <t>FITCARDIOLOGY LTD</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16456733</t>
+          <t>16457244</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2720,12 +2720,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>WGHR JI LTD</t>
+          <t>STOA PROJECTS LTD</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16456731</t>
+          <t>16456212</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2758,12 +2758,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>OPM ILL GO SHOP 4U LTD</t>
+          <t>CHIMNEY CHAPS LTD</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>16456764</t>
+          <t>16456261</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2796,12 +2796,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>PHONE STUDIO SOUTH LIMITED</t>
+          <t>JC DEEP TECH LTD</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16456765</t>
+          <t>16456256</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2834,12 +2834,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>CTLO LTD</t>
+          <t>LOUD AND CLEAR COACHING LIMITED</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>16456701</t>
+          <t>16459549</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2872,12 +2872,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>OILMYCAR LTD</t>
+          <t>NORDIC COOPERATION TECHNOLOGIES LIMITED</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>16456706</t>
+          <t>16459514</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2910,12 +2910,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>EVO AVIATION LIMITED</t>
+          <t>CLARK AND CO DESIGN LIMITED</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>16456253</t>
+          <t>16459516</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2948,12 +2948,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>NEWMINERALS LTD</t>
+          <t>MILLE TRADING LTD</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>16455878</t>
+          <t>16459518</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2986,12 +2986,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>PROOFENANCE LTD</t>
+          <t>SPYRO APPAREL LTD</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>16457943</t>
+          <t>16459515</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3024,12 +3024,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>INDEXIE LTD</t>
+          <t>THE CHAIR SALON LONDON LTD</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>16459546</t>
+          <t>16459512</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3062,12 +3062,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>J.R'S SOUTHERN TWIST LTD</t>
+          <t>AMIS &amp; WARD DEVELOPMENT LTD</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>16459542</t>
+          <t>16459520</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3100,12 +3100,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>SSFBN LIMITED</t>
+          <t>CLICKSPHARE CRAFT LTD</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>16459541</t>
+          <t>16459521</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3138,12 +3138,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>INP SERVICES LTD</t>
+          <t>TASHAN MEDIA LTD</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16459069</t>
+          <t>16459523</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3176,12 +3176,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>RENTAL DISREPAIR CLAIMS LTD</t>
+          <t>S&amp;S ISTITHMĀR LTD</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16459077</t>
+          <t>16459522</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3214,12 +3214,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>MALHAMDALE GLAMPING LIMITED</t>
+          <t>WANNABEE LTD</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>16459064</t>
+          <t>16459526</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3252,12 +3252,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>LATINOS TEESSIDE &amp; HISPANIC SENIORS COMMUNITY LTD</t>
+          <t>FINTIVITY LTD</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16459078</t>
+          <t>16459072</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3290,12 +3290,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>RELIABLE STAFFING RECRUITS LIMITED</t>
+          <t>FASHLER LTD</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>16457238</t>
+          <t>16459082</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3328,12 +3328,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>GODMADE LTD</t>
+          <t>CTPROPS LIMITED</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>16459074</t>
+          <t>16459084</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3366,12 +3366,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>HOLYWELL HOMES LTD</t>
+          <t>NEW MOUNT DAISY LIMITED</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>16457259</t>
+          <t>16457237</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3404,12 +3404,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>AUSTIN RICE LTD</t>
+          <t>INSPOCL LTD</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>NI729522</t>
+          <t>16457967</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3442,12 +3442,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>OMR ELECTRICAL LTD</t>
+          <t>FARRINGDON HOUSE FINANCIAL SERVICES LIMITED</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>16457261</t>
+          <t>16457279</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3480,12 +3480,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>GUIDED BRAKE SERVICE LTD</t>
+          <t>ATSP FIN LTD</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>16457264</t>
+          <t>16456749</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3518,12 +3518,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>BUILTBRITE LTD</t>
+          <t>BREEZY HOMES LIMITED</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>16457962</t>
+          <t>16456709</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3556,12 +3556,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>LGAM PROPERTIES LTD</t>
+          <t>LEOFRIC LTD</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>16457957</t>
+          <t>16456712</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3594,12 +3594,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>DEVIPROX LTD</t>
+          <t>A STAR HEALTH LTD</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>16457970</t>
+          <t>16456234</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3632,12 +3632,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>LEADANICS LIMITED</t>
+          <t>AUSTIN RICE LTD</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>16457965</t>
+          <t>NI729522</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3670,12 +3670,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>INSPOCL LTD</t>
+          <t>LEADANICS LIMITED</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>16457967</t>
+          <t>16457965</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3708,12 +3708,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>A STAR HEALTH LTD</t>
+          <t>DEVIPROX LTD</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>16456234</t>
+          <t>16457970</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3746,12 +3746,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>HARRY'S OFFLICENCE &amp; TAKEAWAY LTD</t>
+          <t>DEHBINI LIMITED</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>16456203</t>
+          <t>16456493</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3784,12 +3784,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>ROCK&amp;WALLS LTD</t>
+          <t>HONG KONG XUNHUA FREIGHT LIMITED</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>16457974</t>
+          <t>16456735</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3822,12 +3822,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>CAMBRIDGE VETS LTD</t>
+          <t>FARYAL ENTERPRISE LIMITED</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16457975</t>
+          <t>16456748</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3860,12 +3860,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>PANEER CRAFT LTD. LIMITED</t>
+          <t>SWIFT BUSINESS GROWTH.AI LTD</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>16457973</t>
+          <t>16456250</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3898,12 +3898,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>MAPLE (510) LIMITED</t>
+          <t>NEWCO SWANSEA SOCIAL INFRASTRUCTURE LP</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>16457954</t>
+          <t>LP024176</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3929,19 +3929,19 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>GK ZYGALA LIMITED</t>
+          <t>MAJESTIC EXTERIOR CLEANING SERVICES LTD</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>16457953</t>
+          <t>16457230</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3974,12 +3974,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>DRIVERIGHT REPAIRS LTD</t>
+          <t>AMIKOBA LTD</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>16459058</t>
+          <t>16459545</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -4012,12 +4012,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>PARKSIDE GETAWAYS LIMITED</t>
+          <t>Y-3 APARTMENTS LTD</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>16459059</t>
+          <t>16457262</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -4050,12 +4050,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>M S GROUP FIRST UK LIMITED</t>
+          <t>JORDAN CAMPBELL LTD</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>16459057</t>
+          <t>NI729519</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4088,12 +4088,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>CAZAM PROPERTY LTD</t>
+          <t>KINARA PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>16459061</t>
+          <t>16456244</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -4126,12 +4126,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>SHOTTON CURRY HOUSE LIMITED</t>
+          <t>UKG BB HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>16459062</t>
+          <t>16456246</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4164,12 +4164,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>OCEANHEART MARINE SERVICE CO., LTD</t>
+          <t>SOCIAL SLOT LTD</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>16459543</t>
+          <t>16456245</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -4202,12 +4202,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>UBAH MEDIA LAB LTD</t>
+          <t>B HOLLAND &amp; SONS (HOLDINGS) LTD</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>16459548</t>
+          <t>16456243</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -4240,12 +4240,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>HAUS OF PALETTE LTD</t>
+          <t>J&amp;S DISTRIBUTIONS LIMITED</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>16456236</t>
+          <t>16456242</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -4278,12 +4278,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>CA ELECTRICAL (YORKSHIRE) LTD</t>
+          <t>ELLISA'S BEAUTY LTD</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>16459547</t>
+          <t>16456750</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -4316,12 +4316,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>JANITZA UK LIMITED</t>
+          <t>MARKETING DG LTD</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>16456233</t>
+          <t>16456254</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -4354,12 +4354,12 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>CALIBRE LDN LIMITED</t>
+          <t>PHOENIX CONSULTING INTERNATIONAL LIMITED</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>16457945</t>
+          <t>16457267</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -4392,12 +4392,12 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>HOUSE OF RODEOS LTD</t>
+          <t>DCR HOLDINGS &amp; INVESTMENTS LTD</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>16456218</t>
+          <t>16457272</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -4423,19 +4423,19 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Investments</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>JAI-HO STAFFING LTD</t>
+          <t>POWERS ELECTRICAL LTD</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>16456221</t>
+          <t>16457270</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -4468,12 +4468,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>WINDOW CLEANING SOUTHEND LTD</t>
+          <t>GLIMORA GLOBAL LTD</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>16456227</t>
+          <t>16457265</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -4506,12 +4506,12 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>IDCHEM CONSULTING LIMITED</t>
+          <t>METAHAVEN LTD</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>16456205</t>
+          <t>16457273</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -4544,12 +4544,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>STEFANPERSAUDLEGACYPROJECT LIMITED</t>
+          <t>YSGARLAD PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>16456208</t>
+          <t>16457268</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -4582,12 +4582,12 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>STOA PROJECTS LTD</t>
+          <t>KHAZAG FREIGHT SERVICES PVT LTD</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>16456212</t>
+          <t>16456754</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -4620,12 +4620,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>CHIMNEY CHAPS LTD</t>
+          <t>FLIP IT GLOBAL LTD</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>16456261</t>
+          <t>16456758</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -4658,12 +4658,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>LEOFRIC LTD</t>
+          <t>APEX PREMIER PROPERTY SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>16456712</t>
+          <t>16456756</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -4696,12 +4696,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>BREEZY HOMES LIMITED</t>
+          <t>MEC SURVEYORS LTD</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>16456709</t>
+          <t>16456734</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -4734,12 +4734,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>ATSP FIN LTD</t>
+          <t>INP SERVICES LTD</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>16456749</t>
+          <t>16459069</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -4772,12 +4772,12 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>FARRINGDON HOUSE FINANCIAL SERVICES LIMITED</t>
+          <t>LGAM PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>16457279</t>
+          <t>16457957</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -4810,12 +4810,12 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>FITCARDIOLOGY LTD</t>
+          <t>BUILTBRITE LTD</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>16457244</t>
+          <t>16457962</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -4848,12 +4848,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>NEW MOUNT DAISY LIMITED</t>
+          <t>GUIDED BRAKE SERVICE LTD</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>16457237</t>
+          <t>16457264</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -4886,12 +4886,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>CTPROPS LIMITED</t>
+          <t>OMR ELECTRICAL LTD</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>16459084</t>
+          <t>16457261</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -4924,12 +4924,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>FASHLER LTD</t>
+          <t>HOLYWELL HOMES LTD</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>16459082</t>
+          <t>16457259</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4962,12 +4962,12 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>FINTIVITY LTD</t>
+          <t>GODMADE LTD</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>16459072</t>
+          <t>16459074</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -5000,12 +5000,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>WANNABEE LTD</t>
+          <t>RELIABLE STAFFING RECRUITS LIMITED</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>16459526</t>
+          <t>16457238</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -5038,12 +5038,12 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>S&amp;S ISTITHMĀR LTD</t>
+          <t>LATINOS TEESSIDE &amp; HISPANIC SENIORS COMMUNITY LTD</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>16459522</t>
+          <t>16459078</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -5076,12 +5076,12 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>TASHAN MEDIA LTD</t>
+          <t>MALHAMDALE GLAMPING LIMITED</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>16459523</t>
+          <t>16459064</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -5114,12 +5114,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>CLICKSPHARE CRAFT LTD</t>
+          <t>RENTAL DISREPAIR CLAIMS LTD</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>16459521</t>
+          <t>16459077</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -5152,12 +5152,12 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>AMIS &amp; WARD DEVELOPMENT LTD</t>
+          <t>SSFBN LIMITED</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>16459520</t>
+          <t>16459541</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -5190,12 +5190,12 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>THE CHAIR SALON LONDON LTD</t>
+          <t>NEHHEALTHCARE LTD</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>16459512</t>
+          <t>16456708</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -5228,12 +5228,12 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>SPYRO APPAREL LTD</t>
+          <t>INDEXIE LTD</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>16459515</t>
+          <t>16459546</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -5266,12 +5266,12 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>MILLE TRADING LTD</t>
+          <t>PROOFENANCE LTD</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>16459518</t>
+          <t>16457943</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -5304,12 +5304,12 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>CLARK AND CO DESIGN LIMITED</t>
+          <t>NEWMINERALS LTD</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>16459516</t>
+          <t>16455878</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -5342,12 +5342,12 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>NORDIC COOPERATION TECHNOLOGIES LIMITED</t>
+          <t>EVO AVIATION LIMITED</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>16459514</t>
+          <t>16456253</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -5380,12 +5380,12 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>LOUD AND CLEAR COACHING LIMITED</t>
+          <t>OILMYCAR LTD</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>16459549</t>
+          <t>16456706</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -5418,12 +5418,12 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>JC DEEP TECH LTD</t>
+          <t>CTLO LTD</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>16456256</t>
+          <t>16456701</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -5448,6 +5448,196 @@
         </is>
       </c>
       <c r="H132" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>PHONE STUDIO SOUTH LIMITED</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>16456765</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr"/>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>OPM ILL GO SHOP 4U LTD</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>16456764</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr"/>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>WGHR JI LTD</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>16456731</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr"/>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>BKK EQUESTRIAN LTD</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>16456733</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr"/>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>J.R'S SOUTHERN TWIST LTD</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>16459542</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr"/>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
         <is>
           <t>Other</t>
         </is>

</xml_diff>

<commit_message>
Auto update: 2025-05-20 05:39:32
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H137"/>
+  <dimension ref="A1:H176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,12 +554,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CLARITY VENTURE SUPPORT LTD</t>
+          <t>BILLION SCENTS LTD</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16460376</t>
+          <t>16460413</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -580,7 +580,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -592,12 +592,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MISBAH GOODS LTD</t>
+          <t>SKINNY SISTERS LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16460377</t>
+          <t>16460411</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -618,7 +618,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -630,12 +630,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PAVITA LOGISTICS LTD</t>
+          <t>HEART OF TOWN II LIMITED</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16460373</t>
+          <t>16460410</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -656,7 +656,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -668,12 +668,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ROAMING RETAIL LIMITED</t>
+          <t>KILIMANJARO MAVENS TREKS &amp; SAFARIS LTD</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16460382</t>
+          <t>16460407</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -694,7 +694,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -706,12 +706,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TRUE NORTH JOINERY LTD</t>
+          <t>JAMIL TALIB LTD</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16460359</t>
+          <t>16460389</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -732,7 +732,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -744,12 +744,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>VIVID MART LTD</t>
+          <t>PRACTICE MAKES PERFECT LTD</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16460370</t>
+          <t>16460388</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -770,7 +770,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -782,12 +782,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MASTER THE CHAIN LTD</t>
+          <t>YAKO CASINO LTD</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16460358</t>
+          <t>16460391</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -808,7 +808,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -820,12 +820,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>FONETHICS SOLUTIONS LTD</t>
+          <t>MINESHOCK LABS LTD</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SC848969</t>
+          <t>16460393</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -846,7 +846,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -858,12 +858,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>M&amp;S SOCIAL CARE CONSULTANTS LTD</t>
+          <t>SURREYSIDECOMPS LTD</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16460353</t>
+          <t>16460422</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -884,7 +884,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -896,12 +896,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>FAMILY COMMREPORT LTD</t>
+          <t>HAYES PARTNERS LTD</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16460356</t>
+          <t>16460412</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -922,24 +922,24 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BANDOS BY ADEBISI LTD</t>
+          <t>NPP RF2 LIMITED</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16460361</t>
+          <t>16460409</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -960,7 +960,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -972,12 +972,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>VITANOVA LEARNING LIMITED</t>
+          <t>PROTO DSGN LIMITED</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16460384</t>
+          <t>16460406</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -998,7 +998,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>04:43:32</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1010,12 +1010,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MEARNS CLEANING SERVICES LTD</t>
+          <t>TIMBRA PROJECTS LTD</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16460387</t>
+          <t>16460396</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>04:43:32</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1048,12 +1048,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>MONEY MART LTD</t>
+          <t>CORNISH IT CONSULTING LTD</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16460383</t>
+          <t>16460395</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1074,7 +1074,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>04:43:32</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1086,12 +1086,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>AA SELLER HUB LTD</t>
+          <t>RESTORCARE HEALTH LTD</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16460385</t>
+          <t>16460404</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>04:43:32</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1124,12 +1124,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>MOTIVATION AND PROSPERITY LTD</t>
+          <t>MAURYA &amp; SONS PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16460379</t>
+          <t>16460402</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1162,12 +1162,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>GMS7 LIMITED</t>
+          <t>COACHED BY JESS LIMITED</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>16460386</t>
+          <t>16460392</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1188,7 +1188,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>04:43:32</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1200,12 +1200,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>NARCISSIST APPAREL LTD</t>
+          <t>THE BROW CLINIC &amp; BEYOND LTD</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16460378</t>
+          <t>16460403</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1238,12 +1238,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BA CORP SOLUTIONS &amp; EVENTS LTD</t>
+          <t>ARORA MATERIALS LIMITED</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16460375</t>
+          <t>16460405</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1276,12 +1276,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>LUXCOMMERCE LTD</t>
+          <t>UNCOMFORTABLE CHATS LIMITED</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>16460360</t>
+          <t>16460394</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1302,7 +1302,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1314,12 +1314,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CLEARLABS PERFORMANCE LTD</t>
+          <t>CC GARAGE LTD</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16460364</t>
+          <t>16460397</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1352,12 +1352,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ACCORD FIRE DOORS LTD</t>
+          <t>GS GEPE II SIDECAR IV GP LLP</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16460363</t>
+          <t>SO308186</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1378,24 +1378,24 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>GP</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>LITBUILD LTD</t>
+          <t>ARDPEATON DEVELOPMENTS LIMITED</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16460368</t>
+          <t>SC848970</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1428,12 +1428,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2BCLOTHING LTD</t>
+          <t>PREMSPY HOLDING LIMITED</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16460354</t>
+          <t>SC848971</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1454,7 +1454,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1466,12 +1466,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>MAK'S TRADERS LTD</t>
+          <t>CALLAN’S CHILDREN COMPLEX CARE COMPANY LIMITED</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16460355</t>
+          <t>16460400</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1492,7 +1492,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1504,12 +1504,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>APEX PLUMBING AND HEATING SOLUTIONS LTD</t>
+          <t>AMGT HOLDING LTD</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16460374</t>
+          <t>16460401</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1530,7 +1530,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1542,12 +1542,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SKYFREIGHTGLOBAL LTD</t>
+          <t>DOME DYNAMICS LTD</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16460366</t>
+          <t>16460416</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1568,7 +1568,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1580,12 +1580,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ETECH VENTURE LIMITED</t>
+          <t>LC COURIERS LTD</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16460372</t>
+          <t>16460390</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1618,12 +1618,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>ORIENT CANTEEN LTD</t>
+          <t>LA AUTOMOTIVE LTD</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16460365</t>
+          <t>16460421</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1644,7 +1644,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1656,12 +1656,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>OMID'S ENTERPRISE LTD</t>
+          <t>SMARTY SPROUTS LTD</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16460381</t>
+          <t>16460399</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1694,12 +1694,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CLEANING MONK LTD</t>
+          <t>DEXKAANE SERVICES LIMITED</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16460369</t>
+          <t>16460419</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1720,7 +1720,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -1732,12 +1732,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>MASR PROPERTIES LTD</t>
+          <t>AGS STRUCTURAL OUTPUTS LTD</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>16460367</t>
+          <t>16460420</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1758,7 +1758,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1770,12 +1770,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>BY FATOU JAI LTD</t>
+          <t>NEW CROSS LOCAL LIMITED</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16460371</t>
+          <t>16460417</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -1808,12 +1808,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>FIND YOUR INDUSTRY LTD</t>
+          <t>INJECTIVE AESTHETICS LTD</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16460362</t>
+          <t>16460415</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1834,7 +1834,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>03:31:34</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1846,17 +1846,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>JANITZA UK LIMITED</t>
+          <t>PARDS MART LTD</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16456233</t>
+          <t>16460414</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1867,12 +1867,12 @@
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -1884,17 +1884,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>UBAH MEDIA LAB LTD</t>
+          <t>RUBU MAJAZ ALMUTAMAYIZAH LTD</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16459548</t>
+          <t>16460408</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1905,12 +1905,12 @@
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -1922,17 +1922,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>HAUS OF PALETTE LTD</t>
+          <t>RATHDOWN LTD</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16456236</t>
+          <t>16460398</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1943,12 +1943,12 @@
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -1960,33 +1960,33 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>CA ELECTRICAL (YORKSHIRE) LTD</t>
+          <t>HOLMCROFT LIMITED</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>16459547</t>
+          <t>OE033935</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>registered</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -1998,17 +1998,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>HOUSE OF RODEOS LTD</t>
+          <t>HEALTHY SWEETS UK LTD</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16456218</t>
+          <t>16460418</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -2019,12 +2019,12 @@
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2036,17 +2036,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>CALIBRE LDN LIMITED</t>
+          <t>MASR PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16457945</t>
+          <t>16460367</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -2057,12 +2057,12 @@
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2074,17 +2074,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>JAI-HO STAFFING LTD</t>
+          <t>APEX PLUMBING AND HEATING SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16456221</t>
+          <t>16460374</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2095,12 +2095,12 @@
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2112,17 +2112,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>WINDOW CLEANING SOUTHEND LTD</t>
+          <t>BA CORP SOLUTIONS &amp; EVENTS LTD</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16456227</t>
+          <t>16460375</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -2133,12 +2133,12 @@
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2150,17 +2150,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>SHOTTON CURRY HOUSE LIMITED</t>
+          <t>LUXCOMMERCE LTD</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16459062</t>
+          <t>16460360</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -2171,12 +2171,12 @@
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -2188,17 +2188,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>OCEANHEART MARINE SERVICE CO., LTD</t>
+          <t>CLEARLABS PERFORMANCE LTD</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16459543</t>
+          <t>16460364</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2209,12 +2209,12 @@
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -2226,17 +2226,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>PANEER CRAFT LTD. LIMITED</t>
+          <t>ACCORD FIRE DOORS LTD</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>16457973</t>
+          <t>16460363</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2247,12 +2247,12 @@
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2264,17 +2264,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>CAZAM PROPERTY LTD</t>
+          <t>LITBUILD LTD</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>16459061</t>
+          <t>16460368</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2285,12 +2285,12 @@
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2302,17 +2302,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>M S GROUP FIRST UK LIMITED</t>
+          <t>MAK'S TRADERS LTD</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16459057</t>
+          <t>16460355</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2323,12 +2323,12 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -2340,17 +2340,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>PARKSIDE GETAWAYS LIMITED</t>
+          <t>SKYFREIGHTGLOBAL LTD</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>16459059</t>
+          <t>16460366</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2361,12 +2361,12 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -2378,17 +2378,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>DRIVERIGHT REPAIRS LTD</t>
+          <t>GMS7 LIMITED</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>16459058</t>
+          <t>16460386</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2399,12 +2399,12 @@
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>04:43:32</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -2416,17 +2416,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>GK ZYGALA LIMITED</t>
+          <t>ETECH VENTURE LIMITED</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16457953</t>
+          <t>16460372</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2437,12 +2437,12 @@
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -2454,17 +2454,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>MAPLE (510) LIMITED</t>
+          <t>ORIENT CANTEEN LTD</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>16457954</t>
+          <t>16460365</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2475,12 +2475,12 @@
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -2492,17 +2492,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>STEFANPERSAUDLEGACYPROJECT LIMITED</t>
+          <t>OMID'S ENTERPRISE LTD</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>16456208</t>
+          <t>16460381</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2513,12 +2513,12 @@
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -2530,17 +2530,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>CAMBRIDGE VETS LTD</t>
+          <t>CLEANING MONK LTD</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>16457975</t>
+          <t>16460369</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2551,12 +2551,12 @@
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -2568,17 +2568,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>ROCK&amp;WALLS LTD</t>
+          <t>BY FATOU JAI LTD</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>16457974</t>
+          <t>16460371</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2589,12 +2589,12 @@
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -2606,17 +2606,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>HARRY'S OFFLICENCE &amp; TAKEAWAY LTD</t>
+          <t>FIND YOUR INDUSTRY LTD</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>16456203</t>
+          <t>16460362</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2627,12 +2627,12 @@
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -2644,17 +2644,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>IDCHEM CONSULTING LIMITED</t>
+          <t>NARCISSIST APPAREL LTD</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>16456205</t>
+          <t>16460378</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2665,12 +2665,12 @@
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -2682,17 +2682,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>FITCARDIOLOGY LTD</t>
+          <t>2BCLOTHING LTD</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16457244</t>
+          <t>16460354</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2703,12 +2703,12 @@
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -2720,17 +2720,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>STOA PROJECTS LTD</t>
+          <t>MOTIVATION AND PROSPERITY LTD</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16456212</t>
+          <t>16460379</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2741,12 +2741,12 @@
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -2758,17 +2758,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>CHIMNEY CHAPS LTD</t>
+          <t>FONETHICS SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>16456261</t>
+          <t>SC848969</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2779,12 +2779,12 @@
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -2796,17 +2796,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>JC DEEP TECH LTD</t>
+          <t>CLARITY VENTURE SUPPORT LTD</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16456256</t>
+          <t>16460376</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2817,12 +2817,12 @@
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -2834,17 +2834,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>LOUD AND CLEAR COACHING LIMITED</t>
+          <t>AA SELLER HUB LTD</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>16459549</t>
+          <t>16460385</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2855,12 +2855,12 @@
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>04:43:32</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -2872,17 +2872,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>NORDIC COOPERATION TECHNOLOGIES LIMITED</t>
+          <t>PAVITA LOGISTICS LTD</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>16459514</t>
+          <t>16460373</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2893,12 +2893,12 @@
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -2910,17 +2910,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>CLARK AND CO DESIGN LIMITED</t>
+          <t>ROAMING RETAIL LIMITED</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>16459516</t>
+          <t>16460382</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2931,12 +2931,12 @@
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -2948,17 +2948,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>MILLE TRADING LTD</t>
+          <t>TRUE NORTH JOINERY LTD</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>16459518</t>
+          <t>16460359</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2969,12 +2969,12 @@
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -2986,17 +2986,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>SPYRO APPAREL LTD</t>
+          <t>VIVID MART LTD</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>16459515</t>
+          <t>16460370</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -3007,12 +3007,12 @@
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -3024,17 +3024,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>THE CHAIR SALON LONDON LTD</t>
+          <t>MASTER THE CHAIN LTD</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>16459512</t>
+          <t>16460358</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -3045,12 +3045,12 @@
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -3062,17 +3062,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>AMIS &amp; WARD DEVELOPMENT LTD</t>
+          <t>MISBAH GOODS LTD</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>16459520</t>
+          <t>16460377</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -3083,12 +3083,12 @@
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -3100,17 +3100,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>CLICKSPHARE CRAFT LTD</t>
+          <t>M&amp;S SOCIAL CARE CONSULTANTS LTD</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>16459521</t>
+          <t>16460353</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -3121,12 +3121,12 @@
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -3138,17 +3138,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>TASHAN MEDIA LTD</t>
+          <t>FAMILY COMMREPORT LTD</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16459523</t>
+          <t>16460356</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -3159,12 +3159,12 @@
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
@@ -3176,17 +3176,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>S&amp;S ISTITHMĀR LTD</t>
+          <t>BANDOS BY ADEBISI LTD</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16459522</t>
+          <t>16460361</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -3197,12 +3197,12 @@
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>03:31:34</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
@@ -3214,17 +3214,17 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>WANNABEE LTD</t>
+          <t>VITANOVA LEARNING LIMITED</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>16459526</t>
+          <t>16460384</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -3235,12 +3235,12 @@
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>04:43:32</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -3252,17 +3252,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>FINTIVITY LTD</t>
+          <t>MEARNS CLEANING SERVICES LTD</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16459072</t>
+          <t>16460387</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -3273,12 +3273,12 @@
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>04:43:32</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
@@ -3290,17 +3290,17 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>FASHLER LTD</t>
+          <t>MONEY MART LTD</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>16459082</t>
+          <t>16460383</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -3311,12 +3311,12 @@
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2025-05-19</t>
+          <t>2025-05-20</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>21:36:29</t>
+          <t>04:43:32</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -3328,12 +3328,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>CTPROPS LIMITED</t>
+          <t>HOLYWELL HOMES LTD</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>16459084</t>
+          <t>16457259</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3366,12 +3366,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>NEW MOUNT DAISY LIMITED</t>
+          <t>SSFBN LIMITED</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>16457237</t>
+          <t>16459541</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3404,12 +3404,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>INSPOCL LTD</t>
+          <t>RENTAL DISREPAIR CLAIMS LTD</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>16457967</t>
+          <t>16459077</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3442,12 +3442,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>FARRINGDON HOUSE FINANCIAL SERVICES LIMITED</t>
+          <t>MALHAMDALE GLAMPING LIMITED</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>16457279</t>
+          <t>16459064</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3480,12 +3480,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>ATSP FIN LTD</t>
+          <t>LATINOS TEESSIDE &amp; HISPANIC SENIORS COMMUNITY LTD</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>16456749</t>
+          <t>16459078</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3518,12 +3518,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>BREEZY HOMES LIMITED</t>
+          <t>RELIABLE STAFFING RECRUITS LIMITED</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>16456709</t>
+          <t>16457238</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3556,12 +3556,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>LEOFRIC LTD</t>
+          <t>GODMADE LTD</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>16456712</t>
+          <t>16459074</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3594,12 +3594,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>A STAR HEALTH LTD</t>
+          <t>BUILTBRITE LTD</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>16456234</t>
+          <t>16457962</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3632,12 +3632,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>AUSTIN RICE LTD</t>
+          <t>OMR ELECTRICAL LTD</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>NI729522</t>
+          <t>16457261</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3670,12 +3670,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>LEADANICS LIMITED</t>
+          <t>GUIDED BRAKE SERVICE LTD</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>16457965</t>
+          <t>16457264</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3708,12 +3708,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>DEVIPROX LTD</t>
+          <t>INDEXIE LTD</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>16457970</t>
+          <t>16459546</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3746,12 +3746,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>DEHBINI LIMITED</t>
+          <t>LGAM PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>16456493</t>
+          <t>16457957</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3784,12 +3784,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>HONG KONG XUNHUA FREIGHT LIMITED</t>
+          <t>INP SERVICES LTD</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>16456735</t>
+          <t>16459069</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3822,12 +3822,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>FARYAL ENTERPRISE LIMITED</t>
+          <t>MEC SURVEYORS LTD</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16456748</t>
+          <t>16456734</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3860,12 +3860,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>SWIFT BUSINESS GROWTH.AI LTD</t>
+          <t>APEX PREMIER PROPERTY SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>16456250</t>
+          <t>16456756</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3898,12 +3898,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>NEWCO SWANSEA SOCIAL INFRASTRUCTURE LP</t>
+          <t>NEHHEALTHCARE LTD</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>LP024176</t>
+          <t>16456708</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3929,19 +3929,19 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>MAJESTIC EXTERIOR CLEANING SERVICES LTD</t>
+          <t>CALIBRE LDN LIMITED</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>16457230</t>
+          <t>16457945</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3974,12 +3974,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>AMIKOBA LTD</t>
+          <t>PROOFENANCE LTD</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>16459545</t>
+          <t>16457943</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -4012,12 +4012,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Y-3 APARTMENTS LTD</t>
+          <t>NEWMINERALS LTD</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>16457262</t>
+          <t>16455878</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -4050,12 +4050,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>JORDAN CAMPBELL LTD</t>
+          <t>EVO AVIATION LIMITED</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>NI729519</t>
+          <t>16456253</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4088,12 +4088,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>KINARA PROPERTIES LTD</t>
+          <t>OILMYCAR LTD</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>16456244</t>
+          <t>16456706</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -4126,12 +4126,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>UKG BB HOLDINGS LTD</t>
+          <t>CTLO LTD</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>16456246</t>
+          <t>16456701</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4164,12 +4164,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>SOCIAL SLOT LTD</t>
+          <t>PHONE STUDIO SOUTH LIMITED</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>16456245</t>
+          <t>16456765</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -4202,12 +4202,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>B HOLLAND &amp; SONS (HOLDINGS) LTD</t>
+          <t>OPM ILL GO SHOP 4U LTD</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>16456243</t>
+          <t>16456764</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -4240,12 +4240,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>J&amp;S DISTRIBUTIONS LIMITED</t>
+          <t>WGHR JI LTD</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>16456242</t>
+          <t>16456731</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -4278,12 +4278,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>ELLISA'S BEAUTY LTD</t>
+          <t>BKK EQUESTRIAN LTD</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>16456750</t>
+          <t>16456733</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -4316,12 +4316,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>MARKETING DG LTD</t>
+          <t>J.R'S SOUTHERN TWIST LTD</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>16456254</t>
+          <t>16459542</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -4354,12 +4354,12 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>PHOENIX CONSULTING INTERNATIONAL LIMITED</t>
+          <t>CA ELECTRICAL (YORKSHIRE) LTD</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>16457267</t>
+          <t>16459547</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -4392,12 +4392,12 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>DCR HOLDINGS &amp; INVESTMENTS LTD</t>
+          <t>HAUS OF PALETTE LTD</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>16457272</t>
+          <t>16456236</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -4423,19 +4423,19 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>POWERS ELECTRICAL LTD</t>
+          <t>UBAH MEDIA LAB LTD</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>16457270</t>
+          <t>16459548</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -4468,12 +4468,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>GLIMORA GLOBAL LTD</t>
+          <t>JANITZA UK LIMITED</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>16457265</t>
+          <t>16456233</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -4506,12 +4506,12 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>METAHAVEN LTD</t>
+          <t>JAI-HO STAFFING LTD</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>16457273</t>
+          <t>16456221</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -4544,12 +4544,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>YSGARLAD PROPERTIES LTD</t>
+          <t>FLIP IT GLOBAL LTD</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>16457268</t>
+          <t>16456758</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -4620,12 +4620,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>FLIP IT GLOBAL LTD</t>
+          <t>YSGARLAD PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>16456758</t>
+          <t>16457268</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -4658,12 +4658,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>APEX PREMIER PROPERTY SOLUTIONS LTD</t>
+          <t>FITCARDIOLOGY LTD</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>16456756</t>
+          <t>16457244</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -4696,12 +4696,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>MEC SURVEYORS LTD</t>
+          <t>WANNABEE LTD</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>16456734</t>
+          <t>16459526</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -4734,12 +4734,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>INP SERVICES LTD</t>
+          <t>S&amp;S ISTITHMĀR LTD</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>16459069</t>
+          <t>16459522</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -4772,12 +4772,12 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>LGAM PROPERTIES LTD</t>
+          <t>TASHAN MEDIA LTD</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>16457957</t>
+          <t>16459523</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -4810,12 +4810,12 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>BUILTBRITE LTD</t>
+          <t>CLICKSPHARE CRAFT LTD</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>16457962</t>
+          <t>16459521</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -4848,12 +4848,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>GUIDED BRAKE SERVICE LTD</t>
+          <t>AMIS &amp; WARD DEVELOPMENT LTD</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>16457264</t>
+          <t>16459520</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -4886,12 +4886,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>OMR ELECTRICAL LTD</t>
+          <t>THE CHAIR SALON LONDON LTD</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>16457261</t>
+          <t>16459512</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -4924,12 +4924,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>HOLYWELL HOMES LTD</t>
+          <t>SPYRO APPAREL LTD</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>16457259</t>
+          <t>16459515</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4962,12 +4962,12 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>GODMADE LTD</t>
+          <t>MILLE TRADING LTD</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>16459074</t>
+          <t>16459518</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -5000,12 +5000,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>RELIABLE STAFFING RECRUITS LIMITED</t>
+          <t>CLARK AND CO DESIGN LIMITED</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>16457238</t>
+          <t>16459516</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -5038,12 +5038,12 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>LATINOS TEESSIDE &amp; HISPANIC SENIORS COMMUNITY LTD</t>
+          <t>NORDIC COOPERATION TECHNOLOGIES LIMITED</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>16459078</t>
+          <t>16459514</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -5076,12 +5076,12 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>MALHAMDALE GLAMPING LIMITED</t>
+          <t>LOUD AND CLEAR COACHING LIMITED</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>16459064</t>
+          <t>16459549</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -5114,12 +5114,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>RENTAL DISREPAIR CLAIMS LTD</t>
+          <t>JC DEEP TECH LTD</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>16459077</t>
+          <t>16456256</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -5152,12 +5152,12 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>SSFBN LIMITED</t>
+          <t>CHIMNEY CHAPS LTD</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>16459541</t>
+          <t>16456261</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -5190,12 +5190,12 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>NEHHEALTHCARE LTD</t>
+          <t>STOA PROJECTS LTD</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>16456708</t>
+          <t>16456212</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -5228,12 +5228,12 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>INDEXIE LTD</t>
+          <t>IDCHEM CONSULTING LIMITED</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>16459546</t>
+          <t>16456205</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -5266,12 +5266,12 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>PROOFENANCE LTD</t>
+          <t>METAHAVEN LTD</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>16457943</t>
+          <t>16457273</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -5304,12 +5304,12 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>NEWMINERALS LTD</t>
+          <t>HARRY'S OFFLICENCE &amp; TAKEAWAY LTD</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>16455878</t>
+          <t>16456203</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -5342,12 +5342,12 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>EVO AVIATION LIMITED</t>
+          <t>ROCK&amp;WALLS LTD</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>16456253</t>
+          <t>16457974</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -5380,12 +5380,12 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>OILMYCAR LTD</t>
+          <t>CAMBRIDGE VETS LTD</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>16456706</t>
+          <t>16457975</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -5418,12 +5418,12 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>CTLO LTD</t>
+          <t>STEFANPERSAUDLEGACYPROJECT LIMITED</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>16456701</t>
+          <t>16456208</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -5456,12 +5456,12 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>PHONE STUDIO SOUTH LIMITED</t>
+          <t>MAPLE (510) LIMITED</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>16456765</t>
+          <t>16457954</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -5494,12 +5494,12 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>OPM ILL GO SHOP 4U LTD</t>
+          <t>GK ZYGALA LIMITED</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>16456764</t>
+          <t>16457953</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -5532,12 +5532,12 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>WGHR JI LTD</t>
+          <t>DRIVERIGHT REPAIRS LTD</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>16456731</t>
+          <t>16459058</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -5570,12 +5570,12 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>BKK EQUESTRIAN LTD</t>
+          <t>PARKSIDE GETAWAYS LIMITED</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>16456733</t>
+          <t>16459059</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -5608,12 +5608,12 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>J.R'S SOUTHERN TWIST LTD</t>
+          <t>M S GROUP FIRST UK LIMITED</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>16459542</t>
+          <t>16459057</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -5638,6 +5638,1488 @@
         </is>
       </c>
       <c r="H137" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>CAZAM PROPERTY LTD</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>16459061</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr"/>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>PANEER CRAFT LTD. LIMITED</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>16457973</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr"/>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>OCEANHEART MARINE SERVICE CO., LTD</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>16459543</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr"/>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>SHOTTON CURRY HOUSE LIMITED</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>16459062</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr"/>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>WINDOW CLEANING SOUTHEND LTD</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>16456227</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr"/>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>FINTIVITY LTD</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>16459072</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr"/>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>FASHLER LTD</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>16459082</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr"/>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>CTPROPS LIMITED</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>16459084</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr"/>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>NEW MOUNT DAISY LIMITED</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>16457237</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr"/>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>GLIMORA GLOBAL LTD</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>16457265</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr"/>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>POWERS ELECTRICAL LTD</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>16457270</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr"/>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>DCR HOLDINGS &amp; INVESTMENTS LTD</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>16457272</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr"/>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>Investments</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>PHOENIX CONSULTING INTERNATIONAL LIMITED</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>16457267</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr"/>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>MARKETING DG LTD</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>16456254</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr"/>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>ELLISA'S BEAUTY LTD</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>16456750</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr"/>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>J&amp;S DISTRIBUTIONS LIMITED</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>16456242</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr"/>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>B HOLLAND &amp; SONS (HOLDINGS) LTD</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>16456243</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr"/>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>SOCIAL SLOT LTD</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>16456245</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr"/>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>UKG BB HOLDINGS LTD</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>16456246</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr"/>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>KINARA PROPERTIES LTD</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>16456244</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr"/>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>JORDAN CAMPBELL LTD</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>NI729519</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr"/>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Y-3 APARTMENTS LTD</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>16457262</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr"/>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>AMIKOBA LTD</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>16459545</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr"/>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>MAJESTIC EXTERIOR CLEANING SERVICES LTD</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>16457230</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr"/>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>NEWCO SWANSEA SOCIAL INFRASTRUCTURE LP</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>LP024176</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr"/>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>SWIFT BUSINESS GROWTH.AI LTD</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>16456250</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr"/>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>FARYAL ENTERPRISE LIMITED</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>16456748</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr"/>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>HOUSE OF RODEOS LTD</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>16456218</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr"/>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>DEHBINI LIMITED</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>16456493</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr"/>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>DEVIPROX LTD</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>16457970</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr"/>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>LEADANICS LIMITED</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>16457965</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr"/>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>AUSTIN RICE LTD</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>NI729522</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr"/>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>A STAR HEALTH LTD</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>16456234</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr"/>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>LEOFRIC LTD</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>16456712</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr"/>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>BREEZY HOMES LIMITED</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>16456709</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr"/>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>ATSP FIN LTD</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>16456749</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr"/>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>FARRINGDON HOUSE FINANCIAL SERVICES LIMITED</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>16457279</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr"/>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>INSPOCL LTD</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>16457967</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr"/>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>HONG KONG XUNHUA FREIGHT LIMITED</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>16456735</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr"/>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>21:36:29</t>
+        </is>
+      </c>
+      <c r="H176" t="inlineStr">
         <is>
           <t>Other</t>
         </is>

</xml_diff>

<commit_message>
Auto update: 2025-05-20 19:04:45
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -516,12 +516,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ASSURED LETTINGS AND SALES LTD</t>
+          <t>YANG HAIJUN LTD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16462049</t>
+          <t>16460671</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -554,12 +554,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>RAPID FULFILL LTD</t>
+          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16462586</t>
+          <t>16460503</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -585,19 +585,19 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ASHTOWN INTERVENTION &amp; COMPLETION SERVICES LTD</t>
+          <t>THE SPICE INVADERS LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SC849120</t>
+          <t>16460505</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -630,12 +630,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DANDINI PANTOMIMES LIMITED</t>
+          <t>DEE BEE TRADING LTD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16462588</t>
+          <t>16460511</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -668,12 +668,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>POINT BREAK 7 LTD</t>
+          <t>INNOVATION MT LTD</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16462560</t>
+          <t>16460646</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -706,12 +706,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TBT KENT LTD</t>
+          <t>BRANWELL PROJECTS LIMITED</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16462558</t>
+          <t>16460653</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -744,12 +744,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ELLAHI PROPERTY HOLDINGS LTD</t>
+          <t>MAYTREE ELITE PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16462030</t>
+          <t>16460650</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -782,12 +782,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>SUBLINE LTD</t>
+          <t>MEDIA WEB PRO LTD</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16462043</t>
+          <t>16460644</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -820,12 +820,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>HOMELORD T LTD</t>
+          <t>ASPC CONTENT CO LTD</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16462031</t>
+          <t>16460643</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -858,12 +858,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ANITA TECHNOLOGY LTD</t>
+          <t>BLUEPRINT VOYAGE MEDIA COMPANY LIMITED</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16462036</t>
+          <t>16460649</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -896,12 +896,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>DAILY NOVA LTD</t>
+          <t>SARASI LTD</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16462033</t>
+          <t>16460670</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -934,12 +934,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CUT N GLOW BEAUTY LIMITED</t>
+          <t>ST PAUL'S COURT DEVELOPMENT LTD</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16462051</t>
+          <t>16460669</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -972,12 +972,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>VIRTUAL CO. UK LTD</t>
+          <t>ASSURED LETTINGS AND SALES LTD</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16460502</t>
+          <t>16462049</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1010,12 +1010,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GEOAIR SOLAR LIMITED</t>
+          <t>SAMVIV PARTNERS LTD</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16462052</t>
+          <t>16460672</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1041,19 +1041,19 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CSS BR ASSET LIMITED</t>
+          <t>COREMARINE SOLUTIONS CIC</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16462021</t>
+          <t>16460663</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1086,12 +1086,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>LEMON TREE REAL ESTATE LIMITED</t>
+          <t>AMPERSAND MANAGEMENT UK LTD</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16462023</t>
+          <t>16460662</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1124,12 +1124,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>DARWIN INVEST LTD</t>
+          <t>TRIPLE J HOUSING LTD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16461938</t>
+          <t>16460681</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1162,12 +1162,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AVIATION TOOL POOLING LLC</t>
+          <t>DXI DAILY NECESSITIES CO., LTD.</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>OE033940</t>
+          <t>16460679</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>active</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -1200,12 +1200,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>MARTIAL FITNESS (SW) LTD</t>
+          <t>PREVENTR ACTIVE FIRE LTD</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16461940</t>
+          <t>16460677</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1238,12 +1238,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>JLI CONSTRUCTION LTD</t>
+          <t>MOUNTAIN SEA SHIP SERVICE CO., LTD</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16461948</t>
+          <t>16460640</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1276,12 +1276,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>IVOLVIA LTD</t>
+          <t>T-REX (GUILDFORD) LIMITED</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>16461947</t>
+          <t>16460637</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1314,12 +1314,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>B AND K FLOORING LIMITED</t>
+          <t>HOMEASE LTD</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16461926</t>
+          <t>16460666</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1352,12 +1352,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>LANUNE LTD</t>
+          <t>INAYA HEALTHCARE LTD</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16461925</t>
+          <t>16460657</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1390,12 +1390,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>KOMO NAIL &amp; BEAUTY LTD</t>
+          <t>VALLEY SEVEN DEVELOPMENTS LIMITED</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16462578</t>
+          <t>16460659</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1428,12 +1428,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>AR BUILDING AND GARDENING SERVICES LTD</t>
+          <t>REIGNING MEDIA LIMITED</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16462581</t>
+          <t>16461275</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1466,12 +1466,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>DGPI LTD</t>
+          <t>YANGLIN CHEN LIMITED</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>SC849118</t>
+          <t>16461915</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1497,19 +1497,19 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>LIT BARBERS LTD</t>
+          <t>CRISPY GLEN LTD</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16462561</t>
+          <t>SC849027</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1542,12 +1542,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>LIU YUMEI LTD</t>
+          <t>KGM CONSTRUCTION LTD</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16462901</t>
+          <t>16461264</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1580,12 +1580,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>MAKPLAS LTD</t>
+          <t>TUK TALENT LTD</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>SC849155</t>
+          <t>16461265</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1618,12 +1618,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CFBUK SECURED FINANCE LTD</t>
+          <t>SW2 CONSTRUCTION LIMITED</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16462904</t>
+          <t>16461262</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1656,12 +1656,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>INTERA AI HOLDINGS UK LIMITED</t>
+          <t>FUNCTION.ALL.OVER LTD</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16462908</t>
+          <t>16461272</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1694,12 +1694,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ALOVER VUBINH LIMITED</t>
+          <t>AMARA WELLS LTD</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16462909</t>
+          <t>SC849026</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1732,12 +1732,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>COLLIN CARE HOLDINGS LIMITED</t>
+          <t>GROUND MORTGAGE SERVICES LIMITED</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>SC849153</t>
+          <t>16461278</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1770,12 +1770,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
+          <t>MUNCHIES KEBAB DESERT LTD</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16462880</t>
+          <t>16461260</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1801,19 +1801,19 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>CAMPBELL &amp; DOIG LTD</t>
+          <t>4D CAPITAL PROPCO (44) LIMITED</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>SC849151</t>
+          <t>16461269</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1839,19 +1839,19 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>3 MORDEN CLIFF LTD</t>
+          <t>MIRE LTD</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16462875</t>
+          <t>16461902</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1884,12 +1884,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>AFROSCOT VENTURES LTD</t>
+          <t>GIG32 LIMITED</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16462878</t>
+          <t>16461898</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1915,19 +1915,19 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>BOWEN BUSINESS LTD</t>
+          <t>LEADALE CITY LTD</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16462877</t>
+          <t>16461899</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1960,12 +1960,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>PAMIR MECHANICAL LTD</t>
+          <t>48 CONEY STREET LIMITED</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>16462876</t>
+          <t>16461897</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1998,12 +1998,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>BLITHFIELD PROPERTY SOLUTIONS LTD</t>
+          <t>FND MOTORS LIMITED</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16462888</t>
+          <t>16461900</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2036,12 +2036,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>WIMWA LTD</t>
+          <t>ALI SHOP LTD</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16462889</t>
+          <t>16461895</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2074,12 +2074,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>GASSINGITUP LTD</t>
+          <t>KASZCZUK LTD</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16462883</t>
+          <t>16461901</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2112,12 +2112,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>MAYROL UK LIMITED</t>
+          <t>AMPLIFORTH CONSULTING LIMITED</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16462870</t>
+          <t>16461904</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2150,12 +2150,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>MANPOD LTD</t>
+          <t>DDPT HOLDINGS LIMITED</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16462873</t>
+          <t>16461906</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2188,12 +2188,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>JWP INDUSTRIES LIMITED</t>
+          <t>GLOBAL CREW LTD</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16462872</t>
+          <t>16461905</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2226,12 +2226,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>LEW-BUD LTD</t>
+          <t>PRIME ATHLETIC CO LTD</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>16462565</t>
+          <t>16461911</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2264,12 +2264,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
+          <t>TMS ASSETS LTD</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SC849117</t>
+          <t>16461913</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2295,19 +2295,19 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>ECCLES-WOOD LTD</t>
+          <t>LANYNSEN HOUSE LTD</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SC849115</t>
+          <t>16461918</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2340,12 +2340,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>THE FISH SHOP 17 LTD</t>
+          <t>LEAD INFO LTD</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>16461921</t>
+          <t>16461919</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2416,12 +2416,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>LEAD INFO LTD</t>
+          <t>THE FISH SHOP 17 LTD</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16461919</t>
+          <t>16461921</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2454,12 +2454,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>INAYA HEALTHCARE LTD</t>
+          <t>KOMO NAIL &amp; BEAUTY LTD</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>16460657</t>
+          <t>16462578</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2492,12 +2492,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>HOMEASE LTD</t>
+          <t>B AND K FLOORING LIMITED</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>16460666</t>
+          <t>16461926</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2530,12 +2530,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>T-REX (GUILDFORD) LIMITED</t>
+          <t>IVOLVIA LTD</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>16460637</t>
+          <t>16461947</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2568,12 +2568,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>MOUNTAIN SEA SHIP SERVICE CO., LTD</t>
+          <t>JLI CONSTRUCTION LTD</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>16460640</t>
+          <t>16461948</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2606,12 +2606,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>PREVENTR ACTIVE FIRE LTD</t>
+          <t>MARTIAL FITNESS (SW) LTD</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>16460677</t>
+          <t>16461940</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2644,12 +2644,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>DXI DAILY NECESSITIES CO., LTD.</t>
+          <t>AVIATION TOOL POOLING LLC</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>16460679</t>
+          <t>OE033940</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2659,7 +2659,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>registered</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -2682,12 +2682,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>TRIPLE J HOUSING LTD</t>
+          <t>DARWIN INVEST LTD</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16460681</t>
+          <t>16461938</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2720,12 +2720,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>AMPERSAND MANAGEMENT UK LTD</t>
+          <t>LEMON TREE REAL ESTATE LIMITED</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16460662</t>
+          <t>16462023</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2758,12 +2758,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>COREMARINE SOLUTIONS CIC</t>
+          <t>CSS BR ASSET LIMITED</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>16460663</t>
+          <t>16462021</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2796,12 +2796,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>SAMVIV PARTNERS LTD</t>
+          <t>GEOAIR SOLAR LIMITED</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16460672</t>
+          <t>16462052</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2827,19 +2827,19 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>ST PAUL'S COURT DEVELOPMENT LTD</t>
+          <t>VIRTUAL CO. UK LTD</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>16460669</t>
+          <t>16460502</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2872,12 +2872,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>YANG HAIJUN LTD</t>
+          <t>CUT N GLOW BEAUTY LIMITED</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>16460671</t>
+          <t>16462051</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2910,12 +2910,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>SARASI LTD</t>
+          <t>DAILY NOVA LTD</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>16460670</t>
+          <t>16462033</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2948,12 +2948,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>BLUEPRINT VOYAGE MEDIA COMPANY LIMITED</t>
+          <t>ANITA TECHNOLOGY LTD</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>16460649</t>
+          <t>16462036</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2986,12 +2986,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>ASPC CONTENT CO LTD</t>
+          <t>HOMELORD T LTD</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>16460643</t>
+          <t>16462031</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3024,12 +3024,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>MEDIA WEB PRO LTD</t>
+          <t>SUBLINE LTD</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>16460644</t>
+          <t>16462043</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3062,12 +3062,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>MAYTREE ELITE PROPERTIES LTD</t>
+          <t>ELLAHI PROPERTY HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>16460650</t>
+          <t>16462030</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3100,12 +3100,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>BRANWELL PROJECTS LIMITED</t>
+          <t>TBT KENT LTD</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>16460653</t>
+          <t>16462558</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3138,12 +3138,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>INNOVATION MT LTD</t>
+          <t>POINT BREAK 7 LTD</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16460646</t>
+          <t>16462560</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3176,12 +3176,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>DEE BEE TRADING LTD</t>
+          <t>DANDINI PANTOMIMES LIMITED</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16460511</t>
+          <t>16462588</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3214,12 +3214,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>THE SPICE INVADERS LTD</t>
+          <t>ASHTOWN INTERVENTION &amp; COMPLETION SERVICES LTD</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>16460505</t>
+          <t>SC849120</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3252,12 +3252,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
+          <t>RAPID FULFILL LTD</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16460503</t>
+          <t>16462586</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3283,19 +3283,19 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>VALLEY SEVEN DEVELOPMENTS LIMITED</t>
+          <t>LANUNE LTD</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>16460659</t>
+          <t>16461925</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3328,12 +3328,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>REIGNING MEDIA LIMITED</t>
+          <t>AR BUILDING AND GARDENING SERVICES LTD</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>16461275</t>
+          <t>16462581</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3366,12 +3366,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>YANGLIN CHEN LIMITED</t>
+          <t>ECCLES-WOOD LTD</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>16461915</t>
+          <t>SC849115</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3404,12 +3404,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>CRISPY GLEN LTD</t>
+          <t>DGPI LTD</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>SC849027</t>
+          <t>SC849118</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3435,19 +3435,19 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>GP</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>LANYNSEN HOUSE LTD</t>
+          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>16461918</t>
+          <t>SC849117</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3473,19 +3473,19 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>TMS ASSETS LTD</t>
+          <t>LEW-BUD LTD</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>16461913</t>
+          <t>16462565</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3518,12 +3518,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>PRIME ATHLETIC CO LTD</t>
+          <t>JWP INDUSTRIES LIMITED</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>16461911</t>
+          <t>16462872</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3556,12 +3556,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>GLOBAL CREW LTD</t>
+          <t>MANPOD LTD</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>16461905</t>
+          <t>16462873</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3594,12 +3594,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>DDPT HOLDINGS LIMITED</t>
+          <t>MAYROL UK LIMITED</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>16461906</t>
+          <t>16462870</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3632,12 +3632,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>AMPLIFORTH CONSULTING LIMITED</t>
+          <t>GASSINGITUP LTD</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>16461904</t>
+          <t>16462883</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3670,12 +3670,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>KASZCZUK LTD</t>
+          <t>WIMWA LTD</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>16461901</t>
+          <t>16462889</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3708,12 +3708,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>ALI SHOP LTD</t>
+          <t>BLITHFIELD PROPERTY SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>16461895</t>
+          <t>16462888</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3746,12 +3746,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>FND MOTORS LIMITED</t>
+          <t>PAMIR MECHANICAL LTD</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>16461900</t>
+          <t>16462876</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3784,12 +3784,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>48 CONEY STREET LIMITED</t>
+          <t>BOWEN BUSINESS LTD</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>16461897</t>
+          <t>16462877</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3822,12 +3822,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>LEADALE CITY LTD</t>
+          <t>AFROSCOT VENTURES LTD</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16461899</t>
+          <t>16462878</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3853,19 +3853,19 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>GIG32 LIMITED</t>
+          <t>3 MORDEN CLIFF LTD</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>16461898</t>
+          <t>16462875</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3898,12 +3898,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>MIRE LTD</t>
+          <t>CAMPBELL &amp; DOIG LTD</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>16461902</t>
+          <t>SC849151</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3936,12 +3936,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>4D CAPITAL PROPCO (44) LIMITED</t>
+          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>16461269</t>
+          <t>16462880</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3974,12 +3974,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>MUNCHIES KEBAB DESERT LTD</t>
+          <t>COLLIN CARE HOLDINGS LIMITED</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>16461260</t>
+          <t>SC849153</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -4012,12 +4012,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>GROUND MORTGAGE SERVICES LIMITED</t>
+          <t>ALOVER VUBINH LIMITED</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>16461278</t>
+          <t>16462909</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -4050,12 +4050,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>AMARA WELLS LTD</t>
+          <t>INTERA AI HOLDINGS UK LIMITED</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>SC849026</t>
+          <t>16462908</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4088,12 +4088,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>FUNCTION.ALL.OVER LTD</t>
+          <t>CFBUK SECURED FINANCE LTD</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>16461272</t>
+          <t>16462904</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -4126,12 +4126,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>SW2 CONSTRUCTION LIMITED</t>
+          <t>MAKPLAS LTD</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>16461262</t>
+          <t>SC849155</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4164,12 +4164,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>TUK TALENT LTD</t>
+          <t>LIU YUMEI LTD</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>16461265</t>
+          <t>16462901</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -4202,12 +4202,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>KGM CONSTRUCTION LTD</t>
+          <t>LIT BARBERS LTD</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>16461264</t>
+          <t>16462561</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">

</xml_diff>

<commit_message>
Auto update: 2025-05-20 19:11:48
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -516,12 +516,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>YANG HAIJUN LTD</t>
+          <t>CUT N GLOW BEAUTY LIMITED</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16460671</t>
+          <t>16462051</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -554,12 +554,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
+          <t>RAPID FULFILL LTD</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16460503</t>
+          <t>16462586</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -585,19 +585,19 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>THE SPICE INVADERS LTD</t>
+          <t>ASHTOWN INTERVENTION &amp; COMPLETION SERVICES LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16460505</t>
+          <t>SC849120</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -630,12 +630,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DEE BEE TRADING LTD</t>
+          <t>DANDINI PANTOMIMES LIMITED</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16460511</t>
+          <t>16462588</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -668,12 +668,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>INNOVATION MT LTD</t>
+          <t>POINT BREAK 7 LTD</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16460646</t>
+          <t>16462560</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -706,12 +706,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BRANWELL PROJECTS LIMITED</t>
+          <t>TBT KENT LTD</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16460653</t>
+          <t>16462558</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -744,12 +744,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MAYTREE ELITE PROPERTIES LTD</t>
+          <t>ELLAHI PROPERTY HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16460650</t>
+          <t>16462030</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -782,12 +782,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MEDIA WEB PRO LTD</t>
+          <t>SUBLINE LTD</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16460644</t>
+          <t>16462043</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -820,12 +820,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ASPC CONTENT CO LTD</t>
+          <t>HOMELORD T LTD</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16460643</t>
+          <t>16462031</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -858,12 +858,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BLUEPRINT VOYAGE MEDIA COMPANY LIMITED</t>
+          <t>ANITA TECHNOLOGY LTD</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16460649</t>
+          <t>16462036</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -896,12 +896,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SARASI LTD</t>
+          <t>DAILY NOVA LTD</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16460670</t>
+          <t>16462033</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -934,12 +934,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ST PAUL'S COURT DEVELOPMENT LTD</t>
+          <t>VIRTUAL CO. UK LTD</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16460669</t>
+          <t>16460502</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -972,12 +972,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ASSURED LETTINGS AND SALES LTD</t>
+          <t>YANG HAIJUN LTD</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16462049</t>
+          <t>16460671</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1010,12 +1010,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SAMVIV PARTNERS LTD</t>
+          <t>GEOAIR SOLAR LIMITED</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16460672</t>
+          <t>16462052</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1041,19 +1041,19 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>COREMARINE SOLUTIONS CIC</t>
+          <t>CSS BR ASSET LIMITED</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16460663</t>
+          <t>16462021</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1086,12 +1086,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>AMPERSAND MANAGEMENT UK LTD</t>
+          <t>LEMON TREE REAL ESTATE LIMITED</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16460662</t>
+          <t>16462023</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1124,12 +1124,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TRIPLE J HOUSING LTD</t>
+          <t>DARWIN INVEST LTD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16460681</t>
+          <t>16461938</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1162,12 +1162,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>DXI DAILY NECESSITIES CO., LTD.</t>
+          <t>AVIATION TOOL POOLING LLC</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>16460679</t>
+          <t>OE033940</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>registered</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -1200,12 +1200,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PREVENTR ACTIVE FIRE LTD</t>
+          <t>MARTIAL FITNESS (SW) LTD</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16460677</t>
+          <t>16461940</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1238,12 +1238,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>MOUNTAIN SEA SHIP SERVICE CO., LTD</t>
+          <t>JLI CONSTRUCTION LTD</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16460640</t>
+          <t>16461948</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1276,12 +1276,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>T-REX (GUILDFORD) LIMITED</t>
+          <t>IVOLVIA LTD</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>16460637</t>
+          <t>16461947</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1314,12 +1314,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>HOMEASE LTD</t>
+          <t>B AND K FLOORING LIMITED</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16460666</t>
+          <t>16461926</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1352,12 +1352,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>INAYA HEALTHCARE LTD</t>
+          <t>KOMO NAIL &amp; BEAUTY LTD</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16460657</t>
+          <t>16462578</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1390,12 +1390,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>VALLEY SEVEN DEVELOPMENTS LIMITED</t>
+          <t>LANUNE LTD</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16460659</t>
+          <t>16461925</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1428,12 +1428,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>REIGNING MEDIA LIMITED</t>
+          <t>AR BUILDING AND GARDENING SERVICES LTD</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16461275</t>
+          <t>16462581</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1466,12 +1466,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>YANGLIN CHEN LIMITED</t>
+          <t>ECCLES-WOOD LTD</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16461915</t>
+          <t>SC849115</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1504,12 +1504,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CRISPY GLEN LTD</t>
+          <t>DGPI LTD</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>SC849027</t>
+          <t>SC849118</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1535,19 +1535,19 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>GP</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>KGM CONSTRUCTION LTD</t>
+          <t>LIT BARBERS LTD</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16461264</t>
+          <t>16462561</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1580,12 +1580,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>TUK TALENT LTD</t>
+          <t>LIU YUMEI LTD</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16461265</t>
+          <t>16462901</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1618,12 +1618,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>SW2 CONSTRUCTION LIMITED</t>
+          <t>MAKPLAS LTD</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16461262</t>
+          <t>SC849155</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1656,12 +1656,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>FUNCTION.ALL.OVER LTD</t>
+          <t>CFBUK SECURED FINANCE LTD</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16461272</t>
+          <t>16462904</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1694,12 +1694,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>AMARA WELLS LTD</t>
+          <t>INTERA AI HOLDINGS UK LIMITED</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>SC849026</t>
+          <t>16462908</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1732,12 +1732,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>GROUND MORTGAGE SERVICES LIMITED</t>
+          <t>ALOVER VUBINH LIMITED</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>16461278</t>
+          <t>16462909</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1770,12 +1770,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>MUNCHIES KEBAB DESERT LTD</t>
+          <t>COLLIN CARE HOLDINGS LIMITED</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16461260</t>
+          <t>SC849153</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1808,12 +1808,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>4D CAPITAL PROPCO (44) LIMITED</t>
+          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16461269</t>
+          <t>16462880</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1846,12 +1846,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>MIRE LTD</t>
+          <t>CAMPBELL &amp; DOIG LTD</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16461902</t>
+          <t>SC849151</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1884,12 +1884,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>GIG32 LIMITED</t>
+          <t>3 MORDEN CLIFF LTD</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16461898</t>
+          <t>16462875</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1922,12 +1922,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>LEADALE CITY LTD</t>
+          <t>AFROSCOT VENTURES LTD</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16461899</t>
+          <t>16462878</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1953,19 +1953,19 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>48 CONEY STREET LIMITED</t>
+          <t>BOWEN BUSINESS LTD</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>16461897</t>
+          <t>16462877</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1998,12 +1998,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>FND MOTORS LIMITED</t>
+          <t>PAMIR MECHANICAL LTD</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16461900</t>
+          <t>16462876</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2036,12 +2036,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ALI SHOP LTD</t>
+          <t>BLITHFIELD PROPERTY SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16461895</t>
+          <t>16462888</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2074,12 +2074,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>KASZCZUK LTD</t>
+          <t>WIMWA LTD</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16461901</t>
+          <t>16462889</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2112,12 +2112,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>AMPLIFORTH CONSULTING LIMITED</t>
+          <t>GASSINGITUP LTD</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16461904</t>
+          <t>16462883</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2150,12 +2150,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>DDPT HOLDINGS LIMITED</t>
+          <t>MAYROL UK LIMITED</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16461906</t>
+          <t>16462870</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2188,12 +2188,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>GLOBAL CREW LTD</t>
+          <t>MANPOD LTD</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16461905</t>
+          <t>16462873</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2226,12 +2226,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>PRIME ATHLETIC CO LTD</t>
+          <t>JWP INDUSTRIES LIMITED</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>16461911</t>
+          <t>16462872</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2264,12 +2264,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>TMS ASSETS LTD</t>
+          <t>LEW-BUD LTD</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>16461913</t>
+          <t>16462565</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2302,12 +2302,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>LANYNSEN HOUSE LTD</t>
+          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16461918</t>
+          <t>SC849117</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2333,19 +2333,19 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>LEAD INFO LTD</t>
+          <t>THE FISH SHOP 17 LTD</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>16461919</t>
+          <t>16461921</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2416,12 +2416,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>THE FISH SHOP 17 LTD</t>
+          <t>LEAD INFO LTD</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16461921</t>
+          <t>16461919</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2454,12 +2454,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>KOMO NAIL &amp; BEAUTY LTD</t>
+          <t>VALLEY SEVEN DEVELOPMENTS LIMITED</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>16462578</t>
+          <t>16460659</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2492,12 +2492,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>B AND K FLOORING LIMITED</t>
+          <t>HOMEASE LTD</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>16461926</t>
+          <t>16460666</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2530,12 +2530,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>IVOLVIA LTD</t>
+          <t>T-REX (GUILDFORD) LIMITED</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>16461947</t>
+          <t>16460637</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2568,12 +2568,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>JLI CONSTRUCTION LTD</t>
+          <t>MOUNTAIN SEA SHIP SERVICE CO., LTD</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>16461948</t>
+          <t>16460640</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2606,12 +2606,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>MARTIAL FITNESS (SW) LTD</t>
+          <t>PREVENTR ACTIVE FIRE LTD</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>16461940</t>
+          <t>16460677</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2644,12 +2644,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>AVIATION TOOL POOLING LLC</t>
+          <t>DXI DAILY NECESSITIES CO., LTD.</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>OE033940</t>
+          <t>16460679</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2659,7 +2659,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>active</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -2682,12 +2682,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>DARWIN INVEST LTD</t>
+          <t>TRIPLE J HOUSING LTD</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16461938</t>
+          <t>16460681</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2720,12 +2720,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>LEMON TREE REAL ESTATE LIMITED</t>
+          <t>AMPERSAND MANAGEMENT UK LTD</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16462023</t>
+          <t>16460662</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2758,12 +2758,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>CSS BR ASSET LIMITED</t>
+          <t>COREMARINE SOLUTIONS CIC</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>16462021</t>
+          <t>16460663</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2796,12 +2796,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>GEOAIR SOLAR LIMITED</t>
+          <t>SAMVIV PARTNERS LTD</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16462052</t>
+          <t>16460672</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2827,19 +2827,19 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>VIRTUAL CO. UK LTD</t>
+          <t>ASSURED LETTINGS AND SALES LTD</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>16460502</t>
+          <t>16462049</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2872,12 +2872,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>CUT N GLOW BEAUTY LIMITED</t>
+          <t>ST PAUL'S COURT DEVELOPMENT LTD</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>16462051</t>
+          <t>16460669</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2910,12 +2910,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>DAILY NOVA LTD</t>
+          <t>SARASI LTD</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>16462033</t>
+          <t>16460670</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2948,12 +2948,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>ANITA TECHNOLOGY LTD</t>
+          <t>BLUEPRINT VOYAGE MEDIA COMPANY LIMITED</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>16462036</t>
+          <t>16460649</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2986,12 +2986,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>HOMELORD T LTD</t>
+          <t>ASPC CONTENT CO LTD</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>16462031</t>
+          <t>16460643</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3024,12 +3024,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>SUBLINE LTD</t>
+          <t>MEDIA WEB PRO LTD</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>16462043</t>
+          <t>16460644</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3062,12 +3062,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>ELLAHI PROPERTY HOLDINGS LTD</t>
+          <t>MAYTREE ELITE PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>16462030</t>
+          <t>16460650</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3100,12 +3100,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>TBT KENT LTD</t>
+          <t>BRANWELL PROJECTS LIMITED</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>16462558</t>
+          <t>16460653</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3138,12 +3138,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>POINT BREAK 7 LTD</t>
+          <t>INNOVATION MT LTD</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16462560</t>
+          <t>16460646</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3176,12 +3176,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>DANDINI PANTOMIMES LIMITED</t>
+          <t>DEE BEE TRADING LTD</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16462588</t>
+          <t>16460511</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3214,12 +3214,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>ASHTOWN INTERVENTION &amp; COMPLETION SERVICES LTD</t>
+          <t>THE SPICE INVADERS LTD</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>SC849120</t>
+          <t>16460505</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3252,12 +3252,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>RAPID FULFILL LTD</t>
+          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16462586</t>
+          <t>16460503</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3283,19 +3283,19 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>LANUNE LTD</t>
+          <t>INAYA HEALTHCARE LTD</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>16461925</t>
+          <t>16460657</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3328,12 +3328,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>AR BUILDING AND GARDENING SERVICES LTD</t>
+          <t>REIGNING MEDIA LIMITED</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>16462581</t>
+          <t>16461275</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3366,12 +3366,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>ECCLES-WOOD LTD</t>
+          <t>LANYNSEN HOUSE LTD</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>SC849115</t>
+          <t>16461918</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3404,12 +3404,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>DGPI LTD</t>
+          <t>YANGLIN CHEN LIMITED</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>SC849118</t>
+          <t>16461915</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3435,19 +3435,19 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
+          <t>TMS ASSETS LTD</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>SC849117</t>
+          <t>16461913</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3473,19 +3473,19 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>LEW-BUD LTD</t>
+          <t>PRIME ATHLETIC CO LTD</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>16462565</t>
+          <t>16461911</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3518,12 +3518,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>JWP INDUSTRIES LIMITED</t>
+          <t>GLOBAL CREW LTD</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>16462872</t>
+          <t>16461905</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3556,12 +3556,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>MANPOD LTD</t>
+          <t>DDPT HOLDINGS LIMITED</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>16462873</t>
+          <t>16461906</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3594,12 +3594,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>MAYROL UK LIMITED</t>
+          <t>AMPLIFORTH CONSULTING LIMITED</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>16462870</t>
+          <t>16461904</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3632,12 +3632,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>GASSINGITUP LTD</t>
+          <t>KASZCZUK LTD</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>16462883</t>
+          <t>16461901</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3670,12 +3670,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>WIMWA LTD</t>
+          <t>ALI SHOP LTD</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>16462889</t>
+          <t>16461895</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3708,12 +3708,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>BLITHFIELD PROPERTY SOLUTIONS LTD</t>
+          <t>FND MOTORS LIMITED</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>16462888</t>
+          <t>16461900</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3746,12 +3746,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>PAMIR MECHANICAL LTD</t>
+          <t>48 CONEY STREET LIMITED</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>16462876</t>
+          <t>16461897</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3784,12 +3784,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>BOWEN BUSINESS LTD</t>
+          <t>LEADALE CITY LTD</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>16462877</t>
+          <t>16461899</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3822,12 +3822,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>AFROSCOT VENTURES LTD</t>
+          <t>GIG32 LIMITED</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16462878</t>
+          <t>16461898</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3853,19 +3853,19 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>3 MORDEN CLIFF LTD</t>
+          <t>MIRE LTD</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>16462875</t>
+          <t>16461902</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3898,12 +3898,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>CAMPBELL &amp; DOIG LTD</t>
+          <t>4D CAPITAL PROPCO (44) LIMITED</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>SC849151</t>
+          <t>16461269</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3929,19 +3929,19 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
+          <t>MUNCHIES KEBAB DESERT LTD</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>16462880</t>
+          <t>16461260</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3967,19 +3967,19 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>COLLIN CARE HOLDINGS LIMITED</t>
+          <t>GROUND MORTGAGE SERVICES LIMITED</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>SC849153</t>
+          <t>16461278</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -4012,12 +4012,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>ALOVER VUBINH LIMITED</t>
+          <t>AMARA WELLS LTD</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>16462909</t>
+          <t>SC849026</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -4050,12 +4050,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>INTERA AI HOLDINGS UK LIMITED</t>
+          <t>FUNCTION.ALL.OVER LTD</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>16462908</t>
+          <t>16461272</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4088,12 +4088,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>CFBUK SECURED FINANCE LTD</t>
+          <t>SW2 CONSTRUCTION LIMITED</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>16462904</t>
+          <t>16461262</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -4126,12 +4126,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>MAKPLAS LTD</t>
+          <t>TUK TALENT LTD</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>SC849155</t>
+          <t>16461265</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4164,12 +4164,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>LIU YUMEI LTD</t>
+          <t>KGM CONSTRUCTION LTD</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>16462901</t>
+          <t>16461264</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -4202,12 +4202,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>LIT BARBERS LTD</t>
+          <t>CRISPY GLEN LTD</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>16462561</t>
+          <t>SC849027</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">

</xml_diff>

<commit_message>
Auto update: 2025-05-20 19:20:14
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -516,12 +516,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CUT N GLOW BEAUTY LIMITED</t>
+          <t>ST PAUL'S COURT DEVELOPMENT LTD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16462051</t>
+          <t>16460669</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -554,12 +554,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>RAPID FULFILL LTD</t>
+          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16462586</t>
+          <t>16460503</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -585,19 +585,19 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ASHTOWN INTERVENTION &amp; COMPLETION SERVICES LTD</t>
+          <t>THE SPICE INVADERS LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SC849120</t>
+          <t>16460505</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -630,12 +630,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DANDINI PANTOMIMES LIMITED</t>
+          <t>DEE BEE TRADING LTD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16462588</t>
+          <t>16460511</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -668,12 +668,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>POINT BREAK 7 LTD</t>
+          <t>INNOVATION MT LTD</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16462560</t>
+          <t>16460646</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -706,12 +706,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TBT KENT LTD</t>
+          <t>BRANWELL PROJECTS LIMITED</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16462558</t>
+          <t>16460653</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -744,12 +744,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ELLAHI PROPERTY HOLDINGS LTD</t>
+          <t>MAYTREE ELITE PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16462030</t>
+          <t>16460650</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -782,12 +782,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>SUBLINE LTD</t>
+          <t>MEDIA WEB PRO LTD</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16462043</t>
+          <t>16460644</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -820,12 +820,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>HOMELORD T LTD</t>
+          <t>ASPC CONTENT CO LTD</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16462031</t>
+          <t>16460643</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -858,12 +858,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ANITA TECHNOLOGY LTD</t>
+          <t>BLUEPRINT VOYAGE MEDIA COMPANY LIMITED</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16462036</t>
+          <t>16460649</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -896,12 +896,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>DAILY NOVA LTD</t>
+          <t>SARASI LTD</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16462033</t>
+          <t>16460670</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -934,12 +934,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>VIRTUAL CO. UK LTD</t>
+          <t>ASSURED LETTINGS AND SALES LTD</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16460502</t>
+          <t>16462049</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -972,12 +972,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>YANG HAIJUN LTD</t>
+          <t>CUT N GLOW BEAUTY LIMITED</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16460671</t>
+          <t>16462051</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1010,12 +1010,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GEOAIR SOLAR LIMITED</t>
+          <t>SAMVIV PARTNERS LTD</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16462052</t>
+          <t>16460672</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1041,19 +1041,19 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CSS BR ASSET LIMITED</t>
+          <t>COREMARINE SOLUTIONS CIC</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16462021</t>
+          <t>16460663</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1086,12 +1086,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>LEMON TREE REAL ESTATE LIMITED</t>
+          <t>AMPERSAND MANAGEMENT UK LTD</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16462023</t>
+          <t>16460662</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1124,12 +1124,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>DARWIN INVEST LTD</t>
+          <t>TRIPLE J HOUSING LTD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16461938</t>
+          <t>16460681</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1162,12 +1162,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AVIATION TOOL POOLING LLC</t>
+          <t>DXI DAILY NECESSITIES CO., LTD.</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>OE033940</t>
+          <t>16460679</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>active</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -1200,12 +1200,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>MARTIAL FITNESS (SW) LTD</t>
+          <t>PREVENTR ACTIVE FIRE LTD</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16461940</t>
+          <t>16460677</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1238,12 +1238,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>JLI CONSTRUCTION LTD</t>
+          <t>MOUNTAIN SEA SHIP SERVICE CO., LTD</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16461948</t>
+          <t>16460640</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1276,12 +1276,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>IVOLVIA LTD</t>
+          <t>T-REX (GUILDFORD) LIMITED</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>16461947</t>
+          <t>16460637</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1314,12 +1314,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>B AND K FLOORING LIMITED</t>
+          <t>HOMEASE LTD</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16461926</t>
+          <t>16460666</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1352,12 +1352,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>KOMO NAIL &amp; BEAUTY LTD</t>
+          <t>VALLEY SEVEN DEVELOPMENTS LIMITED</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16462578</t>
+          <t>16460659</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1390,12 +1390,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>LANUNE LTD</t>
+          <t>INAYA HEALTHCARE LTD</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16461925</t>
+          <t>16460657</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1428,12 +1428,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>AR BUILDING AND GARDENING SERVICES LTD</t>
+          <t>REIGNING MEDIA LIMITED</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16462581</t>
+          <t>16461275</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1466,12 +1466,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ECCLES-WOOD LTD</t>
+          <t>LANYNSEN HOUSE LTD</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>SC849115</t>
+          <t>16461918</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1504,12 +1504,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>DGPI LTD</t>
+          <t>YANGLIN CHEN LIMITED</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>SC849118</t>
+          <t>16461915</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1535,19 +1535,19 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>LIT BARBERS LTD</t>
+          <t>CRISPY GLEN LTD</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16462561</t>
+          <t>SC849027</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1580,12 +1580,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>LIU YUMEI LTD</t>
+          <t>KGM CONSTRUCTION LTD</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16462901</t>
+          <t>16461264</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1618,12 +1618,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>MAKPLAS LTD</t>
+          <t>TUK TALENT LTD</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>SC849155</t>
+          <t>16461265</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1656,12 +1656,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CFBUK SECURED FINANCE LTD</t>
+          <t>SW2 CONSTRUCTION LIMITED</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16462904</t>
+          <t>16461262</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1694,12 +1694,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>INTERA AI HOLDINGS UK LIMITED</t>
+          <t>FUNCTION.ALL.OVER LTD</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16462908</t>
+          <t>16461272</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1732,12 +1732,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ALOVER VUBINH LIMITED</t>
+          <t>AMARA WELLS LTD</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>16462909</t>
+          <t>SC849026</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1770,12 +1770,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>COLLIN CARE HOLDINGS LIMITED</t>
+          <t>GROUND MORTGAGE SERVICES LIMITED</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SC849153</t>
+          <t>16461278</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1808,12 +1808,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
+          <t>MUNCHIES KEBAB DESERT LTD</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16462880</t>
+          <t>16461260</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1839,19 +1839,19 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CAMPBELL &amp; DOIG LTD</t>
+          <t>4D CAPITAL PROPCO (44) LIMITED</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>SC849151</t>
+          <t>16461269</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1877,19 +1877,19 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>3 MORDEN CLIFF LTD</t>
+          <t>MIRE LTD</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16462875</t>
+          <t>16461902</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1922,12 +1922,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>AFROSCOT VENTURES LTD</t>
+          <t>GIG32 LIMITED</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16462878</t>
+          <t>16461898</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1953,19 +1953,19 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>BOWEN BUSINESS LTD</t>
+          <t>LEADALE CITY LTD</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>16462877</t>
+          <t>16461899</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1998,12 +1998,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>PAMIR MECHANICAL LTD</t>
+          <t>48 CONEY STREET LIMITED</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16462876</t>
+          <t>16461897</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2036,12 +2036,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>BLITHFIELD PROPERTY SOLUTIONS LTD</t>
+          <t>FND MOTORS LIMITED</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16462888</t>
+          <t>16461900</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2074,12 +2074,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>WIMWA LTD</t>
+          <t>ALI SHOP LTD</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16462889</t>
+          <t>16461895</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2112,12 +2112,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>GASSINGITUP LTD</t>
+          <t>KASZCZUK LTD</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16462883</t>
+          <t>16461901</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2150,12 +2150,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>MAYROL UK LIMITED</t>
+          <t>AMPLIFORTH CONSULTING LIMITED</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16462870</t>
+          <t>16461904</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2188,12 +2188,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>MANPOD LTD</t>
+          <t>DDPT HOLDINGS LIMITED</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16462873</t>
+          <t>16461906</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2226,12 +2226,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>JWP INDUSTRIES LIMITED</t>
+          <t>GLOBAL CREW LTD</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>16462872</t>
+          <t>16461905</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2264,12 +2264,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>LEW-BUD LTD</t>
+          <t>PRIME ATHLETIC CO LTD</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>16462565</t>
+          <t>16461911</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2302,12 +2302,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
+          <t>TMS ASSETS LTD</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SC849117</t>
+          <t>16461913</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2333,19 +2333,19 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>THE FISH SHOP 17 LTD</t>
+          <t>LEAD INFO LTD</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>16461921</t>
+          <t>16461919</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2416,12 +2416,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>LEAD INFO LTD</t>
+          <t>THE FISH SHOP 17 LTD</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16461919</t>
+          <t>16461921</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2454,12 +2454,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>VALLEY SEVEN DEVELOPMENTS LIMITED</t>
+          <t>LANUNE LTD</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>16460659</t>
+          <t>16461925</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2492,12 +2492,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>HOMEASE LTD</t>
+          <t>B AND K FLOORING LIMITED</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>16460666</t>
+          <t>16461926</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2530,12 +2530,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>T-REX (GUILDFORD) LIMITED</t>
+          <t>IVOLVIA LTD</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>16460637</t>
+          <t>16461947</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2568,12 +2568,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>MOUNTAIN SEA SHIP SERVICE CO., LTD</t>
+          <t>JLI CONSTRUCTION LTD</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>16460640</t>
+          <t>16461948</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2606,12 +2606,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>PREVENTR ACTIVE FIRE LTD</t>
+          <t>MARTIAL FITNESS (SW) LTD</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>16460677</t>
+          <t>16461940</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2644,12 +2644,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>DXI DAILY NECESSITIES CO., LTD.</t>
+          <t>AVIATION TOOL POOLING LLC</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>16460679</t>
+          <t>OE033940</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2659,7 +2659,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>registered</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -2682,12 +2682,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>TRIPLE J HOUSING LTD</t>
+          <t>DARWIN INVEST LTD</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16460681</t>
+          <t>16461938</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2720,12 +2720,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>AMPERSAND MANAGEMENT UK LTD</t>
+          <t>LEMON TREE REAL ESTATE LIMITED</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16460662</t>
+          <t>16462023</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2758,12 +2758,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>COREMARINE SOLUTIONS CIC</t>
+          <t>CSS BR ASSET LIMITED</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>16460663</t>
+          <t>16462021</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2796,12 +2796,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>SAMVIV PARTNERS LTD</t>
+          <t>GEOAIR SOLAR LIMITED</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16460672</t>
+          <t>16462052</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2827,19 +2827,19 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>ASSURED LETTINGS AND SALES LTD</t>
+          <t>YANG HAIJUN LTD</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>16462049</t>
+          <t>16460671</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2872,12 +2872,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>ST PAUL'S COURT DEVELOPMENT LTD</t>
+          <t>VIRTUAL CO. UK LTD</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>16460669</t>
+          <t>16460502</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2910,12 +2910,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>SARASI LTD</t>
+          <t>DAILY NOVA LTD</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>16460670</t>
+          <t>16462033</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2948,12 +2948,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>BLUEPRINT VOYAGE MEDIA COMPANY LIMITED</t>
+          <t>ANITA TECHNOLOGY LTD</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>16460649</t>
+          <t>16462036</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2986,12 +2986,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>ASPC CONTENT CO LTD</t>
+          <t>HOMELORD T LTD</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>16460643</t>
+          <t>16462031</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3024,12 +3024,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>MEDIA WEB PRO LTD</t>
+          <t>SUBLINE LTD</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>16460644</t>
+          <t>16462043</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3062,12 +3062,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>MAYTREE ELITE PROPERTIES LTD</t>
+          <t>ELLAHI PROPERTY HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>16460650</t>
+          <t>16462030</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3100,12 +3100,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>BRANWELL PROJECTS LIMITED</t>
+          <t>TBT KENT LTD</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>16460653</t>
+          <t>16462558</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3138,12 +3138,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>INNOVATION MT LTD</t>
+          <t>POINT BREAK 7 LTD</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16460646</t>
+          <t>16462560</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3176,12 +3176,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>DEE BEE TRADING LTD</t>
+          <t>DANDINI PANTOMIMES LIMITED</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16460511</t>
+          <t>16462588</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3214,12 +3214,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>THE SPICE INVADERS LTD</t>
+          <t>ASHTOWN INTERVENTION &amp; COMPLETION SERVICES LTD</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>16460505</t>
+          <t>SC849120</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3252,12 +3252,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
+          <t>RAPID FULFILL LTD</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16460503</t>
+          <t>16462586</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3283,19 +3283,19 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>INAYA HEALTHCARE LTD</t>
+          <t>KOMO NAIL &amp; BEAUTY LTD</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>16460657</t>
+          <t>16462578</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3328,12 +3328,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>REIGNING MEDIA LIMITED</t>
+          <t>AR BUILDING AND GARDENING SERVICES LTD</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>16461275</t>
+          <t>16462581</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3366,12 +3366,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>LANYNSEN HOUSE LTD</t>
+          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>16461918</t>
+          <t>SC849117</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3397,19 +3397,19 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>YANGLIN CHEN LIMITED</t>
+          <t>ECCLES-WOOD LTD</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>16461915</t>
+          <t>SC849115</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3442,12 +3442,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>TMS ASSETS LTD</t>
+          <t>LEW-BUD LTD</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>16461913</t>
+          <t>16462565</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3480,12 +3480,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>PRIME ATHLETIC CO LTD</t>
+          <t>JWP INDUSTRIES LIMITED</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>16461911</t>
+          <t>16462872</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3518,12 +3518,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>GLOBAL CREW LTD</t>
+          <t>MANPOD LTD</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>16461905</t>
+          <t>16462873</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3556,12 +3556,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>DDPT HOLDINGS LIMITED</t>
+          <t>MAYROL UK LIMITED</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>16461906</t>
+          <t>16462870</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3594,12 +3594,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>AMPLIFORTH CONSULTING LIMITED</t>
+          <t>GASSINGITUP LTD</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>16461904</t>
+          <t>16462883</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3632,12 +3632,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>KASZCZUK LTD</t>
+          <t>WIMWA LTD</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>16461901</t>
+          <t>16462889</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3670,12 +3670,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>ALI SHOP LTD</t>
+          <t>BLITHFIELD PROPERTY SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>16461895</t>
+          <t>16462888</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3708,12 +3708,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>FND MOTORS LIMITED</t>
+          <t>PAMIR MECHANICAL LTD</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>16461900</t>
+          <t>16462876</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3746,12 +3746,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>48 CONEY STREET LIMITED</t>
+          <t>BOWEN BUSINESS LTD</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>16461897</t>
+          <t>16462877</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3784,12 +3784,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>LEADALE CITY LTD</t>
+          <t>AFROSCOT VENTURES LTD</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>16461899</t>
+          <t>16462878</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3815,19 +3815,19 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>GIG32 LIMITED</t>
+          <t>3 MORDEN CLIFF LTD</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16461898</t>
+          <t>16462875</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3860,12 +3860,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>MIRE LTD</t>
+          <t>CAMPBELL &amp; DOIG LTD</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>16461902</t>
+          <t>SC849151</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3898,12 +3898,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>4D CAPITAL PROPCO (44) LIMITED</t>
+          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>16461269</t>
+          <t>16462880</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3936,12 +3936,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>MUNCHIES KEBAB DESERT LTD</t>
+          <t>COLLIN CARE HOLDINGS LIMITED</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>16461260</t>
+          <t>SC849153</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3974,12 +3974,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>GROUND MORTGAGE SERVICES LIMITED</t>
+          <t>ALOVER VUBINH LIMITED</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>16461278</t>
+          <t>16462909</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -4012,12 +4012,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>AMARA WELLS LTD</t>
+          <t>INTERA AI HOLDINGS UK LIMITED</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>SC849026</t>
+          <t>16462908</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -4050,12 +4050,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>FUNCTION.ALL.OVER LTD</t>
+          <t>CFBUK SECURED FINANCE LTD</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>16461272</t>
+          <t>16462904</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4088,12 +4088,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>SW2 CONSTRUCTION LIMITED</t>
+          <t>MAKPLAS LTD</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>16461262</t>
+          <t>SC849155</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -4126,12 +4126,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>TUK TALENT LTD</t>
+          <t>LIU YUMEI LTD</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>16461265</t>
+          <t>16462901</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4164,12 +4164,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>KGM CONSTRUCTION LTD</t>
+          <t>LIT BARBERS LTD</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>16461264</t>
+          <t>16462561</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -4202,12 +4202,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>CRISPY GLEN LTD</t>
+          <t>DGPI LTD</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>SC849027</t>
+          <t>SC849118</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -4233,7 +4233,7 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>GP</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update: 2025-05-20 19:21:54
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -516,12 +516,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ST PAUL'S COURT DEVELOPMENT LTD</t>
+          <t>VIRTUAL CO. UK LTD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16460669</t>
+          <t>16460502</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -554,12 +554,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
+          <t>RAPID FULFILL LTD</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16460503</t>
+          <t>16462586</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -585,19 +585,19 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>THE SPICE INVADERS LTD</t>
+          <t>ASHTOWN INTERVENTION &amp; COMPLETION SERVICES LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16460505</t>
+          <t>SC849120</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -630,12 +630,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DEE BEE TRADING LTD</t>
+          <t>DANDINI PANTOMIMES LIMITED</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16460511</t>
+          <t>16462588</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -668,12 +668,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>INNOVATION MT LTD</t>
+          <t>POINT BREAK 7 LTD</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16460646</t>
+          <t>16462560</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -706,12 +706,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BRANWELL PROJECTS LIMITED</t>
+          <t>TBT KENT LTD</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16460653</t>
+          <t>16462558</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -744,12 +744,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MAYTREE ELITE PROPERTIES LTD</t>
+          <t>ELLAHI PROPERTY HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16460650</t>
+          <t>16462030</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -782,12 +782,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MEDIA WEB PRO LTD</t>
+          <t>SUBLINE LTD</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16460644</t>
+          <t>16462043</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -820,12 +820,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ASPC CONTENT CO LTD</t>
+          <t>HOMELORD T LTD</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16460643</t>
+          <t>16462031</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -858,12 +858,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BLUEPRINT VOYAGE MEDIA COMPANY LIMITED</t>
+          <t>ANITA TECHNOLOGY LTD</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16460649</t>
+          <t>16462036</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -896,12 +896,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SARASI LTD</t>
+          <t>DAILY NOVA LTD</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16460670</t>
+          <t>16462033</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -934,12 +934,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ASSURED LETTINGS AND SALES LTD</t>
+          <t>YANG HAIJUN LTD</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16462049</t>
+          <t>16460671</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -972,12 +972,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CUT N GLOW BEAUTY LIMITED</t>
+          <t>ST PAUL'S COURT DEVELOPMENT LTD</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16462051</t>
+          <t>16460669</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1010,12 +1010,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SAMVIV PARTNERS LTD</t>
+          <t>GEOAIR SOLAR LIMITED</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16460672</t>
+          <t>16462052</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1041,19 +1041,19 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>COREMARINE SOLUTIONS CIC</t>
+          <t>CSS BR ASSET LIMITED</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16460663</t>
+          <t>16462021</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1086,12 +1086,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>AMPERSAND MANAGEMENT UK LTD</t>
+          <t>LEMON TREE REAL ESTATE LIMITED</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16460662</t>
+          <t>16462023</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1124,12 +1124,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TRIPLE J HOUSING LTD</t>
+          <t>DARWIN INVEST LTD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16460681</t>
+          <t>16461938</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1162,12 +1162,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>DXI DAILY NECESSITIES CO., LTD.</t>
+          <t>AVIATION TOOL POOLING LLC</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>16460679</t>
+          <t>OE033940</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>registered</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -1200,12 +1200,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PREVENTR ACTIVE FIRE LTD</t>
+          <t>MARTIAL FITNESS (SW) LTD</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16460677</t>
+          <t>16461940</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1238,12 +1238,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>MOUNTAIN SEA SHIP SERVICE CO., LTD</t>
+          <t>JLI CONSTRUCTION LTD</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16460640</t>
+          <t>16461948</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1276,12 +1276,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>T-REX (GUILDFORD) LIMITED</t>
+          <t>IVOLVIA LTD</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>16460637</t>
+          <t>16461947</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1314,12 +1314,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>HOMEASE LTD</t>
+          <t>B AND K FLOORING LIMITED</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16460666</t>
+          <t>16461926</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1352,12 +1352,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>VALLEY SEVEN DEVELOPMENTS LIMITED</t>
+          <t>LANUNE LTD</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16460659</t>
+          <t>16461925</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1390,12 +1390,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>INAYA HEALTHCARE LTD</t>
+          <t>KOMO NAIL &amp; BEAUTY LTD</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16460657</t>
+          <t>16462578</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1428,12 +1428,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>REIGNING MEDIA LIMITED</t>
+          <t>AR BUILDING AND GARDENING SERVICES LTD</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16461275</t>
+          <t>16462581</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1466,12 +1466,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>LANYNSEN HOUSE LTD</t>
+          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16461918</t>
+          <t>SC849117</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1497,19 +1497,19 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>YANGLIN CHEN LIMITED</t>
+          <t>ECCLES-WOOD LTD</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16461915</t>
+          <t>SC849115</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1542,12 +1542,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CRISPY GLEN LTD</t>
+          <t>DGPI LTD</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>SC849027</t>
+          <t>SC849118</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1573,19 +1573,19 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>GP</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>KGM CONSTRUCTION LTD</t>
+          <t>LIT BARBERS LTD</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16461264</t>
+          <t>16462561</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1618,12 +1618,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>TUK TALENT LTD</t>
+          <t>LIU YUMEI LTD</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16461265</t>
+          <t>16462901</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1656,12 +1656,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SW2 CONSTRUCTION LIMITED</t>
+          <t>MAKPLAS LTD</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16461262</t>
+          <t>SC849155</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1694,12 +1694,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>FUNCTION.ALL.OVER LTD</t>
+          <t>CFBUK SECURED FINANCE LTD</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16461272</t>
+          <t>16462904</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1732,12 +1732,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>AMARA WELLS LTD</t>
+          <t>INTERA AI HOLDINGS UK LIMITED</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>SC849026</t>
+          <t>16462908</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1770,12 +1770,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>GROUND MORTGAGE SERVICES LIMITED</t>
+          <t>ALOVER VUBINH LIMITED</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16461278</t>
+          <t>16462909</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1808,12 +1808,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>MUNCHIES KEBAB DESERT LTD</t>
+          <t>COLLIN CARE HOLDINGS LIMITED</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16461260</t>
+          <t>SC849153</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1846,12 +1846,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>4D CAPITAL PROPCO (44) LIMITED</t>
+          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16461269</t>
+          <t>16462880</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1884,12 +1884,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>MIRE LTD</t>
+          <t>CAMPBELL &amp; DOIG LTD</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16461902</t>
+          <t>SC849151</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1922,12 +1922,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>GIG32 LIMITED</t>
+          <t>3 MORDEN CLIFF LTD</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16461898</t>
+          <t>16462875</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1960,12 +1960,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>LEADALE CITY LTD</t>
+          <t>AFROSCOT VENTURES LTD</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>16461899</t>
+          <t>16462878</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1991,19 +1991,19 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>48 CONEY STREET LIMITED</t>
+          <t>BOWEN BUSINESS LTD</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16461897</t>
+          <t>16462877</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2036,12 +2036,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>FND MOTORS LIMITED</t>
+          <t>PAMIR MECHANICAL LTD</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16461900</t>
+          <t>16462876</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2074,12 +2074,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ALI SHOP LTD</t>
+          <t>BLITHFIELD PROPERTY SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16461895</t>
+          <t>16462888</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2112,12 +2112,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>KASZCZUK LTD</t>
+          <t>WIMWA LTD</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16461901</t>
+          <t>16462889</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2150,12 +2150,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>AMPLIFORTH CONSULTING LIMITED</t>
+          <t>GASSINGITUP LTD</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16461904</t>
+          <t>16462883</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2188,12 +2188,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>DDPT HOLDINGS LIMITED</t>
+          <t>MAYROL UK LIMITED</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16461906</t>
+          <t>16462870</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2226,12 +2226,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>GLOBAL CREW LTD</t>
+          <t>MANPOD LTD</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>16461905</t>
+          <t>16462873</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2264,12 +2264,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>PRIME ATHLETIC CO LTD</t>
+          <t>JWP INDUSTRIES LIMITED</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>16461911</t>
+          <t>16462872</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2302,12 +2302,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>TMS ASSETS LTD</t>
+          <t>LEW-BUD LTD</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16461913</t>
+          <t>16462565</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2340,12 +2340,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>LEAD INFO LTD</t>
+          <t>THE FISH SHOP 17 LTD</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>16461919</t>
+          <t>16461921</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2416,12 +2416,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>THE FISH SHOP 17 LTD</t>
+          <t>LEAD INFO LTD</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16461921</t>
+          <t>16461919</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2454,12 +2454,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>LANUNE LTD</t>
+          <t>INAYA HEALTHCARE LTD</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>16461925</t>
+          <t>16460657</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2492,12 +2492,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>B AND K FLOORING LIMITED</t>
+          <t>HOMEASE LTD</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>16461926</t>
+          <t>16460666</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2530,12 +2530,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>IVOLVIA LTD</t>
+          <t>T-REX (GUILDFORD) LIMITED</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>16461947</t>
+          <t>16460637</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2568,12 +2568,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>JLI CONSTRUCTION LTD</t>
+          <t>MOUNTAIN SEA SHIP SERVICE CO., LTD</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>16461948</t>
+          <t>16460640</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2606,12 +2606,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>MARTIAL FITNESS (SW) LTD</t>
+          <t>PREVENTR ACTIVE FIRE LTD</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>16461940</t>
+          <t>16460677</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2644,12 +2644,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>AVIATION TOOL POOLING LLC</t>
+          <t>DXI DAILY NECESSITIES CO., LTD.</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>OE033940</t>
+          <t>16460679</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2659,7 +2659,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>active</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -2682,12 +2682,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>DARWIN INVEST LTD</t>
+          <t>TRIPLE J HOUSING LTD</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16461938</t>
+          <t>16460681</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2720,12 +2720,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>LEMON TREE REAL ESTATE LIMITED</t>
+          <t>AMPERSAND MANAGEMENT UK LTD</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16462023</t>
+          <t>16460662</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2758,12 +2758,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>CSS BR ASSET LIMITED</t>
+          <t>COREMARINE SOLUTIONS CIC</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>16462021</t>
+          <t>16460663</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2796,12 +2796,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>GEOAIR SOLAR LIMITED</t>
+          <t>SAMVIV PARTNERS LTD</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16462052</t>
+          <t>16460672</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2827,19 +2827,19 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>YANG HAIJUN LTD</t>
+          <t>CUT N GLOW BEAUTY LIMITED</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>16460671</t>
+          <t>16462051</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2872,12 +2872,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>VIRTUAL CO. UK LTD</t>
+          <t>ASSURED LETTINGS AND SALES LTD</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>16460502</t>
+          <t>16462049</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2910,12 +2910,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>DAILY NOVA LTD</t>
+          <t>SARASI LTD</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>16462033</t>
+          <t>16460670</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2948,12 +2948,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>ANITA TECHNOLOGY LTD</t>
+          <t>BLUEPRINT VOYAGE MEDIA COMPANY LIMITED</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>16462036</t>
+          <t>16460649</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2986,12 +2986,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>HOMELORD T LTD</t>
+          <t>ASPC CONTENT CO LTD</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>16462031</t>
+          <t>16460643</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3024,12 +3024,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>SUBLINE LTD</t>
+          <t>MEDIA WEB PRO LTD</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>16462043</t>
+          <t>16460644</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3062,12 +3062,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>ELLAHI PROPERTY HOLDINGS LTD</t>
+          <t>MAYTREE ELITE PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>16462030</t>
+          <t>16460650</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3100,12 +3100,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>TBT KENT LTD</t>
+          <t>BRANWELL PROJECTS LIMITED</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>16462558</t>
+          <t>16460653</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3138,12 +3138,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>POINT BREAK 7 LTD</t>
+          <t>INNOVATION MT LTD</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16462560</t>
+          <t>16460646</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3176,12 +3176,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>DANDINI PANTOMIMES LIMITED</t>
+          <t>DEE BEE TRADING LTD</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16462588</t>
+          <t>16460511</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3214,12 +3214,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>ASHTOWN INTERVENTION &amp; COMPLETION SERVICES LTD</t>
+          <t>THE SPICE INVADERS LTD</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>SC849120</t>
+          <t>16460505</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3252,12 +3252,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>RAPID FULFILL LTD</t>
+          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16462586</t>
+          <t>16460503</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3283,19 +3283,19 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>KOMO NAIL &amp; BEAUTY LTD</t>
+          <t>VALLEY SEVEN DEVELOPMENTS LIMITED</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>16462578</t>
+          <t>16460659</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3328,12 +3328,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>AR BUILDING AND GARDENING SERVICES LTD</t>
+          <t>REIGNING MEDIA LIMITED</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>16462581</t>
+          <t>16461275</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3366,12 +3366,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
+          <t>TMS ASSETS LTD</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>SC849117</t>
+          <t>16461913</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3397,19 +3397,19 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>ECCLES-WOOD LTD</t>
+          <t>LANYNSEN HOUSE LTD</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>SC849115</t>
+          <t>16461918</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3442,12 +3442,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>LEW-BUD LTD</t>
+          <t>PRIME ATHLETIC CO LTD</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>16462565</t>
+          <t>16461911</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3480,12 +3480,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>JWP INDUSTRIES LIMITED</t>
+          <t>GLOBAL CREW LTD</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>16462872</t>
+          <t>16461905</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3518,12 +3518,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>MANPOD LTD</t>
+          <t>DDPT HOLDINGS LIMITED</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>16462873</t>
+          <t>16461906</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3556,12 +3556,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>MAYROL UK LIMITED</t>
+          <t>AMPLIFORTH CONSULTING LIMITED</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>16462870</t>
+          <t>16461904</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3594,12 +3594,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>GASSINGITUP LTD</t>
+          <t>KASZCZUK LTD</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>16462883</t>
+          <t>16461901</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3632,12 +3632,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>WIMWA LTD</t>
+          <t>ALI SHOP LTD</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>16462889</t>
+          <t>16461895</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3670,12 +3670,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>BLITHFIELD PROPERTY SOLUTIONS LTD</t>
+          <t>FND MOTORS LIMITED</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>16462888</t>
+          <t>16461900</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3708,12 +3708,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>PAMIR MECHANICAL LTD</t>
+          <t>48 CONEY STREET LIMITED</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>16462876</t>
+          <t>16461897</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3746,12 +3746,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>BOWEN BUSINESS LTD</t>
+          <t>LEADALE CITY LTD</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>16462877</t>
+          <t>16461899</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3784,12 +3784,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>AFROSCOT VENTURES LTD</t>
+          <t>GIG32 LIMITED</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>16462878</t>
+          <t>16461898</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3815,19 +3815,19 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>3 MORDEN CLIFF LTD</t>
+          <t>MIRE LTD</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16462875</t>
+          <t>16461902</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3860,12 +3860,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>CAMPBELL &amp; DOIG LTD</t>
+          <t>4D CAPITAL PROPCO (44) LIMITED</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>SC849151</t>
+          <t>16461269</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3891,19 +3891,19 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
+          <t>MUNCHIES KEBAB DESERT LTD</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>16462880</t>
+          <t>16461260</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3929,19 +3929,19 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>COLLIN CARE HOLDINGS LIMITED</t>
+          <t>GROUND MORTGAGE SERVICES LIMITED</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>SC849153</t>
+          <t>16461278</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3974,12 +3974,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>ALOVER VUBINH LIMITED</t>
+          <t>AMARA WELLS LTD</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>16462909</t>
+          <t>SC849026</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -4012,12 +4012,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>INTERA AI HOLDINGS UK LIMITED</t>
+          <t>FUNCTION.ALL.OVER LTD</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>16462908</t>
+          <t>16461272</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -4050,12 +4050,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>CFBUK SECURED FINANCE LTD</t>
+          <t>SW2 CONSTRUCTION LIMITED</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>16462904</t>
+          <t>16461262</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4088,12 +4088,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>MAKPLAS LTD</t>
+          <t>TUK TALENT LTD</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>SC849155</t>
+          <t>16461265</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -4126,12 +4126,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>LIU YUMEI LTD</t>
+          <t>KGM CONSTRUCTION LTD</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>16462901</t>
+          <t>16461264</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4164,12 +4164,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>LIT BARBERS LTD</t>
+          <t>CRISPY GLEN LTD</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>16462561</t>
+          <t>SC849027</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -4202,12 +4202,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>DGPI LTD</t>
+          <t>YANGLIN CHEN LIMITED</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>SC849118</t>
+          <t>16461915</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -4233,7 +4233,7 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>Other</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update: 2025-05-20 19:47:16
</commit_message>
<xml_diff>
--- a/master_companies.xlsx
+++ b/master_companies.xlsx
@@ -516,12 +516,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ASSURED LETTINGS AND SALES LTD</t>
+          <t>YANG HAIJUN LTD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16462049</t>
+          <t>16460671</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -554,12 +554,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>RAPID FULFILL LTD</t>
+          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16462586</t>
+          <t>16460503</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -585,19 +585,19 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ASHTOWN INTERVENTION &amp; COMPLETION SERVICES LTD</t>
+          <t>THE SPICE INVADERS LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SC849120</t>
+          <t>16460505</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -630,12 +630,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DANDINI PANTOMIMES LIMITED</t>
+          <t>DEE BEE TRADING LTD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16462588</t>
+          <t>16460511</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -668,12 +668,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>POINT BREAK 7 LTD</t>
+          <t>INNOVATION MT LTD</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16462560</t>
+          <t>16460646</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -706,12 +706,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TBT KENT LTD</t>
+          <t>BRANWELL PROJECTS LIMITED</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16462558</t>
+          <t>16460653</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -744,12 +744,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ELLAHI PROPERTY HOLDINGS LTD</t>
+          <t>MAYTREE ELITE PROPERTIES LTD</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16462030</t>
+          <t>16460650</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -782,12 +782,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>SUBLINE LTD</t>
+          <t>MEDIA WEB PRO LTD</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16462043</t>
+          <t>16460644</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -820,12 +820,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>HOMELORD T LTD</t>
+          <t>ASPC CONTENT CO LTD</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16462031</t>
+          <t>16460643</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -858,12 +858,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ANITA TECHNOLOGY LTD</t>
+          <t>BLUEPRINT VOYAGE MEDIA COMPANY LIMITED</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16462036</t>
+          <t>16460649</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -896,12 +896,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>DAILY NOVA LTD</t>
+          <t>SARASI LTD</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16462033</t>
+          <t>16460670</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -934,12 +934,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CUT N GLOW BEAUTY LIMITED</t>
+          <t>ST PAUL'S COURT DEVELOPMENT LTD</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16462051</t>
+          <t>16460669</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -972,12 +972,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>VIRTUAL CO. UK LTD</t>
+          <t>ASSURED LETTINGS AND SALES LTD</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16460502</t>
+          <t>16462049</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1010,12 +1010,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GEOAIR SOLAR LIMITED</t>
+          <t>SAMVIV PARTNERS LTD</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16462052</t>
+          <t>16460672</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1041,19 +1041,19 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CSS BR ASSET LIMITED</t>
+          <t>COREMARINE SOLUTIONS CIC</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16462021</t>
+          <t>16460663</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1086,12 +1086,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>LEMON TREE REAL ESTATE LIMITED</t>
+          <t>AMPERSAND MANAGEMENT UK LTD</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16462023</t>
+          <t>16460662</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1124,12 +1124,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>DARWIN INVEST LTD</t>
+          <t>TRIPLE J HOUSING LTD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16461938</t>
+          <t>16460681</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1162,12 +1162,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AVIATION TOOL POOLING LLC</t>
+          <t>DXI DAILY NECESSITIES CO., LTD.</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>OE033940</t>
+          <t>16460679</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>registered</t>
+          <t>active</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -1200,12 +1200,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>MARTIAL FITNESS (SW) LTD</t>
+          <t>PREVENTR ACTIVE FIRE LTD</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16461940</t>
+          <t>16460677</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1238,12 +1238,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>JLI CONSTRUCTION LTD</t>
+          <t>MOUNTAIN SEA SHIP SERVICE CO., LTD</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16461948</t>
+          <t>16460640</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1276,12 +1276,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>IVOLVIA LTD</t>
+          <t>T-REX (GUILDFORD) LIMITED</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>16461947</t>
+          <t>16460637</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1314,12 +1314,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>B AND K FLOORING LIMITED</t>
+          <t>HOMEASE LTD</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16461926</t>
+          <t>16460666</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1352,12 +1352,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>LANUNE LTD</t>
+          <t>INAYA HEALTHCARE LTD</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16461925</t>
+          <t>16460657</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1390,12 +1390,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>KOMO NAIL &amp; BEAUTY LTD</t>
+          <t>VALLEY SEVEN DEVELOPMENTS LIMITED</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16462578</t>
+          <t>16460659</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1428,12 +1428,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>AR BUILDING AND GARDENING SERVICES LTD</t>
+          <t>REIGNING MEDIA LIMITED</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16462581</t>
+          <t>16461275</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1466,12 +1466,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>DGPI LTD</t>
+          <t>YANGLIN CHEN LIMITED</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>SC849118</t>
+          <t>16461915</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1497,19 +1497,19 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>LIT BARBERS LTD</t>
+          <t>CRISPY GLEN LTD</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16462561</t>
+          <t>SC849027</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1542,12 +1542,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>LIU YUMEI LTD</t>
+          <t>KGM CONSTRUCTION LTD</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16462901</t>
+          <t>16461264</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1580,12 +1580,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>MAKPLAS LTD</t>
+          <t>TUK TALENT LTD</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>SC849155</t>
+          <t>16461265</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1618,12 +1618,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CFBUK SECURED FINANCE LTD</t>
+          <t>SW2 CONSTRUCTION LIMITED</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16462904</t>
+          <t>16461262</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1656,12 +1656,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>INTERA AI HOLDINGS UK LIMITED</t>
+          <t>FUNCTION.ALL.OVER LTD</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16462908</t>
+          <t>16461272</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1694,12 +1694,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ALOVER VUBINH LIMITED</t>
+          <t>AMARA WELLS LTD</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16462909</t>
+          <t>SC849026</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1732,12 +1732,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>COLLIN CARE HOLDINGS LIMITED</t>
+          <t>GROUND MORTGAGE SERVICES LIMITED</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>SC849153</t>
+          <t>16461278</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1770,12 +1770,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
+          <t>MUNCHIES KEBAB DESERT LTD</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16462880</t>
+          <t>16461260</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1801,19 +1801,19 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>CAMPBELL &amp; DOIG LTD</t>
+          <t>4D CAPITAL PROPCO (44) LIMITED</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>SC849151</t>
+          <t>16461269</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1839,19 +1839,19 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>3 MORDEN CLIFF LTD</t>
+          <t>MIRE LTD</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16462875</t>
+          <t>16461902</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1884,12 +1884,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>AFROSCOT VENTURES LTD</t>
+          <t>GIG32 LIMITED</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16462878</t>
+          <t>16461898</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1915,19 +1915,19 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>BOWEN BUSINESS LTD</t>
+          <t>LEADALE CITY LTD</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16462877</t>
+          <t>16461899</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1960,12 +1960,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>PAMIR MECHANICAL LTD</t>
+          <t>48 CONEY STREET LIMITED</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>16462876</t>
+          <t>16461897</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1998,12 +1998,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>BLITHFIELD PROPERTY SOLUTIONS LTD</t>
+          <t>FND MOTORS LIMITED</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16462888</t>
+          <t>16461900</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2036,12 +2036,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>WIMWA LTD</t>
+          <t>ALI SHOP LTD</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16462889</t>
+          <t>16461895</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2074,12 +2074,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>GASSINGITUP LTD</t>
+          <t>KASZCZUK LTD</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16462883</t>
+          <t>16461901</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2112,12 +2112,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>MAYROL UK LIMITED</t>
+          <t>AMPLIFORTH CONSULTING LIMITED</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16462870</t>
+          <t>16461904</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2150,12 +2150,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>MANPOD LTD</t>
+          <t>DDPT HOLDINGS LIMITED</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16462873</t>
+          <t>16461906</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2188,12 +2188,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>JWP INDUSTRIES LIMITED</t>
+          <t>GLOBAL CREW LTD</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16462872</t>
+          <t>16461905</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2226,12 +2226,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>LEW-BUD LTD</t>
+          <t>PRIME ATHLETIC CO LTD</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>16462565</t>
+          <t>16461911</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2264,12 +2264,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
+          <t>TMS ASSETS LTD</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SC849117</t>
+          <t>16461913</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2295,19 +2295,19 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>ECCLES-WOOD LTD</t>
+          <t>LANYNSEN HOUSE LTD</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SC849115</t>
+          <t>16461918</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2340,12 +2340,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>THE FISH SHOP 17 LTD</t>
+          <t>LEAD INFO LTD</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>16461921</t>
+          <t>16461919</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2416,12 +2416,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>LEAD INFO LTD</t>
+          <t>THE FISH SHOP 17 LTD</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16461919</t>
+          <t>16461921</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2454,12 +2454,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>INAYA HEALTHCARE LTD</t>
+          <t>KOMO NAIL &amp; BEAUTY LTD</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>16460657</t>
+          <t>16462578</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2492,12 +2492,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>HOMEASE LTD</t>
+          <t>B AND K FLOORING LIMITED</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>16460666</t>
+          <t>16461926</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2530,12 +2530,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>T-REX (GUILDFORD) LIMITED</t>
+          <t>IVOLVIA LTD</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>16460637</t>
+          <t>16461947</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2568,12 +2568,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>MOUNTAIN SEA SHIP SERVICE CO., LTD</t>
+          <t>JLI CONSTRUCTION LTD</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>16460640</t>
+          <t>16461948</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2606,12 +2606,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>PREVENTR ACTIVE FIRE LTD</t>
+          <t>MARTIAL FITNESS (SW) LTD</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>16460677</t>
+          <t>16461940</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2644,12 +2644,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>DXI DAILY NECESSITIES CO., LTD.</t>
+          <t>AVIATION TOOL POOLING LLC</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>16460679</t>
+          <t>OE033940</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2659,7 +2659,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>registered</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -2682,12 +2682,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>TRIPLE J HOUSING LTD</t>
+          <t>DARWIN INVEST LTD</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16460681</t>
+          <t>16461938</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2720,12 +2720,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>AMPERSAND MANAGEMENT UK LTD</t>
+          <t>LEMON TREE REAL ESTATE LIMITED</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16460662</t>
+          <t>16462023</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2758,12 +2758,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>COREMARINE SOLUTIONS CIC</t>
+          <t>CSS BR ASSET LIMITED</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>16460663</t>
+          <t>16462021</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2796,12 +2796,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>SAMVIV PARTNERS LTD</t>
+          <t>GEOAIR SOLAR LIMITED</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16460672</t>
+          <t>16462052</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2827,19 +2827,19 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>ST PAUL'S COURT DEVELOPMENT LTD</t>
+          <t>VIRTUAL CO. UK LTD</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>16460669</t>
+          <t>16460502</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2872,12 +2872,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>YANG HAIJUN LTD</t>
+          <t>CUT N GLOW BEAUTY LIMITED</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>16460671</t>
+          <t>16462051</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2910,12 +2910,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>SARASI LTD</t>
+          <t>DAILY NOVA LTD</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>16460670</t>
+          <t>16462033</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2948,12 +2948,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>BLUEPRINT VOYAGE MEDIA COMPANY LIMITED</t>
+          <t>ANITA TECHNOLOGY LTD</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>16460649</t>
+          <t>16462036</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2986,12 +2986,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>ASPC CONTENT CO LTD</t>
+          <t>HOMELORD T LTD</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>16460643</t>
+          <t>16462031</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -3024,12 +3024,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>MEDIA WEB PRO LTD</t>
+          <t>SUBLINE LTD</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>16460644</t>
+          <t>16462043</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -3062,12 +3062,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>MAYTREE ELITE PROPERTIES LTD</t>
+          <t>ELLAHI PROPERTY HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>16460650</t>
+          <t>16462030</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -3100,12 +3100,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>BRANWELL PROJECTS LIMITED</t>
+          <t>TBT KENT LTD</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>16460653</t>
+          <t>16462558</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3138,12 +3138,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>INNOVATION MT LTD</t>
+          <t>POINT BREAK 7 LTD</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16460646</t>
+          <t>16462560</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3176,12 +3176,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>DEE BEE TRADING LTD</t>
+          <t>DANDINI PANTOMIMES LIMITED</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16460511</t>
+          <t>16462588</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3214,12 +3214,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>THE SPICE INVADERS LTD</t>
+          <t>ASHTOWN INTERVENTION &amp; COMPLETION SERVICES LTD</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>16460505</t>
+          <t>SC849120</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3252,12 +3252,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
+          <t>RAPID FULFILL LTD</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16460503</t>
+          <t>16462586</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3283,19 +3283,19 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>VALLEY SEVEN DEVELOPMENTS LIMITED</t>
+          <t>LANUNE LTD</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>16460659</t>
+          <t>16461925</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3328,12 +3328,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>REIGNING MEDIA LIMITED</t>
+          <t>AR BUILDING AND GARDENING SERVICES LTD</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>16461275</t>
+          <t>16462581</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3366,12 +3366,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>YANGLIN CHEN LIMITED</t>
+          <t>ECCLES-WOOD LTD</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>16461915</t>
+          <t>SC849115</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3404,12 +3404,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>CRISPY GLEN LTD</t>
+          <t>DGPI LTD</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>SC849027</t>
+          <t>SC849118</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3435,19 +3435,19 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>GP</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>LANYNSEN HOUSE LTD</t>
+          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>16461918</t>
+          <t>SC849117</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3473,19 +3473,19 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>TMS ASSETS LTD</t>
+          <t>LEW-BUD LTD</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>16461913</t>
+          <t>16462565</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3518,12 +3518,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>PRIME ATHLETIC CO LTD</t>
+          <t>JWP INDUSTRIES LIMITED</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>16461911</t>
+          <t>16462872</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3556,12 +3556,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>GLOBAL CREW LTD</t>
+          <t>MANPOD LTD</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>16461905</t>
+          <t>16462873</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3594,12 +3594,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>DDPT HOLDINGS LIMITED</t>
+          <t>MAYROL UK LIMITED</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>16461906</t>
+          <t>16462870</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3632,12 +3632,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>AMPLIFORTH CONSULTING LIMITED</t>
+          <t>GASSINGITUP LTD</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>16461904</t>
+          <t>16462883</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3670,12 +3670,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>KASZCZUK LTD</t>
+          <t>WIMWA LTD</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>16461901</t>
+          <t>16462889</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3708,12 +3708,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>ALI SHOP LTD</t>
+          <t>BLITHFIELD PROPERTY SOLUTIONS LTD</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>16461895</t>
+          <t>16462888</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3746,12 +3746,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>FND MOTORS LIMITED</t>
+          <t>PAMIR MECHANICAL LTD</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>16461900</t>
+          <t>16462876</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3784,12 +3784,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>48 CONEY STREET LIMITED</t>
+          <t>BOWEN BUSINESS LTD</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>16461897</t>
+          <t>16462877</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3822,12 +3822,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>LEADALE CITY LTD</t>
+          <t>AFROSCOT VENTURES LTD</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16461899</t>
+          <t>16462878</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3853,19 +3853,19 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>GIG32 LIMITED</t>
+          <t>3 MORDEN CLIFF LTD</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>16461898</t>
+          <t>16462875</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3898,12 +3898,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>MIRE LTD</t>
+          <t>CAMPBELL &amp; DOIG LTD</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>16461902</t>
+          <t>SC849151</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3936,12 +3936,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>4D CAPITAL PROPCO (44) LIMITED</t>
+          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>16461269</t>
+          <t>16462880</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3974,12 +3974,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>MUNCHIES KEBAB DESERT LTD</t>
+          <t>COLLIN CARE HOLDINGS LIMITED</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>16461260</t>
+          <t>SC849153</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -4012,12 +4012,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>GROUND MORTGAGE SERVICES LIMITED</t>
+          <t>ALOVER VUBINH LIMITED</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>16461278</t>
+          <t>16462909</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -4050,12 +4050,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>AMARA WELLS LTD</t>
+          <t>INTERA AI HOLDINGS UK LIMITED</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>SC849026</t>
+          <t>16462908</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4088,12 +4088,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>FUNCTION.ALL.OVER LTD</t>
+          <t>CFBUK SECURED FINANCE LTD</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>16461272</t>
+          <t>16462904</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -4126,12 +4126,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>SW2 CONSTRUCTION LIMITED</t>
+          <t>MAKPLAS LTD</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>16461262</t>
+          <t>SC849155</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4164,12 +4164,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>TUK TALENT LTD</t>
+          <t>LIU YUMEI LTD</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>16461265</t>
+          <t>16462901</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -4202,12 +4202,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>KGM CONSTRUCTION LTD</t>
+          <t>LIT BARBERS LTD</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>16461264</t>
+          <t>16462561</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">

</xml_diff>